<commit_message>
Modified   README.md Modified   doc/images/painter.xlsx Add        doc/images/2D-cartesian-position.png Add        doc/images/screen-cartesian.png
</commit_message>
<xml_diff>
--- a/doc/images/painter.xlsx
+++ b/doc/images/painter.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="左右手坐标系" sheetId="1" r:id="rId1"/>
@@ -2905,6 +2905,1193 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="直接箭头连接符 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47FB9BB5-6FE0-4BF2-8882-62C188AAFF0C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="13011150" y="1409701"/>
+          <a:ext cx="4448175" cy="9524"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="直接箭头连接符 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BACDA880-4605-45C0-9FB6-590ED97E277E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13011150" y="1409700"/>
+          <a:ext cx="0" cy="3876675"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="447045" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="文本框 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D07D341D-0846-4D69-8FC2-4397ACE4D2F1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17478375" y="1209675"/>
+          <a:ext cx="447045" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+X</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="437749" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="文本框 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C032F4F3-2C5B-4F7A-A9AF-D05EB6658439}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12792075" y="5286375"/>
+          <a:ext cx="437749" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+Y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="718530" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="文本框 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41517C3D-9CD3-4F8A-92A8-669287ED8702}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14878050" y="1409700"/>
+          <a:ext cx="718530" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>x-axis</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>348620</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>60955</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="400366" cy="716606"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="文本框 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2682AE15-2AAC-4567-B026-AB94868F5C43}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="12820650" y="3038475"/>
+          <a:ext cx="716606" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>y-axis</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="直接箭头连接符 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89015EBD-FFFC-4E6A-90AC-11965EBCDCD4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2228850" y="6000750"/>
+          <a:ext cx="0" cy="4933950"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="直接箭头连接符 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04EA4EB4-8981-445E-8C69-211B0AAD9406}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742950" y="9505950"/>
+          <a:ext cx="5210175" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="直接箭头连接符 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88F55C69-DE15-4F2C-9A86-9168F494350F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2228850" y="7400925"/>
+          <a:ext cx="2228850" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="40" name="直接箭头连接符 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA441123-AD63-4C55-B52E-6037CFE17C88}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4457700" y="7400925"/>
+          <a:ext cx="0" cy="2105025"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4762</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>80964</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>371474</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>328614</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="左大括号 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63B7204B-FD80-4788-BA0F-33607F1007DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="3221831" y="6141245"/>
+          <a:ext cx="247650" cy="2224087"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 92948"/>
+            <a:gd name="adj2" fmla="val 49804"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="275653" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="文本框 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A8E2CBD-E557-4999-B3A5-5A83071CA76B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3209925" y="6753225"/>
+          <a:ext cx="275653" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>x</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="右大括号 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7D720DE-D320-4C91-9772-9C2C63DEB229}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4495799" y="7410450"/>
+          <a:ext cx="257175" cy="2085975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 63888"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="279692" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="文本框 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51A359A2-D9CC-4B6C-8465-F7112C10316C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4819650" y="8220075"/>
+          <a:ext cx="279692" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="586956" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="45" name="文本框 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{079ABE3A-882C-4461-8DD4-2F35F0A06848}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4429125" y="7038975"/>
+          <a:ext cx="586956" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>(x, y)</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="437749" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="文本框 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BF14C7F-5675-4C7D-9706-B3B90C732CD2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2009775" y="5629275"/>
+          <a:ext cx="437749" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+Y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="379463" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="文本框 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A0590D5-6F9C-4357-90C3-5BD99FD4200F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2057400" y="10925175"/>
+          <a:ext cx="379463" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-Y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="447045" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="文本框 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE8C6E4D-F2AB-465D-A0C2-729AF7ECF614}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5924550" y="9315450"/>
+          <a:ext cx="447045" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+X</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="388761" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="49" name="文本框 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBB214E1-6A01-448C-BB3A-8B54FB157D8F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="352425" y="9315450"/>
+          <a:ext cx="388761" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-X</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3207,7 +4394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AS13" sqref="AS13"/>
     </sheetView>
   </sheetViews>
@@ -3224,8 +4411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AN15" sqref="AN15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T31" sqref="T31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Modified   README.md Modified   doc/images/painter.xlsx Add        doc/images/3D-cartesian-position.png
</commit_message>
<xml_diff>
--- a/doc/images/painter.xlsx
+++ b/doc/images/painter.xlsx
@@ -4084,6 +4084,1402 @@
             <a:solidFill>
               <a:srgbClr val="00B050"/>
             </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="50" name="直接箭头连接符 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE2EC831-6AB0-4207-90A9-47939AA017EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10039350" y="6000750"/>
+          <a:ext cx="0" cy="4933950"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="直接箭头连接符 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4971640D-D985-4E5F-BF3B-23E3FB921271}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7800975" y="6353175"/>
+          <a:ext cx="4448175" cy="4229100"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="52" name="直接箭头连接符 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03324E65-D9D4-4EF9-BD97-6F0252BB39AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7429500" y="8458200"/>
+          <a:ext cx="5210175" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="437749" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="53" name="文本框 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD4A0F47-DE0A-4551-BE42-84F7CEB9342A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9829800" y="5629275"/>
+          <a:ext cx="437749" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+Y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="379463" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="54" name="文本框 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30112A56-9CF7-456F-9592-0910322BB220}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9867900" y="10944225"/>
+          <a:ext cx="379463" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-Y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="447045" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="55" name="文本框 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BD89E84-8049-4228-83C9-6A61C56F862A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12620625" y="8267700"/>
+          <a:ext cx="447045" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+X</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="388761" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="56" name="文本框 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDB8B9D8-1DFA-450B-977E-731345633A1E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7048500" y="8258175"/>
+          <a:ext cx="388761" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-X</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="438069" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="57" name="文本框 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B2F10EC-8E2E-4EBF-850D-BB0D486327A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7429500" y="10572750"/>
+          <a:ext cx="438069" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+Z</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>7937</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="直接连接符 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CA9F81B-E3DE-4B02-947E-942451A7A73D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8580439" y="7334250"/>
+          <a:ext cx="1500186" cy="1390650"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>7937</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="直接连接符 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{208D7F61-D770-4365-A282-C7D222D4F9D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8588375" y="8731250"/>
+          <a:ext cx="1588" cy="1047750"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="直接连接符 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6CF7A1B-8DDB-40DF-9CF5-F64059062B6D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8562975" y="9867900"/>
+          <a:ext cx="1847850" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="直接连接符 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75DD57FF-1DDA-4F89-8013-132ABEF83ECD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10445750" y="8731250"/>
+          <a:ext cx="0" cy="1047750"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="59" name="直接连接符 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05704266-E673-497C-A70C-6D76E1742299}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8543925" y="8810625"/>
+          <a:ext cx="1866900" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>365125</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>7938</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="63" name="直接连接符 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE82D591-F4D8-4D3A-A675-A7E4ABE0CCFF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10437813" y="7334250"/>
+          <a:ext cx="1508125" cy="1397000"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>7937</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>7938</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>7938</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="67" name="直接连接符 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78FE9D4B-6AC1-4A5D-AD56-6B03A127E299}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10080625" y="7334250"/>
+          <a:ext cx="1865313" cy="7938"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>7938</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>7938</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="71" name="直接连接符 70">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67DA0906-BA31-491E-87C8-32FC7F1C8D79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11938000" y="7342188"/>
+          <a:ext cx="0" cy="1047750"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>7938</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>341313</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="74" name="直接连接符 73">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53F7221A-9639-40D8-BED5-A201ACD2AA8F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10445750" y="8389938"/>
+          <a:ext cx="1492250" cy="1381125"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>23813</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>222251</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="75" name="右大括号 74">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBC2454E-9956-4AC4-98DE-A77893B51240}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11961813" y="7350125"/>
+          <a:ext cx="198438" cy="1031875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 42283"/>
+            <a:gd name="adj2" fmla="val 49242"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>238126</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>285750</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="279692" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="76" name="文本框 75">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68E196EC-2B2B-40C7-8017-C28439F414C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12176126" y="7620000"/>
+          <a:ext cx="279692" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>15875</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>87313</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>365124</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>334963</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="77" name="左大括号 76">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8710495-6B31-4F67-B755-CFB34181BD22}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="10885488" y="6275388"/>
+          <a:ext cx="247650" cy="1841499"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 51280"/>
+            <a:gd name="adj2" fmla="val 49804"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>55562</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="275653" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="78" name="文本框 77">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BAA7812-7BFC-4596-BAA5-45D80EA1A5AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10874375" y="6699250"/>
+          <a:ext cx="275653" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>x</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>228701</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>1284</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>20129</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>267866</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="79" name="右大括号 78">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72D22668-E86D-4528-B4DC-56D3615B713C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="2804835">
+          <a:off x="11183000" y="7152423"/>
+          <a:ext cx="266582" cy="2029803"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 28289"/>
+            <a:gd name="adj2" fmla="val 49331"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>214313</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="272960" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="80" name="文本框 79">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D1EDF5A-87F9-4C73-A456-6F9142A74A25}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11406188" y="8128000"/>
+          <a:ext cx="272960" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>z</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400">
             <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
             <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
           </a:endParaRPr>
@@ -4411,8 +5807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T31" sqref="T31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AM29" sqref="AM29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Modified   README.md Modified   doc/images/painter.xlsx Add        doc/images/3d-camera-cartesian.png
</commit_message>
<xml_diff>
--- a/doc/images/painter.xlsx
+++ b/doc/images/painter.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="左右手坐标系" sheetId="1" r:id="rId1"/>
     <sheet name="笛卡尔坐标系" sheetId="2" r:id="rId2"/>
+    <sheet name="相机坐标系" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -5393,8 +5394,8 @@
         </a:xfrm>
         <a:prstGeom prst="rightBrace">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 28289"/>
-            <a:gd name="adj2" fmla="val 49331"/>
+            <a:gd name="adj1" fmla="val 143470"/>
+            <a:gd name="adj2" fmla="val 50253"/>
           </a:avLst>
         </a:prstGeom>
       </xdr:spPr>
@@ -5488,6 +5489,1113 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>369278</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>350227</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="直接连接符 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{419EDA6A-B5EC-41EB-B131-15E7805AB7F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1863970" y="2460381"/>
+          <a:ext cx="4488472" cy="704850"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7327</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>14654</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>6</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>344369</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="直接箭头连接符 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{653FF320-DA4C-4C53-BCF3-96774F03B101}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="381000" y="4234962"/>
+          <a:ext cx="1113698" cy="329715"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>7328</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>5</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>3</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="直接箭头连接符 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{201A4CCB-5C2F-4869-88DE-290F33283062}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1128347" y="3516923"/>
+          <a:ext cx="366350" cy="1055080"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2931</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>350228</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="直接连接符 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B1571FE-74B0-4AAB-AB0D-52C5392DB55D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1494692" y="351692"/>
+          <a:ext cx="2931" cy="4218844"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2199</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="直接连接符 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0DB2353-D93A-4422-8FAE-776EBCB36CF6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1496891" y="361217"/>
+          <a:ext cx="4481878" cy="693860"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>7327</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="直接连接符 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FDB890B-28D3-481B-8E49-64ACC013E4AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1494693" y="351692"/>
+          <a:ext cx="373672" cy="2117481"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>7328</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="直接连接符 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B12FC96D-AEE8-411E-BC73-7F4F0ADA4622}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5986097" y="1064602"/>
+          <a:ext cx="366345" cy="2100629"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2932</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>5861</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2932</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>338503</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="直接连接符 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20FBE519-264F-48B6-B929-5C498A14CE73}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1497624" y="2467707"/>
+          <a:ext cx="373673" cy="2091104"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>364881</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>7327</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>350228</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="直接连接符 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E9059D1-E2DF-41D8-B24B-8021EDE546A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1485900" y="3172558"/>
+          <a:ext cx="4866542" cy="1397978"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>34018</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>74840</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="383567" cy="334451"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="62" name="文本框 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A705EC2-7505-4A2C-B953-57A7E5CD6D46}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="782411" y="3258911"/>
+          <a:ext cx="383567" cy="334451"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+Y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>34017</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="390813" cy="334451"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="63" name="文本框 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B07AC967-2E79-4BB7-B444-49275AEEF51A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="34017" y="4068536"/>
+          <a:ext cx="390813" cy="334451"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+X</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>204108</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>285750</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="618824" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="64" name="文本框 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{956F6C07-9D10-431F-8A26-43B52DA3547F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="578304" y="4884964"/>
+          <a:ext cx="618824" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>Origin</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>(0, 0, 0)</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>34018</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>299357</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>346982</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="66" name="直接连接符 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F09744DE-7EAF-497B-86A8-3147ADB9519C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1081768" y="4633232"/>
+          <a:ext cx="340178" cy="312964"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>55562</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>158411</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>110912</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="70" name="图片 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7ED2BDA1-96F9-4BEA-B5FA-4444B35166A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1928812" y="1920876"/>
+          <a:ext cx="2725399" cy="1746036"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2931</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>14654</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>342901</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="直接箭头连接符 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7E74A1E-2353-45D9-82B4-B22FEA818395}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1497623" y="3516923"/>
+          <a:ext cx="759069" cy="1046286"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>40821</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="438069" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61" name="文本框 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C1DA371-9C50-4F1B-94C3-99954AFDAE4B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1870982" y="3224892"/>
+          <a:ext cx="438069" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>Z</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>733</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>7327</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>5862</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="直接连接符 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19491B81-F4A0-4849-9514-2D0DF0BE5A43}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1495425" y="1062404"/>
+          <a:ext cx="4483344" cy="3515458"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>365125</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>150812</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>134938</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="72" name="直接连接符 71">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E79E8C4F-1880-4B14-BB04-ECB860897C83}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1857375" y="2444750"/>
+          <a:ext cx="904875" cy="134938"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="74" name="直接连接符 73">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5730386C-03A7-416E-B47C-11890D1C46E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4184650" y="2851150"/>
+          <a:ext cx="2178050" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5807,8 +6915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AM29" sqref="AM29"/>
+    <sheetView topLeftCell="A17" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AK27" sqref="AK27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5818,4 +6926,21 @@
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" showWhiteSpace="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="V11" sqref="V11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified   README.md Modified   doc/images/painter.xlsx Add        doc/images/vector2D-direction.png Add        doc/images/vector2D-presentation.png Add        doc/images/vector2D.png Add        doc/images/vector3D-translate.png
</commit_message>
<xml_diff>
--- a/doc/images/painter.xlsx
+++ b/doc/images/painter.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="左右手坐标系" sheetId="1" r:id="rId1"/>
     <sheet name="笛卡尔坐标系" sheetId="2" r:id="rId2"/>
     <sheet name="相机坐标系" sheetId="3" r:id="rId3"/>
+    <sheet name="向量" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -66,9 +67,13 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5481,6 +5486,77 @@
             <a:t>z</a:t>
           </a:r>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="379784" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="65" name="文本框 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FB9B607-4E56-43B5-9D35-17ECB3938DC0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12311063" y="5937250"/>
+          <a:ext cx="379784" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-Z</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
             <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
             <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
           </a:endParaRPr>
@@ -6596,6 +6672,2245 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="直接箭头连接符 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B89CE8A-7361-4598-80EB-A95C895CF91F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="742950" y="1409700"/>
+          <a:ext cx="1485900" cy="1409700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="直接箭头连接符 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC97EDDF-BBCC-4969-9C35-5EEA0BD0187B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3352800" y="1428751"/>
+          <a:ext cx="1485900" cy="1390649"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="直接连接符 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6122DCE-F35B-4CDE-8859-3188DE0FC30D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4152900" y="1114425"/>
+          <a:ext cx="609600" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>57151</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>295275</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="直接连接符 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89FBD2B5-FE5A-49BA-A807-DD15020EDE3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3400426" y="2886075"/>
+          <a:ext cx="638174" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="557845" cy="334451"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="文本框 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA4909B8-BAE6-42AB-8850-EF3E08734F7D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3581400" y="923925"/>
+          <a:ext cx="557845" cy="334451"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>Head</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="437877" cy="334451"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="文本框 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4472563A-FA85-47EA-826B-BBF7DB24829F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4105275" y="3019425"/>
+          <a:ext cx="437877" cy="334451"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>Tail</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="直接箭头连接符 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{390164EC-402D-438A-8CB4-829BA2FF2EF4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7058025" y="1428750"/>
+          <a:ext cx="1485900" cy="1390650"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>361949</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>338139</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="左大括号 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAEBA6DC-8BB9-4A74-878A-59FC97E2BB63}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="7689055" y="550070"/>
+          <a:ext cx="214314" cy="1476374"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 41120"/>
+            <a:gd name="adj2" fmla="val 49353"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="右大括号 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D18B9A24-7FC4-4BF9-B087-B75C7B9D1B55}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8562974" y="1428749"/>
+          <a:ext cx="209551" cy="1371601"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 49712"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="267189" cy="334451"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="文本框 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A4A4FB7-2D8A-4864-A8AC-0D385A9F00EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7667625" y="847725"/>
+          <a:ext cx="267189" cy="334451"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>x</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="265650" cy="334451"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="文本框 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{854980E9-7452-4133-83DD-ABB3F0E95D0C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8839200" y="1924050"/>
+          <a:ext cx="265650" cy="334451"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="540341" cy="334451"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="文本框 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22852A3E-CDE3-443E-9F09-A4B642DA64CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7534275" y="2476500"/>
+          <a:ext cx="540341" cy="334451"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>[x, y]</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>4763</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>41275</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>4763</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="直接箭头连接符 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D40949D-21B7-4EB5-A1CB-BA9EC911FD22}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11520488" y="393700"/>
+          <a:ext cx="0" cy="4889500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>366713</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>3175</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="直接箭头连接符 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB4FC920-B184-4D65-964D-C05A866A5C77}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="10396538" y="400050"/>
+          <a:ext cx="4465637" cy="4191000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>365125</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="直接箭头连接符 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AA4CAFC-3418-4540-A14B-0AB6688166DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10023475" y="3533775"/>
+          <a:ext cx="5232400" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>155575</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="437749" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="文本框 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7446053C-952A-43B6-B7D8-5EFF0DBA8A09}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11299825" y="9525"/>
+          <a:ext cx="437749" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+Y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>212725</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>320675</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="379463" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="文本框 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{246A6E37-0258-4887-A1EF-C5666E1E6352}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11356975" y="5254625"/>
+          <a:ext cx="379463" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-Y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>338138</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="447045" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="文本框 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34F4CB54-740D-46E7-9D5F-431A1EB5AC02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15197138" y="3317875"/>
+          <a:ext cx="447045" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+X</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>155575</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="388761" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="文本框 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2588CC11-9AF5-486F-8F57-084B2B679B52}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9658350" y="3327400"/>
+          <a:ext cx="388761" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-X</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>327025</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="438069" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="文本框 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A570818-0BB4-4AA2-8B23-32D90E5E6901}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9985375" y="4572000"/>
+          <a:ext cx="438069" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+Z</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="379784" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="文本框 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D381C05-DB73-45EC-9901-A0BBE95D5685}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14859000" y="38100"/>
+          <a:ext cx="379784" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-Z</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="直接连接符 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B90462F9-07B0-45FA-BB88-632A72BC9621}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11525250" y="1419225"/>
+          <a:ext cx="1485900" cy="1390650"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="直接连接符 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E42039E3-E729-4F8E-99C0-23F7C70E21F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11534775" y="2809875"/>
+          <a:ext cx="1838325" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="直接连接符 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F859E1A-F871-4F74-9E94-B35169CD43A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="13382625" y="1409700"/>
+          <a:ext cx="1466850" cy="1400175"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="直接连接符 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27F06524-C808-4713-A7CC-98C17B28A169}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12992100" y="1409700"/>
+          <a:ext cx="1876425" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="直接连接符 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E3E886B-36B0-41FF-8DA4-302DAE7C194A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13373100" y="2800350"/>
+          <a:ext cx="1" cy="723900"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="直接连接符 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDCD4160-AFD7-4B4C-B5C2-E788AA9DE243}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14859000" y="1419225"/>
+          <a:ext cx="0" cy="714375"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="45" name="直接连接符 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F366955-DB21-4D86-8687-AD3B166B22AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="13354050" y="2133600"/>
+          <a:ext cx="1495425" cy="1400175"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="53" name="直接连接符 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CDF3684-7702-48E6-A37D-EA6D18CF9932}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="13011150" y="1428750"/>
+          <a:ext cx="1" cy="704850"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="56" name="直接连接符 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C163271-88C7-4601-A40E-7B7009CA0AD2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13020675" y="2114550"/>
+          <a:ext cx="1838325" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="61" name="直接箭头连接符 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74393B7F-BD78-40DE-AB25-4D6C91269D5E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11525250" y="1419225"/>
+          <a:ext cx="3333750" cy="2114550"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="64" name="直接箭头连接符 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00A56DCF-78D5-4E9F-9074-1BF503E3EE6F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11525250" y="3524250"/>
+          <a:ext cx="1847850" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx2"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="66" name="直接箭头连接符 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DF0AECE-1BA6-4B9A-BD43-33D858E6ACE0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="13373100" y="2819400"/>
+          <a:ext cx="0" cy="714375"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx2"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="68" name="直接箭头连接符 67">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC4D4E41-6D9B-4C99-A49B-BE3FF9AB2D91}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="13373100" y="1419225"/>
+          <a:ext cx="1485900" cy="1390650"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx2"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="820417" cy="283411"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="69" name="文本框 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DCBCC9B-990C-4AAF-BC76-32169B6ED53E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12058650" y="3619500"/>
+          <a:ext cx="820417" cy="283411"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>右移</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>5</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>单位</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="820417" cy="283411"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="70" name="文本框 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C23839D-7F22-4619-87DA-B7BB14EA5EEC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12515850" y="3038475"/>
+          <a:ext cx="820417" cy="283411"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>上移</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>2</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>单位</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="820417" cy="283411"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="71" name="文本框 70">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F722577-F1F1-4A16-9090-2CC345918C88}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14058900" y="2219325"/>
+          <a:ext cx="820417" cy="283411"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>前移</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>4</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>单位</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6915,8 +9230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AK27" sqref="AK27"/>
+    <sheetView topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AJ22" sqref="AJ22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6932,7 +9247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showWhiteSpace="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showWhiteSpace="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
@@ -6943,4 +9258,27 @@
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AY16" sqref="AY16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="4.875" style="1"/>
+  </cols>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified   README.md Modified   doc/Tiny3DDesign.mdj Modified   doc/images/painter.xlsx Modified   doc/images/s02-stream-design.png
</commit_message>
<xml_diff>
--- a/doc/images/painter.xlsx
+++ b/doc/images/painter.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\MyGame\Tiny3D\steps\doc\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaronwang\workspace\projects\private\Tiny3D\steps\doc\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12170" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="左右手坐标系" sheetId="1" r:id="rId1"/>
@@ -15725,8 +15725,8 @@
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>371451</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3151</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>314300</xdr:rowOff>
     </xdr:to>
@@ -16203,15 +16203,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>180974</xdr:colOff>
+      <xdr:colOff>187324</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>9523</xdr:rowOff>
+      <xdr:rowOff>15873</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>200024</xdr:colOff>
+      <xdr:colOff>206374</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:rowOff>15874</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -16226,8 +16226,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="6867524" y="16925923"/>
-          <a:ext cx="1876425" cy="1409701"/>
+          <a:off x="6816724" y="17084673"/>
+          <a:ext cx="1860550" cy="1422401"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
           <a:avLst>
@@ -16630,86 +16630,33 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>6354</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="163" name="直接箭头连接符 162">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F96B0EB1-4CA6-4BD6-B96B-AFAAA4A8CCA5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="10772775" y="15868650"/>
-          <a:ext cx="1857375" cy="704850"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>41276</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>342900</xdr:rowOff>
+      <xdr:colOff>361955</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="166" name="矩形 165">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9214273-2E3B-4612-B76A-CD7CDBE054E6}"/>
+        <xdr:cNvPr id="167" name="直角三角形 166">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4060EF3F-581F-4DB7-B9F1-C5430CAF86AD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10782300" y="16573500"/>
-          <a:ext cx="1838325" cy="1390650"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:xfrm rot="16200000">
+          <a:off x="11263318" y="15467012"/>
+          <a:ext cx="676274" cy="1828801"/>
+        </a:xfrm>
+        <a:prstGeom prst="rtTriangle">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
@@ -16757,33 +16704,88 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>41276</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>361953</xdr:colOff>
+      <xdr:colOff>361956</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>352424</xdr:rowOff>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="163" name="直接箭头连接符 162">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F96B0EB1-4CA6-4BD6-B96B-AFAAA4A8CCA5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="167" idx="4"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10680700" y="16043276"/>
+          <a:ext cx="1835156" cy="657224"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="167" name="直角三角形 166">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4060EF3F-581F-4DB7-B9F1-C5430CAF86AD}"/>
+        <xdr:cNvPr id="166" name="矩形 165">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9214273-2E3B-4612-B76A-CD7CDBE054E6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm rot="16200000">
-          <a:off x="11391902" y="15335248"/>
-          <a:ext cx="676274" cy="1781178"/>
-        </a:xfrm>
-        <a:prstGeom prst="rtTriangle">
+        <a:xfrm>
+          <a:off x="10782300" y="16573500"/>
+          <a:ext cx="1838325" cy="1390650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
@@ -18170,7 +18172,7 @@
       <selection activeCell="AS13" sqref="AS13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18187,7 +18189,7 @@
       <selection activeCell="AJ22" sqref="AJ22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18204,7 +18206,7 @@
       <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18224,9 +18226,9 @@
       <selection activeCell="AY16" sqref="AY16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="4.875" style="1"/>
+    <col min="1" max="16384" width="4.83203125" style="1"/>
   </cols>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -18244,12 +18246,12 @@
   <dimension ref="O45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AW58" sqref="AW58"/>
+      <selection activeCell="AJ47" sqref="AJ47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="45" spans="15:15" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="15:15" ht="28.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O45" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified   doc/images/painter.xlsx Modified   doc/images/triangle-area.png Modified   doc/images/triangle-centroid.png Modified   doc/一起动手实现3D渲染引擎.md Add        doc/images/triangle-barycentric.png Add        doc/一起动手实现3D渲染引擎.pdf
</commit_message>
<xml_diff>
--- a/doc/images/painter.xlsx
+++ b/doc/images/painter.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaronwang\workspace\projects\private\Tiny3D\steps\doc\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\MyGame\Tiny3D\steps\doc\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12170" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="左右手坐标系" sheetId="1" r:id="rId1"/>
@@ -8923,6 +8923,61 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="128" name="直接连接符 127">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1211CE25-3640-45CD-922D-7A5162016F62}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="838200" y="21859875"/>
+          <a:ext cx="5486400" cy="1790700"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
@@ -16515,63 +16570,6 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="159" name="直接箭头连接符 158">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CB04715-20DF-4F60-BCE3-0EC0370D74DA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9648825" y="17973675"/>
-          <a:ext cx="3724275" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="00B050"/>
-          </a:solidFill>
-          <a:headEnd type="triangle"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>28</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>42</xdr:row>
@@ -16630,13 +16628,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>6354</xdr:colOff>
+      <xdr:colOff>9528</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>41276</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>361955</xdr:colOff>
+      <xdr:colOff>361957</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:to>
@@ -16653,8 +16651,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000">
-          <a:off x="11263318" y="15467012"/>
-          <a:ext cx="676274" cy="1828801"/>
+          <a:off x="11366506" y="15316198"/>
+          <a:ext cx="669924" cy="1838329"/>
         </a:xfrm>
         <a:prstGeom prst="rtTriangle">
           <a:avLst/>
@@ -16703,16 +16701,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>41276</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>361956</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>342900</xdr:rowOff>
+      <xdr:colOff>361958</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -16729,8 +16727,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="10680700" y="16043276"/>
-          <a:ext cx="1835156" cy="657224"/>
+          <a:off x="10763250" y="15900401"/>
+          <a:ext cx="1857383" cy="682624"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -16828,6 +16826,63 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="159" name="直接箭头连接符 158">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CB04715-20DF-4F60-BCE3-0EC0370D74DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9648825" y="17973675"/>
+          <a:ext cx="3724275" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -17399,14 +17454,14 @@
               <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
               <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
             </a:rPr>
-            <a:t>(0,</a:t>
+            <a:t>(0.5,</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" altLang="zh-CN" sz="1000" baseline="0">
               <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
               <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
             </a:rPr>
-            <a:t> 0.5, 0.5)</a:t>
+            <a:t> 0.5, 0)</a:t>
           </a:r>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1000">
             <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
@@ -17591,7 +17646,7 @@
               <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
               <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
             </a:rPr>
-            <a:t>(0.25, 0, 0.75)</a:t>
+            <a:t>(0.75, 0, 0.25)</a:t>
           </a:r>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1000">
             <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
@@ -17669,7 +17724,7 @@
       <xdr:row>44</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="689035" cy="312330"/>
+    <xdr:ext cx="1007199" cy="312330"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="182" name="文本框 181">
@@ -17684,7 +17739,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14735175" y="15554325"/>
-          <a:ext cx="689035" cy="312330"/>
+          <a:ext cx="1007199" cy="312330"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17716,14 +17771,14 @@
               <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
               <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
             </a:rPr>
-            <a:t>(6,</a:t>
+            <a:t>(-0.2,</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" altLang="zh-CN" sz="1000" baseline="0">
               <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
               <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
             </a:rPr>
-            <a:t> 6, -2)</a:t>
+            <a:t> 0.6, 0.6)</a:t>
           </a:r>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1000">
             <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
@@ -17866,6 +17921,1633 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>190501</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>209525</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>57124</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="160" name="图片 159">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9245B467-635B-4FBB-BEF6-14B712709AE3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4095750" y="22745701"/>
+          <a:ext cx="200000" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>228601</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>66646</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>95224</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="162" name="图片 161">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68341677-4E47-43CA-A852-5ABEA62B5AE7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3552825" y="22078951"/>
+          <a:ext cx="228571" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>209551</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38070</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>85697</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="164" name="图片 163">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7207566-F3CC-44E7-A7CA-58DBAE4B401F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3143250" y="22412326"/>
+          <a:ext cx="238095" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="68" name="直接连接符 67">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B479148F-9E5F-4797-8963-6EAC5F64BDEC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2276475" y="20107275"/>
+          <a:ext cx="3114675" cy="4181475"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>200026</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="126" name="直接连接符 125">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FA926D1-2B2E-4DAD-8627-CB8DB1C13707}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="847725" y="20640676"/>
+          <a:ext cx="4733925" cy="3448049"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="183" name="直接连接符 182">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC9CE28F-DC6F-4BB4-841E-BA51DFF6D592}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1714500" y="21697950"/>
+          <a:ext cx="4591050" cy="3324226"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="187" name="直接连接符 186">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7287768-AFA9-4DED-B688-3D72DCC5B55F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1133475" y="20097750"/>
+          <a:ext cx="3648075" cy="4905375"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>74065</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>232684</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>153962</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>262141</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="158" name="等腰三角形 157">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{968C9D4A-92BB-43BE-954D-6D73C003C0FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="1074581">
+          <a:off x="3045865" y="22083034"/>
+          <a:ext cx="1565797" cy="734307"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 33756"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>285750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="188" name="直接连接符 187">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15FC8B76-9A12-425A-A650-DB159F91CF1E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="838200" y="21078825"/>
+          <a:ext cx="5486400" cy="1790700"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="189" name="直接连接符 188">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7343400-E954-4179-9939-A5FD3D5CB808}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="733425" y="20097750"/>
+          <a:ext cx="3400425" cy="2486025"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="190" name="直接连接符 189">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4358204D-2C2D-4D66-9B9C-574FEE918849}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="828675" y="20288250"/>
+          <a:ext cx="5486400" cy="1790700"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="191" name="直接连接符 190">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A894200A-86DF-470C-A4F4-A7DD2B5CA360}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="781050" y="21164550"/>
+          <a:ext cx="2857500" cy="3848100"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="192" name="直接连接符 191">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7033B99C-D8C5-4D6B-9792-E7E596EC6B5E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="704850" y="22593300"/>
+          <a:ext cx="5486400" cy="1790700"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="193" name="直接连接符 192">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1DCD370-B022-4F5A-8A7F-6567E77DAAF1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3438525" y="20097750"/>
+          <a:ext cx="2857500" cy="3905250"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="194" name="直接连接符 193">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39BE4F81-EECF-4CE8-B68D-D4ABFD8214BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4524375" y="20050125"/>
+          <a:ext cx="1790700" cy="2419350"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="195" name="直接连接符 194">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAF78B4C-7064-4739-BA08-0980DC37A869}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="771525" y="23393400"/>
+          <a:ext cx="4943475" cy="1619250"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="196" name="直接连接符 195">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{274173F8-0B92-467D-B077-77BDD3CAAEE7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742950" y="22621875"/>
+          <a:ext cx="1790700" cy="2419350"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="633571" cy="255180"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="197" name="文本框 196">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF307425-C5CC-4173-B07B-579B12F31A63}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4572000" y="22869525"/>
+          <a:ext cx="633571" cy="255180"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="800">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>(1, 0, 0)</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="800">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>304799</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="633571" cy="226605"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="198" name="文本框 197">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6881F92B-BEC1-47CC-B305-C5B57FEC8DB3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2752725" y="22155149"/>
+          <a:ext cx="633571" cy="226605"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="800">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>(0, 0, 1)</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="800">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="633571" cy="226605"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="199" name="文本框 198">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4193783D-2CB2-48D0-8DD9-0E28C069135C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3495675" y="21593174"/>
+          <a:ext cx="633571" cy="226605"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="800">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>(0, 1, 0)</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="800">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228620</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>209534</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>371431</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>66633</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="200" name="图片 199">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C56A20F2-0E3D-4744-8BB7-F6A4904F12B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="19385686">
+          <a:off x="3943370" y="21707459"/>
+          <a:ext cx="514286" cy="209524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>95249</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>257175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>276155</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>104750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="201" name="图片 200">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3C4E16B-8E0D-4936-AFD5-3A797BBB1635}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="1077049">
+          <a:off x="3438524" y="22812375"/>
+          <a:ext cx="552381" cy="200000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>38102</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>219052</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>190439</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="202" name="图片 201">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40B40C69-19A3-461E-AFAD-A2D0573E7E52}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="3153993">
+          <a:off x="3962420" y="22402782"/>
+          <a:ext cx="504762" cy="180952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="633571" cy="226605"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="203" name="文本框 202">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58EDFA81-5FEB-4CE2-BEFE-636791D588A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2295525" y="21326475"/>
+          <a:ext cx="633571" cy="226605"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="800">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>(-1, 1, 1)</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="800">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="633571" cy="226605"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="204" name="文本框 203">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF7372A6-CFEA-4E71-9734-BB50D46806AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1562100" y="21859875"/>
+          <a:ext cx="633571" cy="226605"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="800">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>(-1, 0, 2)</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="800">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="633571" cy="217080"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="205" name="文本框 204">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CDF066B-AC92-48A7-A016-EE4B4C8BF6AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2009775" y="22669500"/>
+          <a:ext cx="633571" cy="217080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="800">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>(0, -1, 2)</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="800">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="633571" cy="217080"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="206" name="文本框 205">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56B6D5AB-997E-45CF-BAF0-32CE6C78E630}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3857625" y="23402925"/>
+          <a:ext cx="633571" cy="217080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="800">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>(1, -1, 1)</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="800">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="633571" cy="217080"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="207" name="文本框 206">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{974A9FDE-E51A-4901-B7B7-C01ECAB7AD37}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3076575" y="23955375"/>
+          <a:ext cx="633571" cy="217080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="800">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>(1, -2, 2)</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="800">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>295275</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="633571" cy="217080"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="208" name="文本框 207">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0BE4A11-DA99-48A9-92FC-0CCEF36A941A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1276350" y="23202900"/>
+          <a:ext cx="633571" cy="217080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="800">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>(0, -1, 3)</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="800">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -18172,7 +19854,7 @@
       <selection activeCell="AS13" sqref="AS13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18189,7 +19871,7 @@
       <selection activeCell="AJ22" sqref="AJ22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18206,7 +19888,7 @@
       <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18226,9 +19908,9 @@
       <selection activeCell="AY16" sqref="AY16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="4.83203125" style="1"/>
+    <col min="1" max="16384" width="4.875" style="1"/>
   </cols>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -18245,13 +19927,13 @@
   </sheetPr>
   <dimension ref="O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AJ47" sqref="AJ47"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y68" sqref="Y68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="45" spans="15:15" ht="28.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="15:15" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O45" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified   doc/images/painter.xlsx Modified   doc/一起动手实现3D渲染引擎.md Add        doc/images/triangle-calc-3d-centroid.png Add        doc/images/triangle-calc-centroid.png
</commit_message>
<xml_diff>
--- a/doc/images/painter.xlsx
+++ b/doc/images/painter.xlsx
@@ -8920,6 +8920,50 @@
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>227839</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="153" name="图片 152">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{471FCD33-DE1D-48DD-B7BA-30A4AD3D57DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9182100" y="21678900"/>
+          <a:ext cx="704089" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
@@ -9766,50 +9810,6 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6343650" y="3181350"/>
-          <a:ext cx="314286" cy="295238"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>38055</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>352390</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="27" name="图片 26">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001B000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
@@ -9817,8 +9817,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9334500" y="781050"/>
-          <a:ext cx="361905" cy="276190"/>
+          <a:off x="6343650" y="3181350"/>
+          <a:ext cx="314286" cy="295238"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9827,78 +9827,25 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>352424</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="28" name="直接箭头连接符 27">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001C000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="10410825" y="1066800"/>
-          <a:ext cx="2590800" cy="2105024"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>342870</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>342864</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>38055</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>352390</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="29" name="图片 28">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001D000000}"/>
+        <xdr:cNvPr id="27" name="图片 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9914,8 +9861,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10134600" y="2876550"/>
-          <a:ext cx="238095" cy="285714"/>
+          <a:off x="9334500" y="781050"/>
+          <a:ext cx="361905" cy="276190"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9924,25 +9871,78 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>352424</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="直接箭头连接符 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10410825" y="1066800"/>
+          <a:ext cx="2590800" cy="2105024"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>76176</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>333336</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>342870</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>342864</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="30" name="图片 29">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001E000000}"/>
+        <xdr:cNvPr id="29" name="图片 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9952,6 +9952,50 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10134600" y="2876550"/>
+          <a:ext cx="238095" cy="285714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>76176</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>333336</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="图片 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -11459,7 +11503,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -11568,7 +11612,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -12116,7 +12160,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -12160,7 +12204,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -12264,7 +12308,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -14640,50 +14684,6 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12941301" y="12820650"/>
-          <a:ext cx="252604" cy="323850"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>82551</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>322943</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>336551</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="65" name="图片 64">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000041000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
@@ -14691,8 +14691,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12547600" y="11817351"/>
-          <a:ext cx="297543" cy="254000"/>
+          <a:off x="12941301" y="12820650"/>
+          <a:ext cx="252604" cy="323850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14703,23 +14703,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>349250</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>298450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>192231</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>82551</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>322943</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>336551</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="66" name="图片 65">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000042000000}"/>
+        <xdr:cNvPr id="65" name="图片 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000041000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14735,8 +14735,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11398250" y="13100050"/>
-          <a:ext cx="228600" cy="249381"/>
+          <a:off x="12547600" y="11817351"/>
+          <a:ext cx="297543" cy="254000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14747,23 +14747,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>135978</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>298450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>192231</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="89" name="图片 88">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000059000000}"/>
+        <xdr:cNvPr id="66" name="图片 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000042000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14779,8 +14779,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12788900" y="12255500"/>
-          <a:ext cx="237578" cy="222250"/>
+          <a:off x="11398250" y="13100050"/>
+          <a:ext cx="228600" cy="249381"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14791,23 +14791,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>50801</xdr:colOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>260351</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>279401</xdr:colOff>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>135978</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>133351</xdr:rowOff>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="109" name="图片 108">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00006D000000}"/>
+        <xdr:cNvPr id="89" name="图片 88">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000059000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14817,6 +14817,50 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12788900" y="12255500"/>
+          <a:ext cx="237578" cy="222250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>50801</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>260351</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>279401</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="109" name="图片 108">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00006D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -15245,50 +15289,6 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="16281400" y="12192001"/>
-          <a:ext cx="175759" cy="196850"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>82551</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>44451</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>279401</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>299627</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="123" name="图片 122">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00007B000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
         <a:stretch>
           <a:fillRect/>
@@ -15296,8 +15296,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17024351" y="13201651"/>
-          <a:ext cx="196850" cy="255176"/>
+          <a:off x="16281400" y="12192001"/>
+          <a:ext cx="175759" cy="196850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15309,22 +15309,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>46</xdr:col>
-      <xdr:colOff>82550</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:colOff>82551</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>44451</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>46</xdr:col>
-      <xdr:colOff>248074</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>304800</xdr:rowOff>
+      <xdr:colOff>279401</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>299627</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="124" name="图片 123">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00007C000000}"/>
+        <xdr:cNvPr id="123" name="图片 122">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00007B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15340,8 +15340,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17024350" y="10756900"/>
-          <a:ext cx="165524" cy="215900"/>
+          <a:off x="17024351" y="13201651"/>
+          <a:ext cx="196850" cy="255176"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15353,22 +15353,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>46</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>31751</xdr:rowOff>
+      <xdr:colOff>82550</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>46</xdr:col>
-      <xdr:colOff>325437</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>241301</xdr:rowOff>
+      <xdr:colOff>248074</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="125" name="图片 124">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00007D000000}"/>
+        <xdr:cNvPr id="124" name="图片 123">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00007C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15384,8 +15384,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17005300" y="12122151"/>
-          <a:ext cx="261937" cy="209550"/>
+          <a:off x="17024350" y="10756900"/>
+          <a:ext cx="165524" cy="215900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15394,88 +15394,25 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>340692</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>139175</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>89074</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>215995</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="等腰三角形 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8099D3FF-1E18-4B72-AE8A-14B92C2F61F6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="1074581">
-          <a:off x="1455117" y="15645875"/>
-          <a:ext cx="3463132" cy="2543795"/>
-        </a:xfrm>
-        <a:prstGeom prst="triangle">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 31467"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>228575</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>247623</xdr:rowOff>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>31751</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>325437</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>241301</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="图片 15">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A2DA649-8E13-4435-87C5-A0EA32CEABCE}"/>
+        <xdr:cNvPr id="125" name="图片 124">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00007D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15491,8 +15428,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4486275" y="18707100"/>
-          <a:ext cx="200000" cy="219048"/>
+          <a:off x="17005300" y="12122151"/>
+          <a:ext cx="261937" cy="209550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15501,25 +15438,88 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>340692</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>139175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>89074</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>215995</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="等腰三角形 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8099D3FF-1E18-4B72-AE8A-14B92C2F61F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="1074581">
+          <a:off x="1455117" y="15645875"/>
+          <a:ext cx="3463132" cy="2543795"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 31467"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>133321</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>333348</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>228575</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>247623</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="41" name="图片 40">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10E06EE2-D7B9-4818-BD4B-CCCCE27C5C68}"/>
+        <xdr:cNvPr id="16" name="图片 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A2DA649-8E13-4435-87C5-A0EA32CEABCE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15535,8 +15535,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2876550" y="15268575"/>
-          <a:ext cx="228571" cy="219048"/>
+          <a:off x="4486275" y="18707100"/>
+          <a:ext cx="200000" cy="219048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15547,23 +15547,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>285750</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>352395</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>161896</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>133321</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>333348</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="42" name="图片 41">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19F5EA9B-46E6-4E85-8A30-FD02500B65AD}"/>
+        <xdr:cNvPr id="41" name="图片 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10E06EE2-D7B9-4818-BD4B-CCCCE27C5C68}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15579,8 +15579,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="857250" y="17554575"/>
-          <a:ext cx="238095" cy="228571"/>
+          <a:off x="2876550" y="15268575"/>
+          <a:ext cx="228571" cy="219048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15589,208 +15589,25 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>256085</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>239977</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>17525</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>251411</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="43" name="弧形 42">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0524BC82-0405-464B-BC5A-773AB535C44A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="17259736">
-          <a:off x="3864888" y="18319599"/>
-          <a:ext cx="716284" cy="504390"/>
-        </a:xfrm>
-        <a:prstGeom prst="arc">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 15864058"/>
-            <a:gd name="adj2" fmla="val 20644207"/>
-          </a:avLst>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>84553</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>239297</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>57887</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>38837</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="116" name="弧形 115">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5095713F-B8DE-4942-BE1D-CCB1778031BC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="9492062">
-          <a:off x="2684878" y="15393572"/>
-          <a:ext cx="716284" cy="504390"/>
-        </a:xfrm>
-        <a:prstGeom prst="arc">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 16312574"/>
-            <a:gd name="adj2" fmla="val 21531377"/>
-          </a:avLst>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>123824</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>333375</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>97158</xdr:colOff>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>285750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>352395</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>132915</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="119" name="弧形 118">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6ED9F430-48B5-4351-A863-AD685ABFB6AB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="2351618">
-          <a:off x="866774" y="17249775"/>
-          <a:ext cx="716284" cy="504390"/>
-        </a:xfrm>
-        <a:prstGeom prst="arc">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 16312574"/>
-            <a:gd name="adj2" fmla="val 21449785"/>
-          </a:avLst>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>3151</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>314300</xdr:rowOff>
+      <xdr:rowOff>161896</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="129" name="图片 128">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7FC534C-59F8-4E32-B57C-12E9BCE67207}"/>
+        <xdr:cNvPr id="42" name="图片 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19F5EA9B-46E6-4E85-8A30-FD02500B65AD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15806,8 +15623,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1666875" y="16325850"/>
-          <a:ext cx="190476" cy="200000"/>
+          <a:off x="857250" y="17554575"/>
+          <a:ext cx="238095" cy="228571"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15816,25 +15633,208 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>256085</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>239977</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>17525</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>251411</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="弧形 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0524BC82-0405-464B-BC5A-773AB535C44A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="17259736">
+          <a:off x="3864888" y="18319599"/>
+          <a:ext cx="716284" cy="504390"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 15864058"/>
+            <a:gd name="adj2" fmla="val 20644207"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>84553</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>239297</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>57887</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>38837</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="116" name="弧形 115">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5095713F-B8DE-4942-BE1D-CCB1778031BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="9492062">
+          <a:off x="2684878" y="15393572"/>
+          <a:ext cx="716284" cy="504390"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 16312574"/>
+            <a:gd name="adj2" fmla="val 21531377"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>123824</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>97158</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>132915</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="119" name="弧形 118">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6ED9F430-48B5-4351-A863-AD685ABFB6AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="2351618">
+          <a:off x="866774" y="17249775"/>
+          <a:ext cx="716284" cy="504390"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 16312574"/>
+            <a:gd name="adj2" fmla="val 21449785"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>247650</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>47599</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>76177</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3151</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>314300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="130" name="图片 129">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DC943A7-2592-43F3-9809-C4DEA5EA8D6A}"/>
+        <xdr:cNvPr id="129" name="图片 128">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7FC534C-59F8-4E32-B57C-12E9BCE67207}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15850,8 +15850,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2438400" y="18221325"/>
-          <a:ext cx="209524" cy="180952"/>
+          <a:off x="1666875" y="16325850"/>
+          <a:ext cx="190476" cy="200000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15862,23 +15862,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>285724</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>76175</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47599</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>76177</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="131" name="图片 130">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E944944-5EC4-4B3E-B3A3-0C1132AF5767}"/>
+        <xdr:cNvPr id="130" name="图片 129">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DC943A7-2592-43F3-9809-C4DEA5EA8D6A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15894,8 +15894,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3790950" y="16792575"/>
-          <a:ext cx="209524" cy="200000"/>
+          <a:off x="2438400" y="18221325"/>
+          <a:ext cx="209524" cy="180952"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15906,23 +15906,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>1876</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>182587</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>209550</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>285724</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>76175</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="132" name="图片 131">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA91F917-0239-4BFE-86A4-F8B992E64D4F}"/>
+        <xdr:cNvPr id="131" name="图片 130">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E944944-5EC4-4B3E-B3A3-0C1132AF5767}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15938,8 +15938,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4095750" y="18327976"/>
-          <a:ext cx="173062" cy="207674"/>
+          <a:off x="3790950" y="16792575"/>
+          <a:ext cx="209524" cy="200000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15950,23 +15950,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>228572</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>76173</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>1876</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>182587</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="133" name="图片 132">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784696FA-492B-46FA-92E3-885AFB6F5E9C}"/>
+        <xdr:cNvPr id="132" name="图片 131">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA91F917-0239-4BFE-86A4-F8B992E64D4F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15982,8 +15982,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2828897" y="15687674"/>
-          <a:ext cx="219076" cy="200025"/>
+          <a:off x="4095750" y="18327976"/>
+          <a:ext cx="173062" cy="207674"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15994,23 +15994,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>361927</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>19026</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228572</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76173</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="134" name="图片 133">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DC397E1-8A96-4D22-B476-1B4C12622D00}"/>
+        <xdr:cNvPr id="133" name="图片 132">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784696FA-492B-46FA-92E3-885AFB6F5E9C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16020,6 +16020,50 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2828897" y="15687674"/>
+          <a:ext cx="219076" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>361927</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>19026</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="134" name="图片 133">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DC397E1-8A96-4D22-B476-1B4C12622D00}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -16975,50 +17019,6 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="18230850" y="18716625"/>
-          <a:ext cx="200000" cy="219048"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>44</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>45</xdr:col>
-      <xdr:colOff>133321</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>342873</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="170" name="图片 169">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{575511FC-59FD-436A-A1EF-736C182B7B72}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
         <a:stretch>
           <a:fillRect/>
@@ -17026,8 +17026,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16621125" y="15278100"/>
-          <a:ext cx="228571" cy="219048"/>
+          <a:off x="18230850" y="18716625"/>
+          <a:ext cx="200000" cy="219048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17038,23 +17038,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>295275</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>352395</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>171421</xdr:rowOff>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>133321</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>342873</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="171" name="图片 170">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DE031E6-50A0-4403-A443-DCFD16323F5E}"/>
+        <xdr:cNvPr id="170" name="图片 169">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{575511FC-59FD-436A-A1EF-736C182B7B72}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17064,6 +17064,50 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16621125" y="15278100"/>
+          <a:ext cx="228571" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>295275</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>352395</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>171421</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="171" name="图片 170">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DE031E6-50A0-4403-A443-DCFD16323F5E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -17816,59 +17860,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm rot="18708752">
-          <a:off x="15325726" y="16459200"/>
-          <a:ext cx="514286" cy="209524"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>42</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>333374</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>43</xdr:col>
-      <xdr:colOff>199956</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>180949</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="185" name="图片 184">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56B56E2A-2B85-4AEC-A57C-D52F786E1E77}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm rot="1064821">
-          <a:off x="15621000" y="17954624"/>
-          <a:ext cx="552381" cy="200000"/>
+        <a:xfrm rot="18708752">
+          <a:off x="15325726" y="16459200"/>
+          <a:ext cx="514286" cy="209524"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17879,23 +17879,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>47</xdr:col>
-      <xdr:colOff>219055</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>285770</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>48</xdr:col>
-      <xdr:colOff>28532</xdr:colOff>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>85682</xdr:rowOff>
+      <xdr:rowOff>333374</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>199956</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>180949</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="186" name="图片 185">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E721085A-53B2-4D68-9938-9DFA360A644A}"/>
+        <xdr:cNvPr id="185" name="图片 184">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56B56E2A-2B85-4AEC-A57C-D52F786E1E77}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17910,9 +17910,9 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm rot="3785256">
-          <a:off x="17516475" y="17364075"/>
-          <a:ext cx="504762" cy="180952"/>
+        <a:xfrm rot="1064821">
+          <a:off x="15621000" y="17954624"/>
+          <a:ext cx="552381" cy="200000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17923,23 +17923,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>190501</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>209525</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>57124</xdr:rowOff>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>219055</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>285770</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>28532</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>85682</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="160" name="图片 159">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9245B467-635B-4FBB-BEF6-14B712709AE3}"/>
+        <xdr:cNvPr id="186" name="图片 185">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E721085A-53B2-4D68-9938-9DFA360A644A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17948,15 +17948,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4095750" y="22745701"/>
-          <a:ext cx="200000" cy="219048"/>
+        <a:xfrm rot="3785256">
+          <a:off x="17516475" y="17364075"/>
+          <a:ext cx="504762" cy="180952"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17967,23 +17967,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>228601</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>66646</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>95224</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>190501</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>209525</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>57124</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="162" name="图片 161">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68341677-4E47-43CA-A852-5ABEA62B5AE7}"/>
+        <xdr:cNvPr id="160" name="图片 159">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9245B467-635B-4FBB-BEF6-14B712709AE3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17999,8 +17999,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3552825" y="22078951"/>
-          <a:ext cx="228571" cy="219048"/>
+          <a:off x="4095750" y="22745701"/>
+          <a:ext cx="200000" cy="219048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -18011,23 +18011,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>228601</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>66646</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>209551</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>38070</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>85697</xdr:rowOff>
+      <xdr:rowOff>95224</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="164" name="图片 163">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7207566-F3CC-44E7-A7CA-58DBAE4B401F}"/>
+        <xdr:cNvPr id="162" name="图片 161">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68341677-4E47-43CA-A852-5ABEA62B5AE7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18037,6 +18037,50 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3552825" y="22078951"/>
+          <a:ext cx="228571" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>209551</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38070</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>85697</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="164" name="图片 163">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7207566-F3CC-44E7-A7CA-58DBAE4B401F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -19053,59 +19097,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm rot="19385686">
-          <a:off x="3943370" y="21707459"/>
-          <a:ext cx="514286" cy="209524"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>95249</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>257175</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>276155</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>104750</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="201" name="图片 200">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3C4E16B-8E0D-4936-AFD5-3A797BBB1635}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm rot="1077049">
-          <a:off x="3438524" y="22812375"/>
-          <a:ext cx="552381" cy="200000"/>
+        <a:xfrm rot="19385686">
+          <a:off x="3943370" y="21707459"/>
+          <a:ext cx="514286" cy="209524"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -19116,23 +19116,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>38102</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>219052</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>95249</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>190439</xdr:rowOff>
+      <xdr:rowOff>257175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>276155</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>104750</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="202" name="图片 201">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40B40C69-19A3-461E-AFAD-A2D0573E7E52}"/>
+        <xdr:cNvPr id="201" name="图片 200">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3C4E16B-8E0D-4936-AFD5-3A797BBB1635}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19142,6 +19142,50 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="1077049">
+          <a:off x="3438524" y="22812375"/>
+          <a:ext cx="552381" cy="200000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>38102</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>219052</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>190439</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="202" name="图片 201">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40B40C69-19A3-461E-AFAD-A2D0573E7E52}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -19548,6 +19592,1378 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>312117</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>167750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>60499</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>244570</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="209" name="等腰三角形 208">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B613182-1A7B-403D-A3CC-A75E50D943CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="1074581">
+          <a:off x="7741617" y="20255975"/>
+          <a:ext cx="3463132" cy="2543795"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 31467"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>200000</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>276198</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="210" name="图片 209">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29F17BB4-4079-4B73-AAEE-C001EC30EDE4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10772775" y="23317200"/>
+          <a:ext cx="200000" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>104746</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>9498</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="211" name="图片 210">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAA69513-36B7-4C8D-A1AF-BAE5E12E9247}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9163050" y="19878675"/>
+          <a:ext cx="228571" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>323820</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>190471</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="212" name="图片 211">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6004B13C-A9FC-4936-BB62-E85B5DB4DC62}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7143750" y="22164675"/>
+          <a:ext cx="238095" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>32012</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>338193</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="48" name="直接连接符 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{319B2415-8C05-467E-8BCE-2B940EEB63FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="209" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="9144000" y="20120237"/>
+          <a:ext cx="109593" cy="1758688"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>4894</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>2875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="55" name="直接连接符 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1876A2BC-F1BB-442D-947F-A4E387BB9824}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="209" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7434394" y="21869400"/>
+          <a:ext cx="1709606" cy="336250"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>328411</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>10574</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="110" name="直接连接符 109">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87826C85-A987-4C33-A807-6DAAF1D20943}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="209" idx="4"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="9144000" y="21869400"/>
+          <a:ext cx="1585711" cy="1401224"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>252094</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>48894</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="216" name="椭圆 215">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9E31E42-4DAD-4DB7-8C2C-0FE9715574F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9124950" y="21850350"/>
+          <a:ext cx="42544" cy="48894"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>114276</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>66650</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="140" name="图片 139">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C644265-3B72-4EAB-A300-A05EE8FFC898}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8467725" y="21364575"/>
+          <a:ext cx="190476" cy="200000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>276204</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>247626</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="141" name="图片 140">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C119F6C-A57E-4C43-B3CB-50DF797C1D50}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9020175" y="22259925"/>
+          <a:ext cx="171429" cy="190476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>361930</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>76176</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="144" name="图片 143">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA0A0E4A-6DBF-4764-BCE6-746EF1640A77}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9486900" y="21383625"/>
+          <a:ext cx="161905" cy="190476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>209531</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>352398</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="145" name="图片 144">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9257B6F4-9C52-484C-8BE6-9126FD724C05}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8972550" y="21631275"/>
+          <a:ext cx="152381" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>57125</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>76170</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="217" name="图片 216">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF382CF6-F4FE-471C-86C4-6FD2B8CA90E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12858750" y="22040850"/>
+          <a:ext cx="200000" cy="238095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>295275</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>142850</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>152374</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="218" name="图片 217">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66A3E6B3-CB08-4F3B-A896-A66296F26A89}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13687425" y="21088350"/>
+          <a:ext cx="200000" cy="209524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>209526</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>133320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="219" name="图片 218">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A0803E5-BE6C-44AC-9DB3-F1D685B51CF6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14135100" y="22098000"/>
+          <a:ext cx="190476" cy="238095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>312117</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>167750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>60499</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>244570</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="220" name="等腰三角形 219">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D25785A3-7C92-45FE-88D4-72717B48F8CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="1074581">
+          <a:off x="12199317" y="20255975"/>
+          <a:ext cx="3463132" cy="2543795"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 31467"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>200000</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>276198</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="221" name="图片 220">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BEB97923-F785-4F26-9F53-330E76302ED3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15230475" y="23317200"/>
+          <a:ext cx="200000" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>104746</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>9498</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="222" name="图片 221">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F99B172-2C7E-4608-8706-2051498AB5CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13620750" y="19878675"/>
+          <a:ext cx="228571" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>323820</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>190471</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="223" name="图片 222">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D50CB420-91D1-46EA-A7FA-15A5D4DDDB42}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11601450" y="22164675"/>
+          <a:ext cx="238095" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>98401</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>28550</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="224" name="图片 223">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B4D7256-0C29-4144-95EE-11B7A01EBC99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12534900" y="20974050"/>
+          <a:ext cx="193651" cy="200000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>76174</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>28552</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="225" name="图片 224">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EE05428-612E-43B3-ADB9-BBBC8F1862CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13239750" y="22755225"/>
+          <a:ext cx="209524" cy="180952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>295275</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>161899</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>142850</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="226" name="图片 225">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA792043-FA3E-4C1D-8A2D-E8DA6BD86945}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14439900" y="21440775"/>
+          <a:ext cx="209524" cy="200000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>114276</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>66650</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="227" name="图片 226">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20B49512-AFD3-4A59-A5D7-EC9604D1C3C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12925425" y="21364575"/>
+          <a:ext cx="190476" cy="200000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>276204</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>247626</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="228" name="图片 227">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E11135E-F183-4AC4-B824-1843BEB89833}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13477875" y="22259925"/>
+          <a:ext cx="171429" cy="190476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>47605</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>47601</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="229" name="图片 228">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B6186BB-8192-4206-85FA-EC61EE948523}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14001750" y="21707475"/>
+          <a:ext cx="161905" cy="190476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>209531</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>352398</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="230" name="图片 229">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80AF55C2-C6FF-4A14-8391-8B117787607C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13430250" y="21631275"/>
+          <a:ext cx="152381" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>223706</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>333299</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>15613</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="231" name="直接连接符 230">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C11E6DB-2A62-40C6-A820-3B9408B41623}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="13596806" y="20107275"/>
+          <a:ext cx="109593" cy="1758688"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>6088</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>223706</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>342338</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="232" name="直接连接符 231">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8D9549F-FADC-4BE5-8A28-AD6BE9417C59}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11887200" y="21856438"/>
+          <a:ext cx="1709606" cy="336250"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>223706</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>6088</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>323517</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>350037</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="233" name="直接连接符 232">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2D88D2A-E47D-474B-82A1-AA071775D634}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="13596806" y="21856438"/>
+          <a:ext cx="1585711" cy="1401224"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -19927,8 +21343,8 @@
   </sheetPr>
   <dimension ref="O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y68" sqref="Y68"/>
+    <sheetView tabSelected="1" topLeftCell="G49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AS61" sqref="AS61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Modified   doc/images/painter.xlsx Modified   doc/一起动手实现3D渲染引擎.md
</commit_message>
<xml_diff>
--- a/doc/images/painter.xlsx
+++ b/doc/images/painter.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\MyGame\Tiny3D\steps\doc\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaronwang\workspace\projects\private\Tiny3D\steps\doc\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12170" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="左右手坐标系" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="几何图元" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -8920,6 +8921,61 @@
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="椭圆 34"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5461000" y="27127200"/>
+          <a:ext cx="1822450" cy="1765300"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>24</xdr:col>
@@ -20962,6 +21018,1635 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>327992</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>164575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>76374</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>241395</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="214" name="等腰三角形 213">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B613182-1A7B-403D-A3CC-A75E50D943CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="1074581">
+          <a:off x="1064592" y="26478975"/>
+          <a:ext cx="3431382" cy="2566020"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 31467"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>15875</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>53975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>215875</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>273023</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="215" name="图片 214">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29F17BB4-4079-4B73-AAEE-C001EC30EDE4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4067175" y="29568775"/>
+          <a:ext cx="200000" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>263525</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>120621</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>6323</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="234" name="图片 233">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAA69513-36B7-4C8D-A1AF-BAE5E12E9247}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2473325" y="26098500"/>
+          <a:ext cx="225396" cy="222223"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>311150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>339695</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>187296</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="235" name="图片 234">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6004B13C-A9FC-4936-BB62-E85B5DB4DC62}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="469900" y="28403550"/>
+          <a:ext cx="238095" cy="231746"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>41537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>354069</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="236" name="直接连接符 235">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{319B2415-8C05-467E-8BCE-2B940EEB63FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2393950" y="26355937"/>
+          <a:ext cx="169919" cy="2612763"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>16582</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>191206</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>347598</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>7219</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="237" name="直接连接符 236">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1876A2BC-F1BB-442D-947F-A4E387BB9824}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="214" idx="2"/>
+          <a:endCxn id="214" idx="5"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="753182" y="27928006"/>
+          <a:ext cx="2540816" cy="527213"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>188245</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>19201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>341112</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>4224</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="238" name="直接连接符 237">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87826C85-A987-4C33-A807-6DAAF1D20943}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="214" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1661445" y="27400401"/>
+          <a:ext cx="2362667" cy="2118623"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>258444</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>36194</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="239" name="椭圆 238">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9E31E42-4DAD-4DB7-8C2C-0FE9715574F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2425700" y="28079700"/>
+          <a:ext cx="42544" cy="48894"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>321643</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>151874</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>70025</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>228694</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="240" name="等腰三角形 239">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B613182-1A7B-403D-A3CC-A75E50D943CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="1074581">
+          <a:off x="5109543" y="26466274"/>
+          <a:ext cx="3431382" cy="2566020"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 31467"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>41274</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>209526</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>260322</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="241" name="图片 240">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29F17BB4-4079-4B73-AAEE-C001EC30EDE4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8112126" y="29556074"/>
+          <a:ext cx="200000" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>257176</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>126999</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>114272</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>349222</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="242" name="图片 241">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAA69513-36B7-4C8D-A1AF-BAE5E12E9247}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6518276" y="26085799"/>
+          <a:ext cx="225396" cy="222223"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>95251</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>298449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>333346</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>174595</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="243" name="图片 242">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6004B13C-A9FC-4936-BB62-E85B5DB4DC62}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4514851" y="28390849"/>
+          <a:ext cx="238095" cy="231746"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>137794</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>296544</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="244" name="椭圆 243">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9E31E42-4DAD-4DB7-8C2C-0FE9715574F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6356350" y="27984450"/>
+          <a:ext cx="42544" cy="48894"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>196850</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>292910</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>101480</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="247" name="直接连接符 246">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{319B2415-8C05-467E-8BCE-2B940EEB63FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6089650" y="28029710"/>
+          <a:ext cx="272930" cy="811990"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>131564</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>273050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>254810</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="248" name="直接连接符 247">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{319B2415-8C05-467E-8BCE-2B940EEB63FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="244" idx="7"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6392664" y="27654250"/>
+          <a:ext cx="820936" cy="337360"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>101480</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>254810</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="249" name="直接连接符 248">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{319B2415-8C05-467E-8BCE-2B940EEB63FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="244" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="5670550" y="27444700"/>
+          <a:ext cx="692030" cy="546910"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>327991</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>158225</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>76373</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>235045</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="250" name="等腰三角形 249">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B613182-1A7B-403D-A3CC-A75E50D943CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="1074581">
+          <a:off x="9535491" y="26472625"/>
+          <a:ext cx="3431382" cy="2566020"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 31467"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>15874</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>215874</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>266673</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="251" name="图片 250">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29F17BB4-4079-4B73-AAEE-C001EC30EDE4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12538074" y="29562425"/>
+          <a:ext cx="200000" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>263524</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>120620</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>355573</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="252" name="图片 251">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAA69513-36B7-4C8D-A1AF-BAE5E12E9247}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10944224" y="26092150"/>
+          <a:ext cx="225396" cy="222223"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>101599</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>339694</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>180946</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="253" name="图片 252">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6004B13C-A9FC-4936-BB62-E85B5DB4DC62}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8940799" y="28397200"/>
+          <a:ext cx="238095" cy="231746"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="254" name="椭圆 253"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9207500" y="26333450"/>
+          <a:ext cx="3714750" cy="3886200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>23494</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>207644</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="256" name="椭圆 255">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9E31E42-4DAD-4DB7-8C2C-0FE9715574F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11029950" y="28251150"/>
+          <a:ext cx="42544" cy="48894"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>354070</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>355480</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>165910</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="259" name="直接连接符 258">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{319B2415-8C05-467E-8BCE-2B940EEB63FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="256" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11034770" y="26333450"/>
+          <a:ext cx="1410" cy="1924860"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>16581</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>183197</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>869</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="262" name="直接连接符 261">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{319B2415-8C05-467E-8BCE-2B940EEB63FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="256" idx="2"/>
+          <a:endCxn id="250" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="9224081" y="28275597"/>
+          <a:ext cx="1805869" cy="173272"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>17264</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>200484</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>335287</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>344878</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="266" name="直接连接符 265">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{319B2415-8C05-467E-8BCE-2B940EEB63FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="256" idx="5"/>
+          <a:endCxn id="250" idx="4"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11066264" y="28292884"/>
+          <a:ext cx="1422923" cy="1211194"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="276" name="立方体 275"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1111250" y="31756350"/>
+          <a:ext cx="2127250" cy="596900"/>
+        </a:xfrm>
+        <a:prstGeom prst="cube">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 29505"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="277" name="椭圆 276"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1022350" y="30956250"/>
+          <a:ext cx="2343150" cy="2298700"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>17144</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>80644</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="278" name="椭圆 277">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9E31E42-4DAD-4DB7-8C2C-0FE9715574F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2184400" y="32035750"/>
+          <a:ext cx="42544" cy="48894"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>254000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>28702</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>47752</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="287" name="立方体 286"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5073650" y="31191200"/>
+          <a:ext cx="1216152" cy="1216152"/>
+        </a:xfrm>
+        <a:prstGeom prst="cube">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="289" name="椭圆 288"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4806950" y="30949900"/>
+          <a:ext cx="1822450" cy="1758950"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>213994</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>220344</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="290" name="椭圆 289">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9E31E42-4DAD-4DB7-8C2C-0FE9715574F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5695950" y="31819850"/>
+          <a:ext cx="42544" cy="48894"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -21270,7 +22955,7 @@
       <selection activeCell="AS13" sqref="AS13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21283,11 +22968,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="AJ22" sqref="AJ22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21304,7 +22989,7 @@
       <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21320,13 +23005,13 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AY16" sqref="AY16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="4.875" style="1"/>
+    <col min="1" max="16384" width="4.83203125" style="1"/>
   </cols>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -21343,13 +23028,13 @@
   </sheetPr>
   <dimension ref="O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AS61" sqref="AS61"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y92" sqref="Y92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="45" spans="15:15" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="15:15" ht="28.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O45" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified   doc/images/painter.xlsx Modified   doc/images/triangle-circ-point.png
</commit_message>
<xml_diff>
--- a/doc/images/painter.xlsx
+++ b/doc/images/painter.xlsx
@@ -8967,15 +8967,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>342900</xdr:rowOff>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>19006</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>209523</xdr:rowOff>
+      <xdr:colOff>9481</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>76173</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8998,7 +8998,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11182350" y="27832050"/>
+          <a:off x="11172825" y="28051125"/>
           <a:ext cx="352381" cy="219048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -22478,8 +22478,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11029950" y="28251150"/>
-          <a:ext cx="42544" cy="48894"/>
+          <a:off x="11122025" y="28000325"/>
+          <a:ext cx="45719" cy="48894"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -22514,69 +22514,74 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>354067</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>22487</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>16799</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>187981</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>349176</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>165910</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="259" name="直接连接符 258">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003010000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="250" idx="5"/>
+          <a:endCxn id="256" idx="7"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="11161049" y="27677131"/>
+          <a:ext cx="703852" cy="330354"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>187417</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>7919</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
       <xdr:colOff>635</xdr:colOff>
       <xdr:row>79</xdr:row>
-      <xdr:rowOff>207644</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="259" name="直接连接符 258">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003010000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="250" idx="0"/>
-          <a:endCxn id="256" idx="4"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11126842" y="26101937"/>
-          <a:ext cx="18043" cy="1947282"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>16581</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>183197</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>349250</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>869</xdr:rowOff>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -22588,18 +22593,23 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="256" idx="2"/>
-          <a:endCxn id="250" idx="2"/>
+          <a:stCxn id="256" idx="0"/>
+          <a:endCxn id="250" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="9224081" y="28275597"/>
-          <a:ext cx="1805869" cy="173272"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="10217242" y="27144644"/>
+          <a:ext cx="927643" cy="855681"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="1">
@@ -22620,16 +22630,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>207644</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>17264</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>200484</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>335287</xdr:colOff>
-      <xdr:row>82</xdr:row>
-      <xdr:rowOff>344878</xdr:rowOff>
+      <xdr:colOff>635</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -22641,18 +22651,22 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="256" idx="5"/>
-          <a:endCxn id="250" idx="4"/>
+          <a:stCxn id="256" idx="4"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11066264" y="28292884"/>
-          <a:ext cx="1422923" cy="1211194"/>
+        <a:xfrm flipH="1">
+          <a:off x="10925175" y="28049219"/>
+          <a:ext cx="219710" cy="659131"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="1">
@@ -23045,6 +23059,59 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>354067</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>22487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>635</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="280" name="直接连接符 279">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF4B4E25-8D51-4146-8122-D0F8438AF0AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="256" idx="0"/>
+          <a:endCxn id="250" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="11126842" y="26101937"/>
+          <a:ext cx="18043" cy="1898388"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -23426,8 +23493,8 @@
   </sheetPr>
   <dimension ref="O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE94" sqref="AE94"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AM78" sqref="AM78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Modified   doc/images/painter.xlsx Modified   doc/一起动手实现3D渲染引擎.md Add        doc/images/triangle-benz.png
</commit_message>
<xml_diff>
--- a/doc/images/painter.xlsx
+++ b/doc/images/painter.xlsx
@@ -23114,6 +23114,588 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>619</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="257" name="等腰三角形 256">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0563E967-79F0-4CCD-83A6-A73FA2844CF0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6686550" y="30318075"/>
+          <a:ext cx="3324225" cy="2458069"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 66764"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="310983" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="258" name="文本框 257">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0DAC1BD-5EC5-4FEA-A255-39956B1D2AEA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8848725" y="29937075"/>
+          <a:ext cx="310983" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>A</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="297325" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="260" name="文本框 259">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0831D1A2-CAF2-4661-BB7C-20D59DDF650F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6315075" y="32775525"/>
+          <a:ext cx="297325" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>B</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="310983" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="265" name="文本框 264">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A6EAAC9-6B51-4668-A26B-902714BC5FC5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10029825" y="32775525"/>
+          <a:ext cx="310983" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>C</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>90169</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>277494</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="267" name="椭圆 266">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7EB6E93-6EB6-4F70-AD9C-64FB9BB658A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8591550" y="31946850"/>
+          <a:ext cx="42544" cy="48894"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>83939</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>362011</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>235760</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="269" name="直接连接符 268">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B048AC19-E125-4637-A0C2-93065D693F9F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="267" idx="7"/>
+          <a:endCxn id="257" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8627864" y="30318075"/>
+          <a:ext cx="278072" cy="1635935"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>83939</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>270334</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>619</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="270" name="直接连接符 269">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CE260EE-1C85-4D87-8485-7CAAF7B10A17}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="257" idx="4"/>
+          <a:endCxn id="267" idx="5"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8627864" y="31988584"/>
+          <a:ext cx="1382911" cy="787560"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>270334</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>53855</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>619</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="273" name="直接连接符 272">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83E0F000-43C3-4139-B32A-A8D558E3E9C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="267" idx="3"/>
+          <a:endCxn id="257" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6686550" y="31988584"/>
+          <a:ext cx="1911230" cy="787560"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="294504" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="279" name="文本框 278">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EBCE974-394B-49CD-84A8-9AE1C85A5624}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8458200" y="31956375"/>
+          <a:ext cx="294504" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>P</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -23493,8 +24075,8 @@
   </sheetPr>
   <dimension ref="O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AM78" sqref="AM78"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AG90" sqref="AG90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Modified   doc/images/painter.xlsx Modified   doc/一起动手实现3D渲染引擎.md Add        doc/images/tetrahedron.png Add        doc/一起动手实现3D渲染引擎1.md
</commit_message>
<xml_diff>
--- a/doc/images/painter.xlsx
+++ b/doc/images/painter.xlsx
@@ -25241,6 +25241,1157 @@
             <a:t>r'</a:t>
           </a:r>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="274" name="直接连接符 273">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BD9721E-9FD8-4500-8278-E97461726262}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7077075" y="34556700"/>
+          <a:ext cx="723900" cy="2076450"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="294" name="直接连接符 293">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{318F0CE5-0FBE-405C-9FE1-A74DB410CBE3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7800975" y="34566225"/>
+          <a:ext cx="742950" cy="2781300"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="299" name="直接连接符 298">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3A5E844-FF79-495B-B4AA-F97798AEBD3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7077075" y="36633150"/>
+          <a:ext cx="1476375" cy="723900"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>5953</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>363141</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>5954</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="301" name="直接连接符 300">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75D6A2AA-4F45-4B16-8545-778B1B0A83AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7756922" y="34444781"/>
+          <a:ext cx="1464469" cy="1738314"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>11906</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>5954</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>345282</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="310" name="直接连接符 309">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05A76393-7C22-4BC0-9450-2BCD6B4AD412}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8489156" y="36189047"/>
+          <a:ext cx="744142" cy="1035844"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>11906</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="314" name="直接连接符 313">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3844370E-30B6-4165-A123-B02598B1D0AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7041356" y="36189047"/>
+          <a:ext cx="2185988" cy="321469"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="lgDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>217885</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>347663</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="310983" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="318" name="文本框 317">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CF87000-DC82-4753-848B-9842A429E35E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7647385" y="34180463"/>
+          <a:ext cx="310983" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>A</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400">
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="228600" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="323" name="文本框 322">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3095C724-AAB4-4E64-AAF6-68476DFC534C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9267825" y="36099750"/>
+          <a:ext cx="228600" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>B</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400">
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>110728</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304763" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="324" name="文本框 323">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6C5A8FC-B07E-447B-909E-613B66ADECAD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6797278" y="36452175"/>
+          <a:ext cx="304763" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>C</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400">
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="321435" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="325" name="文本框 324">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07B83E13-CD99-4D8B-A797-22107D40581C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8410575" y="37309425"/>
+          <a:ext cx="321435" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>D</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400">
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>223519</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>239394</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="326" name="椭圆 325">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1D6876D-B063-4A65-B2B5-9A371BB0AC1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7981950" y="36137850"/>
+          <a:ext cx="42544" cy="48894"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>23813</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>214947</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>327421</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="328" name="直接连接符 327">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEDA7BA9-64A9-4AB2-A394-CA548A26F295}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="326" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7036594" y="36040853"/>
+          <a:ext cx="895350" cy="463709"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>223519</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>214947</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>11906</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="334" name="直接连接符 333">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33FF8830-5B23-4D9D-BF21-E7BCCBED1D4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="326" idx="6"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7974488" y="36040853"/>
+          <a:ext cx="1252856" cy="148194"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>35718</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>202247</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="348" name="直接连接符 347">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E753195-C4FD-4B98-9EAB-29D1333CCC9B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="326" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7750969" y="34456687"/>
+          <a:ext cx="202247" cy="1559719"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>217289</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>232234</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>365961</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>340894</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="149" name="直接连接符 148">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BF0B4C4-5209-419A-90B7-FE7098DC8599}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="326" idx="5"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8007736" y="36026181"/>
+          <a:ext cx="519646" cy="1161424"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>257175</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="330988" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="151" name="文本框 150">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F92346E-C329-48E3-975A-B49FB0AB3154}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7715250" y="35852100"/>
+          <a:ext cx="330988" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>O</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400">
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="283924" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="156" name="文本框 155">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B93AA02-55DB-40F1-AEBB-33D01AE0C041}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8105775" y="35623500"/>
+          <a:ext cx="283924" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>a</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400">
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="299313" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="352" name="文本框 351">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4CEB171-CD36-4E50-B04E-A63D499F7DC6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8867775" y="36718875"/>
+          <a:ext cx="299313" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>b</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400">
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>285750</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="274691" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="353" name="文本框 352">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5386DDFE-CBEF-4E20-B672-F18D413753C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7591425" y="36937950"/>
+          <a:ext cx="274691" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>c</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400">
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
             <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
             <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
           </a:endParaRPr>
@@ -25628,8 +26779,8 @@
   </sheetPr>
   <dimension ref="O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C92" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X102" sqref="X102"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AK104" sqref="AK104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Modified   doc/images/painter.xlsx Missing    doc/images/sphere-objects.png Modified   doc/一起动手实现3D渲染引擎.md Add        doc/images/AABB-transformation.png Add        doc/images/AABB.png Add        doc/images/OBB-transformation.png Add        doc/images/OBB.png Add        doc/images/bounding-sphere.png Add        doc/images/bounding-volumn.png
</commit_message>
<xml_diff>
--- a/doc/images/painter.xlsx
+++ b/doc/images/painter.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\MyGame\Tiny3D\steps\doc\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaronwang\workspace\projects\private\Tiny3D\steps\doc\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12170" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="左右手坐标系" sheetId="1" r:id="rId1"/>
@@ -5576,6 +5576,50 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="67" name="直接连接符 66"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9702800" y="2476500"/>
+          <a:ext cx="241300" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>369278</xdr:colOff>
       <xdr:row>6</xdr:row>
@@ -6668,6 +6712,1449 @@
         </a:fillRef>
         <a:effectRef idx="0">
           <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>11410</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>14654</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>4089</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>344369</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="直接箭头连接符 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8482310" y="4281854"/>
+          <a:ext cx="1097579" cy="329715"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>11411</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>4088</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>3</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="直接箭头连接符 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="9218911" y="3556000"/>
+          <a:ext cx="360977" cy="1066803"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>7015</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>350228</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="直接连接符 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000012000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="9569450" y="3213100"/>
+          <a:ext cx="13365" cy="1404328"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>6282</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>4083</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="直接连接符 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000014000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9582082" y="365125"/>
+          <a:ext cx="4417401" cy="701675"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>4084</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>4083</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>7327</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="直接连接符 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000016000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9579884" y="355600"/>
+          <a:ext cx="368299" cy="2140927"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>664</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>234950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>350229</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="直接连接符 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00001E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9576464" y="4146550"/>
+          <a:ext cx="1529686" cy="470879"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>74840</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="383567" cy="334451"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="文本框 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00003E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8877301" y="3275240"/>
+          <a:ext cx="383567" cy="334451"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+Y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="390813" cy="334451"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="文本框 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00003F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8140700" y="4088493"/>
+          <a:ext cx="390813" cy="334451"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+X</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>208191</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>285750</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="618824" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="文本框 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000040000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8679091" y="4908550"/>
+          <a:ext cx="618824" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>Origin</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>(0, 0, 0)</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>337458</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>34018</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>303440</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>346982</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="直接连接符 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000042000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9176658" y="4656818"/>
+          <a:ext cx="334282" cy="312964"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>7014</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>18737</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>342901</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="直接箭头连接符 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9582814" y="3556000"/>
+          <a:ext cx="748323" cy="1054101"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>4083</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>40821</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="438069" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="文本框 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00003D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9948183" y="3241221"/>
+          <a:ext cx="438069" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>Z</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>4083</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="40" name="直接连接符 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00004A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9944100" y="2495550"/>
+          <a:ext cx="4423683" cy="698500"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>367322</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>346075</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="直接连接符 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000018000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14001750" y="1066800"/>
+          <a:ext cx="360972" cy="2124075"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>332642</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="42" name="直接连接符 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00001C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9582150" y="3905250"/>
+          <a:ext cx="120650" cy="694592"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>292100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>11236</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="直接连接符 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000020000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9575800" y="3492500"/>
+          <a:ext cx="1409700" cy="1141536"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>298450</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>298450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="直接连接符 5"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9582150" y="3213100"/>
+          <a:ext cx="1397000" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>311150</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>292100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>234950</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="直接连接符 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10991850" y="3492500"/>
+          <a:ext cx="120650" cy="654050"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>120650</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>336550</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="直接连接符 10"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9575800" y="3225800"/>
+          <a:ext cx="120650" cy="666750"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="直接连接符 12"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9690100" y="3898900"/>
+          <a:ext cx="1416050" cy="241300"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="50" name="直接连接符 49"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9569450" y="349250"/>
+          <a:ext cx="12700" cy="2870200"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>298450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="52" name="直接连接符 51"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10985500" y="1073150"/>
+          <a:ext cx="3009900" cy="2425700"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="55" name="直接连接符 54"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11118850" y="3194050"/>
+          <a:ext cx="3244850" cy="946150"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1372492" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="71" name="文本框 70"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11353800" y="4279900"/>
+          <a:ext cx="1372492" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>Near Clip Plane</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>190858</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="75" name="直接连接符 74"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="71" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="10744200" y="3943350"/>
+          <a:ext cx="609600" cy="514708"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>207063</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>221505</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1405837" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="77" name="文本框 76"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14202463" y="577105"/>
+          <a:ext cx="1405837" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>Far</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1" baseline="0">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t> Clip Plane</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="79" name="直接连接符 78"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="12172951" y="825500"/>
+          <a:ext cx="2025649" cy="863600"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -26706,7 +28193,7 @@
       <selection activeCell="AS13" sqref="AS13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26723,7 +28210,7 @@
       <selection activeCell="AJ22" sqref="AJ22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26736,11 +28223,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AO8" sqref="AO8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26760,9 +28247,9 @@
       <selection activeCell="AY16" sqref="AY16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="4.875" style="1"/>
+    <col min="1" max="16384" width="4.83203125" style="1"/>
   </cols>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -26779,13 +28266,13 @@
   </sheetPr>
   <dimension ref="O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AK104" sqref="AK104"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D111" sqref="D111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="45" spans="15:15" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="15:15" ht="28.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O45" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified   doc/images/painter.xlsx Modified   doc/一起动手实现3D渲染引擎.md Add        doc/images/frustum.png
</commit_message>
<xml_diff>
--- a/doc/images/painter.xlsx
+++ b/doc/images/painter.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaronwang\workspace\projects\private\Tiny3D\steps\doc\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\MyGame\Tiny3D\steps\doc\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12170" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="左右手坐标系" sheetId="1" r:id="rId1"/>
@@ -5589,7 +5589,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="67" name="直接连接符 66"/>
+        <xdr:cNvPr id="67" name="直接连接符 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000043000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -6738,7 +6744,7 @@
         <xdr:cNvPr id="21" name="直接箭头连接符 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6794,7 +6800,7 @@
         <xdr:cNvPr id="23" name="直接箭头连接符 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6850,7 +6856,7 @@
         <xdr:cNvPr id="25" name="直接连接符 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6901,7 +6907,7 @@
         <xdr:cNvPr id="27" name="直接连接符 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00001B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6952,7 +6958,7 @@
         <xdr:cNvPr id="29" name="直接连接符 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00001D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7003,7 +7009,7 @@
         <xdr:cNvPr id="31" name="直接连接符 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00001E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00001F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7049,7 +7055,7 @@
         <xdr:cNvPr id="33" name="文本框 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00003E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000021000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7120,7 +7126,7 @@
         <xdr:cNvPr id="34" name="文本框 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00003F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000022000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7191,7 +7197,7 @@
         <xdr:cNvPr id="35" name="文本框 34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000040000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7261,7 +7267,7 @@
         <xdr:cNvPr id="36" name="直接连接符 35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000042000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000024000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7316,7 +7322,7 @@
         <xdr:cNvPr id="37" name="直接箭头连接符 36">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000025000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7364,7 +7370,7 @@
         <xdr:cNvPr id="38" name="文本框 37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00003D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000026000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7450,7 +7456,7 @@
         <xdr:cNvPr id="40" name="直接连接符 39">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00004A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000028000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7501,7 +7507,7 @@
         <xdr:cNvPr id="41" name="直接连接符 40">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000029000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7552,7 +7558,7 @@
         <xdr:cNvPr id="42" name="直接连接符 41">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00001C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00002A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7603,7 +7609,7 @@
         <xdr:cNvPr id="43" name="直接连接符 42">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000020000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00002B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7651,7 +7657,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="6" name="直接连接符 5"/>
+        <xdr:cNvPr id="6" name="直接连接符 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -7696,7 +7708,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="直接连接符 8"/>
+        <xdr:cNvPr id="9" name="直接连接符 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -7741,7 +7759,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="11" name="直接连接符 10"/>
+        <xdr:cNvPr id="11" name="直接连接符 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -7786,7 +7810,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="13" name="直接连接符 12"/>
+        <xdr:cNvPr id="13" name="直接连接符 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -7831,7 +7861,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="50" name="直接连接符 49"/>
+        <xdr:cNvPr id="50" name="直接连接符 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000032000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -7875,7 +7911,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="52" name="直接连接符 51"/>
+        <xdr:cNvPr id="52" name="直接连接符 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000034000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -7919,7 +7961,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="55" name="直接连接符 54"/>
+        <xdr:cNvPr id="55" name="直接连接符 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000037000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -7958,7 +8006,13 @@
     <xdr:ext cx="1372492" cy="356316"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="71" name="文本框 70"/>
+        <xdr:cNvPr id="71" name="文本框 70">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000047000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -8022,7 +8076,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="75" name="直接连接符 74"/>
+        <xdr:cNvPr id="75" name="直接连接符 74">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00004B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="71" idx="1"/>
         </xdr:cNvCxnSpPr>
@@ -8055,21 +8115,27 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>207063</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>221505</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1405837" cy="356316"/>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>368988</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>66129</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1405837" cy="400366"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="77" name="文本框 76"/>
+        <xdr:cNvPr id="77" name="文本框 76">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00004D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14202463" y="577105"/>
-          <a:ext cx="1405837" cy="356316"/>
+        <a:xfrm rot="21181310">
+          <a:off x="10770288" y="1475829"/>
+          <a:ext cx="1405837" cy="400366"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8093,24 +8159,28 @@
       <xdr:txBody>
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
           <a:spAutoFit/>
+          <a:scene3d>
+            <a:camera prst="perspectiveContrastingLeftFacing"/>
+            <a:lightRig rig="threePt" dir="t"/>
+          </a:scene3d>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
               <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
               <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
             </a:rPr>
             <a:t>Far</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1" baseline="0">
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1" baseline="0">
               <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
               <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
             </a:rPr>
             <a:t> Clip Plane</a:t>
           </a:r>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
             <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
             <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
           </a:endParaRPr>
@@ -8119,50 +8189,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>19051</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>266700</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="79" name="直接连接符 78"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="12172951" y="825500"/>
-          <a:ext cx="2025649" cy="863600"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -10425,7 +10451,7 @@
         <xdr:cNvPr id="121" name="图片 120">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D39A09E-807A-48AA-8346-8C8438336AA4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000079000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10469,7 +10495,7 @@
         <xdr:cNvPr id="319" name="图片 318">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45C930AF-E393-4C48-8003-85FB078F964B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003F010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10513,7 +10539,7 @@
         <xdr:cNvPr id="264" name="图片 263">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1911DAE8-A1FB-46EE-B0D4-AD9CBA3B188F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000008010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10557,7 +10583,7 @@
         <xdr:cNvPr id="263" name="图片 262">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A2057B7-7897-4D98-BB67-A1E94753D8A8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000007010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10601,7 +10627,7 @@
         <xdr:cNvPr id="261" name="图片 260">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54B274B2-C868-4B8F-83E7-11C7A677808E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10645,7 +10671,7 @@
         <xdr:cNvPr id="63" name="图片 62">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF392508-E49C-42F3-86EA-2372B86B4081}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10689,7 +10715,7 @@
         <xdr:cNvPr id="50" name="图片 49">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E0B3530-5C37-48E2-A030-8102EADAE8E6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000032000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10733,7 +10759,7 @@
         <xdr:cNvPr id="255" name="图片 254">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82F3A98D-3693-481B-8432-DC669BFBDDD5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000FF000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10777,7 +10803,7 @@
         <xdr:cNvPr id="246" name="图片 245">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{478D9213-3C23-4300-95AD-2CF48594BF1C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000F6000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10821,7 +10847,7 @@
         <xdr:cNvPr id="245" name="图片 244">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AA50951-C023-47BB-9572-E452BFDC5B49}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000F5000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24654,7 +24680,7 @@
         <xdr:cNvPr id="280" name="直接连接符 279">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF4B4E25-8D51-4146-8122-D0F8438AF0AA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000018010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24707,7 +24733,7 @@
         <xdr:cNvPr id="257" name="等腰三角形 256">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0563E967-79F0-4CCD-83A6-A73FA2844CF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000001010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24765,7 +24791,7 @@
         <xdr:cNvPr id="258" name="文本框 257">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0DAC1BD-5EC5-4FEA-A255-39956B1D2AEA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24840,7 +24866,7 @@
         <xdr:cNvPr id="260" name="文本框 259">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0831D1A2-CAF2-4661-BB7C-20D59DDF650F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24915,7 +24941,7 @@
         <xdr:cNvPr id="265" name="文本框 264">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A6EAAC9-6B51-4668-A26B-902714BC5FC5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000009010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24995,7 +25021,7 @@
         <xdr:cNvPr id="267" name="椭圆 266">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7EB6E93-6EB6-4F70-AD9C-64FB9BB658A0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000B010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25055,7 +25081,7 @@
         <xdr:cNvPr id="269" name="直接连接符 268">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B048AC19-E125-4637-A0C2-93065D693F9F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000D010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25108,7 +25134,7 @@
         <xdr:cNvPr id="270" name="直接连接符 269">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CE260EE-1C85-4D87-8485-7CAAF7B10A17}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000E010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25161,7 +25187,7 @@
         <xdr:cNvPr id="273" name="直接连接符 272">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83E0F000-43C3-4139-B32A-A8D558E3E9C0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000011010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25209,7 +25235,7 @@
         <xdr:cNvPr id="279" name="文本框 278">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EBCE974-394B-49CD-84A8-9AE1C85A5624}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000017010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25289,7 +25315,7 @@
         <xdr:cNvPr id="282" name="图片 281">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EADBD94-E4C5-4888-B24B-2D2273187615}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001A010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25333,7 +25359,7 @@
         <xdr:cNvPr id="283" name="图片 282">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34D86CD1-7E23-48C7-82F7-F80F8F2AE336}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001B010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25377,7 +25403,7 @@
         <xdr:cNvPr id="284" name="等腰三角形 283">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD46FB21-30DA-4735-835E-3991F40AF60A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001C010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25440,7 +25466,7 @@
         <xdr:cNvPr id="285" name="图片 284">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{684053B7-B055-459C-B7A5-8DAD5547D4FF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001D010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25484,7 +25510,7 @@
         <xdr:cNvPr id="286" name="图片 285">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC49A481-6B9B-4EB7-95AA-5F6EE2AEF3A1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001E010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25528,7 +25554,7 @@
         <xdr:cNvPr id="288" name="图片 287">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CF64B5A-18E2-4489-B2A8-138639765288}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000020010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25572,7 +25598,7 @@
         <xdr:cNvPr id="291" name="椭圆 290">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F7213F5-EB25-406F-A999-62BE85ADBED0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000023010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25633,7 +25659,7 @@
         <xdr:cNvPr id="293" name="直接连接符 292">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67E8037C-C680-4221-AABB-8137EB7FDF86}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000025010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25686,7 +25712,7 @@
         <xdr:cNvPr id="295" name="直接连接符 294">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01A8E611-FEC6-45B6-9E75-EAA6ED742EAA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000027010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25739,7 +25765,7 @@
         <xdr:cNvPr id="297" name="直接连接符 296">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DC16FAD-BF24-4F63-9209-18A088553D10}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000029010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25791,7 +25817,7 @@
         <xdr:cNvPr id="298" name="直接连接符 297">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22428942-1125-4C8E-A5A2-9DADBDB0BC09}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002A010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25846,7 +25872,7 @@
         <xdr:cNvPr id="303" name="直接连接符 302">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38F701D4-04B7-418E-BB86-446F6FCD9877}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002F010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25901,7 +25927,7 @@
         <xdr:cNvPr id="304" name="直接连接符 303">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1152A8F3-DC78-4926-AFB6-FFBAA018CBFF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000030010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25956,7 +25982,7 @@
         <xdr:cNvPr id="292" name="椭圆 291">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D958A3A-DBB1-4B43-ABA4-2BA98DF5AA0B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000024010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26016,7 +26042,7 @@
         <xdr:cNvPr id="305" name="图片 304">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E09FA5B-9A82-47DD-909B-765410D64C54}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000031010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26060,7 +26086,7 @@
         <xdr:cNvPr id="306" name="图片 305">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C00477DD-8BB2-4B56-99D0-28BE1D0BEAEE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000032010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26104,7 +26130,7 @@
         <xdr:cNvPr id="307" name="图片 306">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92A62624-E77A-4DCB-8813-2567F0A2B61D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000033010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26148,7 +26174,7 @@
         <xdr:cNvPr id="308" name="椭圆 307">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3020A129-DEDE-4EAD-B4F8-A26BAF55D6EA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000034010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26209,7 +26235,7 @@
         <xdr:cNvPr id="309" name="椭圆 308">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{951D1B42-4B5F-47FF-B688-A3F751C369CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000035010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26269,7 +26295,7 @@
         <xdr:cNvPr id="311" name="直接连接符 310">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC8DD371-0C80-4022-B980-A7284FB88FF2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000037010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26322,7 +26348,7 @@
         <xdr:cNvPr id="312" name="椭圆 311">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A19B8BA-0FA1-45EC-898D-450CECE56307}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000038010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26382,7 +26408,7 @@
         <xdr:cNvPr id="316" name="直接连接符 315">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7DFDAB9-FEA4-413D-9C23-328E2629F957}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003C010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26435,7 +26461,7 @@
         <xdr:cNvPr id="317" name="文本框 316">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C4A04BE-DF79-498F-822E-0A039AA12F05}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003D010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26511,7 +26537,7 @@
         <xdr:cNvPr id="320" name="椭圆 319">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A58DF5D-DEA3-4DF1-8998-31EAB7C6B978}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000040010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26579,7 +26605,7 @@
         <xdr:cNvPr id="112" name="图片 111">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55DB324B-F6BE-49AB-B45F-9BFB95B84A62}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000070000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26623,7 +26649,7 @@
         <xdr:cNvPr id="127" name="椭圆 126">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F5B8CA8-C3EB-4089-842E-DA2222DEEFB3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00007F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26684,7 +26710,7 @@
         <xdr:cNvPr id="321" name="文本框 320">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9C3EE79-34F7-4198-BC40-DE7C245C8154}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000041010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26754,7 +26780,7 @@
         <xdr:cNvPr id="274" name="直接连接符 273">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BD9721E-9FD8-4500-8278-E97461726262}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000012010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26804,7 +26830,7 @@
         <xdr:cNvPr id="294" name="直接连接符 293">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{318F0CE5-0FBE-405C-9FE1-A74DB410CBE3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000026010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26854,7 +26880,7 @@
         <xdr:cNvPr id="299" name="直接连接符 298">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3A5E844-FF79-495B-B4AA-F97798AEBD3F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002B010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26904,7 +26930,7 @@
         <xdr:cNvPr id="301" name="直接连接符 300">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75D6A2AA-4F45-4B16-8545-778B1B0A83AD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002D010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26954,7 +26980,7 @@
         <xdr:cNvPr id="310" name="直接连接符 309">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05A76393-7C22-4BC0-9450-2BCD6B4AD412}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000036010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27004,7 +27030,7 @@
         <xdr:cNvPr id="314" name="直接连接符 313">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3844370E-30B6-4165-A123-B02598B1D0AA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003A010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27052,7 +27078,7 @@
         <xdr:cNvPr id="318" name="文本框 317">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CF87000-DC82-4753-848B-9842A429E35E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003E010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27123,7 +27149,7 @@
         <xdr:cNvPr id="323" name="文本框 322">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3095C724-AAB4-4E64-AAF6-68476DFC534C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000043010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27194,7 +27220,7 @@
         <xdr:cNvPr id="324" name="文本框 323">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6C5A8FC-B07E-447B-909E-613B66ADECAD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000044010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27265,7 +27291,7 @@
         <xdr:cNvPr id="325" name="文本框 324">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07B83E13-CD99-4D8B-A797-22107D40581C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000045010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27341,7 +27367,7 @@
         <xdr:cNvPr id="326" name="椭圆 325">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1D6876D-B063-4A65-B2B5-9A371BB0AC1F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000046010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27401,7 +27427,7 @@
         <xdr:cNvPr id="328" name="直接连接符 327">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEDA7BA9-64A9-4AB2-A394-CA548A26F295}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000048010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27456,7 +27482,7 @@
         <xdr:cNvPr id="334" name="直接连接符 333">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33FF8830-5B23-4D9D-BF21-E7BCCBED1D4F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00004E010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27511,7 +27537,7 @@
         <xdr:cNvPr id="348" name="直接连接符 347">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E753195-C4FD-4B98-9EAB-29D1333CCC9B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00005C010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27566,7 +27592,7 @@
         <xdr:cNvPr id="149" name="直接连接符 148">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BF0B4C4-5209-419A-90B7-FE7098DC8599}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000095000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27616,7 +27642,7 @@
         <xdr:cNvPr id="151" name="文本框 150">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F92346E-C329-48E3-975A-B49FB0AB3154}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000097000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27687,7 +27713,7 @@
         <xdr:cNvPr id="156" name="文本框 155">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B93AA02-55DB-40F1-AEBB-33D01AE0C041}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00009C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27758,7 +27784,7 @@
         <xdr:cNvPr id="352" name="文本框 351">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4CEB171-CD36-4E50-B04E-A63D499F7DC6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000060010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27829,7 +27855,7 @@
         <xdr:cNvPr id="353" name="文本框 352">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5386DDFE-CBEF-4E20-B672-F18D413753C1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000061010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28193,7 +28219,7 @@
       <selection activeCell="AS13" sqref="AS13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28206,11 +28232,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="AJ22" sqref="AJ22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28223,11 +28249,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AO8" sqref="AO8"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AR18" sqref="AR18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28247,9 +28273,9 @@
       <selection activeCell="AY16" sqref="AY16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="4.83203125" style="1"/>
+    <col min="1" max="16384" width="4.875" style="1"/>
   </cols>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -28266,13 +28292,13 @@
   </sheetPr>
   <dimension ref="O45"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D111" sqref="D111"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="45" spans="15:15" ht="28.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="15:15" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O45" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified   doc/images/painter.xlsx Modified   doc/一起动手实现3D渲染引擎.md Add        doc/images/vector-add-interpretation.png Add        doc/images/vector-additive.png Add        doc/images/vector-length.png Add        doc/images/vector-mul-scalar.png Add        doc/images/vector-negative.png Add        doc/images/vector-normalize.png
</commit_message>
<xml_diff>
--- a/doc/images/painter.xlsx
+++ b/doc/images/painter.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaronwang\workspace\projects\private\Tiny3D\steps\doc\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\MyGame\Tiny3D\steps\doc\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12170" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="左右手坐标系" sheetId="1" r:id="rId1"/>
@@ -10446,7 +10446,7 @@
         <xdr:cNvPr id="40" name="直接箭头连接符 39">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000028000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10499,7 +10499,7 @@
         <xdr:cNvPr id="42" name="直接箭头连接符 41">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00002A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10552,7 +10552,7 @@
         <xdr:cNvPr id="44" name="直接箭头连接符 43">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00002C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10605,7 +10605,7 @@
         <xdr:cNvPr id="46" name="直接箭头连接符 45">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00002E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10658,7 +10658,7 @@
         <xdr:cNvPr id="49" name="直接箭头连接符 48">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000031000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10711,7 +10711,7 @@
         <xdr:cNvPr id="52" name="直接箭头连接符 51">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000034000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10756,7 +10756,13 @@
     <xdr:ext cx="481286" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="48" name="文本框 47"/>
+        <xdr:cNvPr id="48" name="文本框 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000030000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10813,7 +10819,13 @@
     <xdr:ext cx="567720" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="60" name="文本框 59"/>
+        <xdr:cNvPr id="60" name="文本框 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00003C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10870,7 +10882,13 @@
     <xdr:ext cx="481286" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="62" name="文本框 61"/>
+        <xdr:cNvPr id="62" name="文本框 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00003E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10927,7 +10945,13 @@
     <xdr:ext cx="524503" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="63" name="文本框 62"/>
+        <xdr:cNvPr id="63" name="文本框 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00003F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10984,7 +11008,13 @@
     <xdr:ext cx="481286" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="65" name="文本框 64"/>
+        <xdr:cNvPr id="65" name="文本框 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000041000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -11041,7 +11071,13 @@
     <xdr:ext cx="524503" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="67" name="文本框 66"/>
+        <xdr:cNvPr id="67" name="文本框 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000043000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -11083,6 +11119,4486 @@
             <a:t>]</a:t>
           </a:r>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="直接连接符 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70FF2FE7-E0E3-427F-9C55-016D301386B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7248525" y="6762750"/>
+          <a:ext cx="190500" cy="276225"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>357188</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="直接连接符 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EB03866-6221-4E34-9CE6-F728CB73CF42}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9458325" y="5362575"/>
+          <a:ext cx="185738" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="直接箭头连接符 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5516069A-AFD7-450A-AB49-AE97F82AE43F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7448550" y="5667376"/>
+          <a:ext cx="2219325" cy="1390649"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="直接连接符 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D0BF531-02F9-4E94-981E-42EEC530AD6F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7439025" y="7048500"/>
+          <a:ext cx="2219325" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="直接连接符 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93F16D3E-05AD-4948-B734-0734A0668BF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9658350" y="5667375"/>
+          <a:ext cx="0" cy="1371600"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="直接连接符 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76015C12-9094-4BDC-9BBA-4C918A17EACB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9658350" y="5657850"/>
+          <a:ext cx="361950" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="72" name="直接连接符 71">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25A0D511-26A9-41CB-AB27-D3360405B7D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9658350" y="7048500"/>
+          <a:ext cx="361950" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="73" name="直接连接符 72">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8234346A-B2E8-4CB0-8535-5C083E68691C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7429500" y="7058025"/>
+          <a:ext cx="0" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="77" name="直接连接符 76">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDBF0435-081E-4AB4-9228-DCE7A021DE1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9658350" y="7048500"/>
+          <a:ext cx="0" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>257175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="79" name="直接连接符 78">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78146CA3-4CF2-4BCA-B364-13C83250856B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7391400" y="5543550"/>
+          <a:ext cx="2085975" cy="1314450"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95252</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>276225</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="81" name="直接连接符 80">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C47B9838-DDBC-4CA7-94F9-F33CF33D4D31}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9839325" y="5734052"/>
+          <a:ext cx="1" cy="1238248"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>304801</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="85" name="直接连接符 84">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDDD1F85-1303-4723-BD46-FDC8935504F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7496175" y="7239000"/>
+          <a:ext cx="2095501" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>76149</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9489</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="89" name="图片 88">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE82CE5C-D14D-4A86-AC2E-499EFD1E6BFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="19702003">
+          <a:off x="8201026" y="6067425"/>
+          <a:ext cx="419048" cy="285714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>199977</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>342864</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="90" name="图片 89">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{124DDA03-8183-4563-8F99-D50DD8BBE132}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8362950" y="7105650"/>
+          <a:ext cx="380952" cy="285714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>28527</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>152364</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="91" name="图片 90">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BC4E008-445D-492B-9A1C-7FEDBBA1AFB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9677400" y="6210300"/>
+          <a:ext cx="380952" cy="285714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="92" name="矩形 91">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{051985B7-930A-4613-B244-596226D4A3AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6858000" y="5181600"/>
+          <a:ext cx="3467100" cy="2419350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="93" name="直接箭头连接符 92">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DBAD525-45D8-41A3-B5A2-314ABC4E0827}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="13001625" y="6000750"/>
+          <a:ext cx="752475" cy="1409701"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>9527</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="97" name="直接箭头连接符 96">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{505B3E78-5882-4003-99A2-6D033F71532A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="13744575" y="4581525"/>
+          <a:ext cx="1495425" cy="2828927"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>9527</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="99" name="直接箭头连接符 98">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30B85653-E320-43FC-8CED-17AF642A953C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="14487525" y="6705600"/>
+          <a:ext cx="371475" cy="704852"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="101" name="直接箭头连接符 100">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EBC80EA-A81B-438D-977F-7E5C7AF37EB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="15240000" y="6000750"/>
+          <a:ext cx="733425" cy="1400175"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>161889</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>257146</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="105" name="图片 104">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF6A024A-AEB9-4CAC-A2E7-30E418719952}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12877800" y="7429500"/>
+          <a:ext cx="285714" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>142839</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>257146</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="106" name="图片 105">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6517E79C-31F8-4AF6-B45A-C637C039A106}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13601700" y="7429500"/>
+          <a:ext cx="285714" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>104661</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>257146</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="107" name="图片 106">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70E6F4AB-5C3E-415F-B2EC-B38C3E773808}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14049375" y="7429500"/>
+          <a:ext cx="914286" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>219027</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>257146</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="108" name="图片 107">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{060F84AE-8479-425D-B150-C171202646BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15068550" y="7429500"/>
+          <a:ext cx="380952" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="109" name="直接箭头连接符 108">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACE5CED3-2DCC-4027-B0C3-14E4BF2AFB9D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3352800" y="9172576"/>
+          <a:ext cx="733425" cy="1400174"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="110" name="椭圆 109">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC3EAA16-62D5-4EDE-9DDA-DF710FEA155D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2981325" y="10220325"/>
+          <a:ext cx="733425" cy="704850"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="112" name="直接箭头连接符 111">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90648F1D-09BD-45AC-A0B9-52EEF0FF9236}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3352800" y="10267950"/>
+          <a:ext cx="171450" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="117" name="直接箭头连接符 116">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43410449-AD74-4B2F-B731-FF4F0765A348}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3352800" y="10229850"/>
+          <a:ext cx="733425" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>209551</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="120" name="直接箭头连接符 119">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{156B7302-8BA8-4D3D-8284-B27C0EA43839}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3352800" y="10429876"/>
+          <a:ext cx="333375" cy="142874"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="122" name="直接箭头连接符 121">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AAA7AEA-4BF3-449F-88DA-733D96B3C65A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3352800" y="10572750"/>
+          <a:ext cx="733425" cy="704850"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>264067</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>249202</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="125" name="直接箭头连接符 124">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D8F8C7E-01DE-4169-8997-EB458031981F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="110" idx="5"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3352800" y="10582275"/>
+          <a:ext cx="254542" cy="239677"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="129" name="直接箭头连接符 128">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B61B940-998B-4DB4-A257-4FC57F603CD8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2981325" y="9877425"/>
+          <a:ext cx="361952" cy="695326"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>221708</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>55599</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="134" name="直接箭头连接符 133">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5711309A-1340-4917-A5A5-F069DB75139F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3193508" y="10275924"/>
+          <a:ext cx="159292" cy="296826"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="139" name="直接箭头连接符 138">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A292BC2A-7B58-4CB2-A451-127E753FDCD0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1866900" y="10572750"/>
+          <a:ext cx="1485900" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="143" name="直接箭头连接符 142">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DEFF2CD-9C7A-4D4A-BFB2-EC8685DA14B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3009900" y="10572750"/>
+          <a:ext cx="342900" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="146" name="直接箭头连接符 145">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65E50015-AAAB-4D11-9EC2-8764296B8302}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2609850" y="10572750"/>
+          <a:ext cx="742950" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>116933</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>249202</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="150" name="直接箭头连接符 149">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80E61FEC-62F5-4AE9-BF66-9887AB41C394}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="110" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3088733" y="10572750"/>
+          <a:ext cx="264067" cy="249202"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="153" name="直接箭头连接符 152">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DA4030B-322A-4B70-B545-8461A5DFEEEC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3352800" y="10572750"/>
+          <a:ext cx="1847850" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="156" name="直接箭头连接符 155">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9889E6A-81D8-43A7-8019-E58C884EBD8A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3352800" y="10572750"/>
+          <a:ext cx="361951" cy="76200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>9528</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="160" name="直接箭头连接符 159">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8E6D72C-BBBE-4952-AFF4-7945DA572964}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7429500" y="9172575"/>
+          <a:ext cx="1123950" cy="1057278"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="163" name="直接箭头连接符 162">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19A0C9EF-9BCF-4DB3-BCA0-B0701730BDB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7429500" y="10220325"/>
+          <a:ext cx="1857375" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="165" name="直接箭头连接符 164">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1006688A-7329-436E-992A-580CD7F45D03}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8553450" y="9172575"/>
+          <a:ext cx="733425" cy="1047750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="169" name="直接箭头连接符 168">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64215948-8C99-48E6-BF85-86A4918C4AEA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9667875" y="8820150"/>
+          <a:ext cx="1485900" cy="704850"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="172" name="直接箭头连接符 171">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D0AB8E5-C02E-4892-A0BA-155ECE411C22}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="9658350" y="9525000"/>
+          <a:ext cx="1104900" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="176" name="直接箭头连接符 175">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D1F0109-DCA6-480D-A86D-97DBE4874681}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10772775" y="8820150"/>
+          <a:ext cx="381000" cy="1409700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>276225</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>199965</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>152371</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="182" name="图片 181">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14522A99-79A4-4EA3-A239-92621DD78FC6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7524750" y="9439275"/>
+          <a:ext cx="476190" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>333315</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>199996</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="183" name="图片 182">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54EA3518-1988-403C-A39C-7BA5777E3BE7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11001375" y="9486900"/>
+          <a:ext cx="476190" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>314301</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>238096</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="184" name="图片 183">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7E45698-0BD7-4129-9474-B9DB326BE480}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8296275" y="10229850"/>
+          <a:ext cx="190476" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>190479</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>190471</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="188" name="图片 187">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E740FB8-9E39-4312-B05D-DF24FFD6D98F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8934450" y="9477375"/>
+          <a:ext cx="171429" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>342876</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>19021</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="189" name="图片 188">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BB576D5-252A-433C-8AA4-AA40D1CB03FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10182225" y="8953500"/>
+          <a:ext cx="190476" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>171429</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>238096</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="190" name="图片 189">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB34C687-3450-42E6-A1A5-0A110199CFEA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10029825" y="9877425"/>
+          <a:ext cx="171429" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="191" name="直接箭头连接符 190">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A78DD0F-C429-42DE-8C77-D033E846E293}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7429500" y="10934700"/>
+          <a:ext cx="1857375" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>342901</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="192" name="直接箭头连接符 191">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D530FEB-965F-46EA-85C2-A21313C2B508}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="7429500" y="10934700"/>
+          <a:ext cx="742950" cy="1038226"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="196" name="直接箭头连接符 195">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B1C6B32-F7DD-4DD3-8BE4-1D7B7113F1B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8172450" y="10925176"/>
+          <a:ext cx="1114426" cy="1057274"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>114240</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>323821</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="200" name="图片 199">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E930D3B-0FEC-465D-8DBA-A3C9F329BE40}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8181975" y="10668000"/>
+          <a:ext cx="476190" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>38076</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>28546</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="201" name="图片 200">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F37D8365-A5EF-42B2-9458-04EBA72DA0F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8763000" y="11430000"/>
+          <a:ext cx="190476" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>333354</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>19021</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="202" name="图片 201">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E43ED91-214B-44EB-A211-8C1FBDE5475E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7591425" y="11420475"/>
+          <a:ext cx="171429" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="203" name="直接箭头连接符 202">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D036F415-7DE6-46FE-A5A9-1D73186B01CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9658350" y="10944224"/>
+          <a:ext cx="1857375" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="204" name="直接箭头连接符 203">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC5868F9-0083-45B4-9CBC-0843F99C1198}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="9658350" y="10944224"/>
+          <a:ext cx="742950" cy="1038226"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="205" name="直接箭头连接符 204">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E780EEA9-4AB9-458D-893D-752434F93F27}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10401300" y="10934700"/>
+          <a:ext cx="1114426" cy="1057274"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>85665</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>323821</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="207" name="图片 206">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17856DD4-F76A-4D77-8E6E-CCFBC43112BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10382250" y="10668000"/>
+          <a:ext cx="476190" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>66654</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>47596</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="208" name="图片 207">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FB65C37-1FBE-43A3-9B3D-F6EC5C11D4B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11039475" y="11449050"/>
+          <a:ext cx="171429" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>352401</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>47596</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="209" name="图片 208">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED20F967-31B3-4799-8C6B-7A2E0D2A69EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9820275" y="11449050"/>
+          <a:ext cx="190476" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>4763</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>4763</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>339725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="210" name="直接箭头连接符 209">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA9A16AB-A571-49B7-AB5C-EA69F28D6881}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18578513" y="736600"/>
+          <a:ext cx="0" cy="4889500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>366713</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>3175</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="211" name="直接箭头连接符 210">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{157B3D09-C689-4D44-97DF-8F72BBE3E2CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="17454563" y="742950"/>
+          <a:ext cx="4465637" cy="4191000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>365125</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>60</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="212" name="直接箭头连接符 211">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CA0B4D5-DF7C-4564-978B-05F9A2029994}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17081500" y="3876675"/>
+          <a:ext cx="5232400" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>155575</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="437749" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="213" name="文本框 212">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB1A80D8-73DC-481D-86A0-CA80A490B8F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18357850" y="352425"/>
+          <a:ext cx="437749" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+Y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>212725</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>311150</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="379463" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="214" name="文本框 213">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2D51D97-1D3C-478E-A9E3-1CEC7A00ED52}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18415000" y="5597525"/>
+          <a:ext cx="379463" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-Y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="388761" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="215" name="文本框 214">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38AA4F76-A79A-4D76-A4B9-BF3014D17C6B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16716375" y="3670300"/>
+          <a:ext cx="388761" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-X</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>327025</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="438069" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="216" name="文本框 215">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74AFB4DB-EF2A-4FD4-B9A7-08DF86645674}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17043400" y="4914900"/>
+          <a:ext cx="438069" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+Z</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="379784" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="217" name="文本框 216">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3064A3E1-0FE9-411C-BFAE-266E81F784C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21917025" y="381000"/>
+          <a:ext cx="379784" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-Z</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="218" name="直接连接符 217">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4442E18-2417-4BB8-A717-2048008797EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="18583275" y="1762125"/>
+          <a:ext cx="1485900" cy="1390650"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="219" name="直接连接符 218">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7181298-2849-4386-B5C3-ECD026735F48}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18592800" y="3152775"/>
+          <a:ext cx="1838325" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="220" name="直接连接符 219">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EEAE51D-78A6-40C2-8350-297E07131A50}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20050125" y="1752600"/>
+          <a:ext cx="1876425" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="221" name="直接连接符 220">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FB31806-22A5-43F7-83E3-0F5928809415}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21917025" y="1762125"/>
+          <a:ext cx="0" cy="714375"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>58</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="222" name="直接连接符 221">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B720B33-D34D-49EA-90B0-9BFCDC443787}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="20412075" y="2476500"/>
+          <a:ext cx="1495425" cy="1400175"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="223" name="直接连接符 222">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DCEE0A7-7309-46B5-935F-7807CC1B84D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="20069175" y="1771650"/>
+          <a:ext cx="1" cy="704850"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="224" name="直接连接符 223">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F189F56-5D6B-4C32-AAD9-9EBCB10A36A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20078700" y="2457450"/>
+          <a:ext cx="1838325" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="225" name="直接箭头连接符 224">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4ED321F6-3BE8-47C1-9C21-D3BD8AFEEF45}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="18583275" y="1762125"/>
+          <a:ext cx="3333750" cy="2114550"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="226" name="直接箭头连接符 225">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB614739-847A-4175-8EDC-4735C7168654}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18583275" y="3867150"/>
+          <a:ext cx="1847850" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx2"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="227" name="直接箭头连接符 226">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7464D0FD-1A8C-4668-8449-7B278E27F57E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="20431125" y="3162300"/>
+          <a:ext cx="0" cy="714375"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx2"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="228" name="直接箭头连接符 227">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5967AD5F-DB6F-47E5-8914-5F6C86F4F8FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="20431125" y="1762125"/>
+          <a:ext cx="1485900" cy="1390650"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx2"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1384674" cy="283411"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="229" name="文本框 228">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DC83116-5500-4A13-A24B-210F00959696}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19116675" y="3962400"/>
+          <a:ext cx="1384674" cy="283411"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>第一步，右移</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>5</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>单位</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1384674" cy="283411"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="230" name="文本框 229">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2FFF0C5-1BA9-4A7B-967B-270F59727CBA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20421600" y="3286125"/>
+          <a:ext cx="1384674" cy="283411"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>第二步，上移</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>2</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>单位</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1384674" cy="283411"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="231" name="文本框 230">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A07952E-FE5C-4548-AE32-8A22F2EA2D9A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21116925" y="2562225"/>
+          <a:ext cx="1384674" cy="283411"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>第三步，前移</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>4</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>单位</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -28879,7 +33395,7 @@
       <selection activeCell="AS13" sqref="AS13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28896,7 +33412,7 @@
       <selection activeCell="AJ22" sqref="AJ22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28913,7 +33429,7 @@
       <selection activeCell="AR18" sqref="AR18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28929,13 +33445,13 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BM12" sqref="BM12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="4.83203125" style="1"/>
+    <col min="1" max="16384" width="4.875" style="1"/>
   </cols>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -28956,9 +33472,9 @@
       <selection activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="45" spans="15:15" ht="28.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="15:15" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O45" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified   doc/images/painter.xlsx Modified   doc/一起动手实现3D渲染引擎.md Modified   doc/一起动手实现3D渲染引擎.pdf
</commit_message>
<xml_diff>
--- a/doc/images/painter.xlsx
+++ b/doc/images/painter.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\MyGame\Tiny3D\steps\doc\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaronwang\workspace\projects\private\Tiny3D\steps\doc\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12170" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="左右手坐标系" sheetId="1" r:id="rId1"/>
@@ -8194,161 +8194,25 @@
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>358609</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>348629</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>34445</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>317774</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="254" name="平行四边形 253">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8C0D485-A1C4-42C5-92D7-580CAC6E9D49}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="20945152">
-          <a:off x="10388434" y="14093204"/>
-          <a:ext cx="418786" cy="321570"/>
-        </a:xfrm>
-        <a:prstGeom prst="parallelogram">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 18666"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="accent3"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>217344</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>303271</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>55413</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>177650</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="253" name="平行四边形 252">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{468C32B4-6400-4EF0-8F37-0B017660BB88}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="18961482">
-          <a:off x="10247169" y="14047846"/>
-          <a:ext cx="581019" cy="226804"/>
-        </a:xfrm>
-        <a:prstGeom prst="parallelogram">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 99277"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="accent3"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>133326</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>66646</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>292100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>333354</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>165071</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="180" name="图片 179">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B65EA82D-7560-4BCA-8732-BE85497D7F63}"/>
+        <xdr:cNvPr id="232" name="图片 231">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6442E85-0161-4B8E-91FB-7615A4D3B56D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8364,8 +8228,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11458575" y="14287500"/>
-          <a:ext cx="190476" cy="228571"/>
+          <a:off x="3479800" y="15938500"/>
+          <a:ext cx="168254" cy="228571"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8376,23 +8240,67 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>342900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>123804</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>219046</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>47604</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>101571</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="181" name="图片 180">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B95E5B22-79C3-4A0D-8DC6-0D18344E6995}"/>
+        <xdr:cNvPr id="261" name="图片 260">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6442E85-0161-4B8E-91FB-7615A4D3B56D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5403850" y="15875000"/>
+          <a:ext cx="168254" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>254000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>317476</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>130146</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="260" name="图片 259">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C7351C5-0D70-46B4-BB58-A18A7793AAAA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8402,6 +8310,279 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6756400" y="15900400"/>
+          <a:ext cx="190476" cy="231746"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>336550</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="76" name="直接连接符 75"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1473200" y="15119350"/>
+          <a:ext cx="2209800" cy="1574800"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>358609</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>348629</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>34445</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>317774</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="254" name="平行四边形 253">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8C0D485-A1C4-42C5-92D7-580CAC6E9D49}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="20945152">
+          <a:off x="10388434" y="14093204"/>
+          <a:ext cx="418786" cy="321570"/>
+        </a:xfrm>
+        <a:prstGeom prst="parallelogram">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 18666"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>217344</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>303271</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>55413</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>177650</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="253" name="平行四边形 252">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{468C32B4-6400-4EF0-8F37-0B017660BB88}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="18961482">
+          <a:off x="10247169" y="14047846"/>
+          <a:ext cx="581019" cy="226804"/>
+        </a:xfrm>
+        <a:prstGeom prst="parallelogram">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 99277"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>133326</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>66646</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="180" name="图片 179">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B65EA82D-7560-4BCA-8732-BE85497D7F63}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11458575" y="14287500"/>
+          <a:ext cx="190476" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>123804</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>219046</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="181" name="图片 180">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B95E5B22-79C3-4A0D-8DC6-0D18344E6995}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -13871,6 +14052,50 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8296275" y="10229850"/>
+          <a:ext cx="190476" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>190479</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>190471</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="188" name="图片 187">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000BC000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
@@ -13878,8 +14103,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8296275" y="10229850"/>
-          <a:ext cx="190476" cy="228571"/>
+          <a:off x="8934450" y="9477375"/>
+          <a:ext cx="171429" cy="228571"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13890,23 +14115,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>342876</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>314325</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>190479</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>190471</xdr:rowOff>
+      <xdr:rowOff>19021</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="188" name="图片 187">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000BC000000}"/>
+        <xdr:cNvPr id="189" name="图片 188">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000BD000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13922,8 +14147,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8934450" y="9477375"/>
-          <a:ext cx="171429" cy="228571"/>
+          <a:off x="10182225" y="8953500"/>
+          <a:ext cx="190476" cy="228571"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13935,22 +14160,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>342876</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>19021</xdr:rowOff>
+      <xdr:colOff>171429</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>238096</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="189" name="图片 188">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000BD000000}"/>
+        <xdr:cNvPr id="190" name="图片 189">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000BE000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13966,8 +14191,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10182225" y="8953500"/>
-          <a:ext cx="190476" cy="228571"/>
+          <a:off x="10029825" y="9877425"/>
+          <a:ext cx="171429" cy="228571"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13976,25 +14201,228 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="191" name="直接箭头连接符 190">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000BF000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7429500" y="10934700"/>
+          <a:ext cx="1857375" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>342901</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="192" name="直接箭头连接符 191">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000C0000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="7429500" y="10934700"/>
+          <a:ext cx="742950" cy="1038226"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="196" name="直接箭头连接符 195">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000C4000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8172450" y="10925176"/>
+          <a:ext cx="1114426" cy="1057274"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>171429</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>238096</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>114240</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>323821</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="190" name="图片 189">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000BE000000}"/>
+        <xdr:cNvPr id="200" name="图片 199">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000C8000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8181975" y="10668000"/>
+          <a:ext cx="476190" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>38076</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>28546</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="201" name="图片 200">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000C9000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14010,8 +14438,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10029825" y="9877425"/>
-          <a:ext cx="171429" cy="228571"/>
+          <a:off x="8763000" y="11430000"/>
+          <a:ext cx="190476" cy="228571"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14020,228 +14448,25 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="191" name="直接箭头连接符 190">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000BF000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7429500" y="10934700"/>
-          <a:ext cx="1857375" cy="1"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>333354</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>342901</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="192" name="直接箭头连接符 191">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000C0000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="7429500" y="10934700"/>
-          <a:ext cx="742950" cy="1038226"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="196" name="直接箭头连接符 195">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000C4000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="8172450" y="10925176"/>
-          <a:ext cx="1114426" cy="1057274"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>114240</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>323821</xdr:rowOff>
+      <xdr:rowOff>19021</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="200" name="图片 199">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000C8000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8181975" y="10668000"/>
-          <a:ext cx="476190" cy="228571"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>38076</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>28546</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="201" name="图片 200">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000C9000000}"/>
+        <xdr:cNvPr id="202" name="图片 201">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000CA000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14257,50 +14482,6 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8763000" y="11430000"/>
-          <a:ext cx="190476" cy="228571"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>333354</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>19021</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="202" name="图片 201">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000CA000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
           <a:off x="7591425" y="11420475"/>
           <a:ext cx="171429" cy="228571"/>
         </a:xfrm>
@@ -14541,7 +14722,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -14585,7 +14766,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -16628,6 +16809,50 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14230350" y="9626600"/>
+          <a:ext cx="190476" cy="231746"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>222250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>3154</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>98396</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="159" name="图片 158">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00009F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
@@ -16635,8 +16860,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14230350" y="9626600"/>
-          <a:ext cx="190476" cy="231746"/>
+          <a:off x="14566900" y="11245850"/>
+          <a:ext cx="168254" cy="231746"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16645,25 +16870,131 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="149" name="直接箭头连接符 148">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08584F2C-F729-4BE8-84B0-D699ACE852C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2228850" y="13049249"/>
+          <a:ext cx="742950" cy="1038226"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>352424</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="152" name="直接箭头连接符 151">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81044155-2C0D-4985-A6B3-44852DF5911F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2971800" y="11991975"/>
+          <a:ext cx="1123950" cy="2105024"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>222250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>40</xdr:col>
-      <xdr:colOff>3154</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>98396</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>333351</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>28546</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="159" name="图片 158">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00009F000000}"/>
+        <xdr:cNvPr id="154" name="图片 153">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C7351C5-0D70-46B4-BB58-A18A7793AAAA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16679,8 +17010,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14566900" y="11245850"/>
-          <a:ext cx="168254" cy="231746"/>
+          <a:off x="2371725" y="13544550"/>
+          <a:ext cx="190476" cy="228571"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16689,131 +17020,25 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>342900</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="149" name="直接箭头连接符 148">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08584F2C-F729-4BE8-84B0-D699ACE852C8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="2228850" y="13049249"/>
-          <a:ext cx="742950" cy="1038226"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>352424</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="152" name="直接箭头连接符 151">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81044155-2C0D-4985-A6B3-44852DF5911F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="2971800" y="11991975"/>
-          <a:ext cx="1123950" cy="2105024"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>333351</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>28546</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>57129</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>285721</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="154" name="图片 153">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C7351C5-0D70-46B4-BB58-A18A7793AAAA}"/>
+        <xdr:cNvPr id="155" name="图片 154">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6442E85-0161-4B8E-91FB-7615A4D3B56D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16829,7 +17054,500 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2371725" y="13544550"/>
+          <a:off x="3600450" y="13096875"/>
+          <a:ext cx="171429" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>118972</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>332527</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>224455</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>218227</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="弧形 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D02E7D9-C7D4-4918-AC2A-2B4F64C827D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="21349100">
+          <a:off x="2719297" y="13724677"/>
+          <a:ext cx="476958" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 11957827"/>
+            <a:gd name="adj2" fmla="val 20605912"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>123796</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>314296</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="图片 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73C316D9-BBE8-4D07-AF2C-C34A1BA2B9AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2867025" y="13477875"/>
+          <a:ext cx="228571" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="161" name="直接箭头连接符 160">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9C1AD3A-ADEC-4355-8F6D-9D8F32A00CDB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5210175" y="12696825"/>
+          <a:ext cx="2228850" cy="1409700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="162" name="直接箭头连接符 161">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FB93D36-3107-4AFB-9891-9192AC3FB2E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5219700" y="14106524"/>
+          <a:ext cx="2219325" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>352424</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="164" name="直接箭头连接符 163">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80469EE0-F720-445B-A9FB-27220F7BBA0A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7429500" y="12696825"/>
+          <a:ext cx="0" cy="1400174"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="166" name="直接箭头连接符 165">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D52396C-600D-4AD0-9836-5A32CB522384}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5210175" y="14106525"/>
+          <a:ext cx="1114425" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>361921</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>304771</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="173" name="图片 172">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{009F3B76-4EEA-4BA8-9B95-AF0990D9BF45}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5705475" y="13820775"/>
+          <a:ext cx="228571" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>276194</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>304769</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="240" name="图片 239">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAC37058-4952-46EC-BEF1-8F0EDA3527D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7086600" y="14154150"/>
+          <a:ext cx="247619" cy="247619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>285719</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>276194</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="241" name="图片 240">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F43A9DE-20E6-4C38-A9CC-7F9757805AD0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7467600" y="13068300"/>
+          <a:ext cx="247619" cy="247619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>314301</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>266671</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="242" name="图片 241">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{662A392A-4AAD-499D-A078-D098B19119E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6810375" y="12725400"/>
           <a:ext cx="190476" cy="228571"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -16841,23 +17559,646 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>285730</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>276196</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="243" name="图片 242">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D22A354-2985-4CA5-81E2-F1A0F2261D15}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6067425" y="14144625"/>
+          <a:ext cx="161905" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>9528</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="178" name="直接箭头连接符 177">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16D26EE3-D148-4657-B1F7-37DC53676743}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10401300" y="13744575"/>
+          <a:ext cx="742950" cy="714378"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="179" name="直接箭头连接符 178">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A18EAF3-B615-4DF9-AD5C-4C5BAF66065B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10401300" y="14106525"/>
+          <a:ext cx="1866900" cy="352424"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>52297</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>94403</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>157780</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>332528</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="185" name="弧形 184">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2955EB9-8B9F-4B82-9EE6-C0F4F3BD8C07}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="1744720">
+          <a:off x="10453597" y="14191403"/>
+          <a:ext cx="476958" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 14727179"/>
+            <a:gd name="adj2" fmla="val 20605912"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="193" name="直接箭头连接符 192">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F2F59D9-C07C-416F-888C-659BF1065435}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10410825" y="12696826"/>
+          <a:ext cx="1" cy="1762124"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>57129</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>342843</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>285721</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="155" name="图片 154">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6442E85-0161-4B8E-91FB-7615A4D3B56D}"/>
+        <xdr:cNvPr id="255" name="图片 254">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA53D9F2-C3E1-48F1-9311-154DA045C7AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9915525" y="13096875"/>
+          <a:ext cx="457143" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>9528</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="197" name="直接箭头连接符 196">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0BFC200-EE25-4ED2-9F66-CBF1E5EE7FAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="13373100" y="13049250"/>
+          <a:ext cx="752475" cy="1057278"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="198" name="直接箭头连接符 197">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F81720DA-30A6-48FB-975D-447AD6888551}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="13373100" y="14097000"/>
+          <a:ext cx="1876425" cy="9524"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="55" name="直接连接符 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{455AC8A4-C098-42A6-914E-B8CE7E5BD606}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="14116050" y="13039725"/>
+          <a:ext cx="1866900" cy="9526"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>2</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="206" name="直接连接符 205">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D947A25-761F-4033-9BE1-D0EF0949179D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="15240000" y="13039725"/>
+          <a:ext cx="733425" cy="1057277"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="256" name="直接连接符 255">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{315CE25E-ACFC-44FE-ABDB-ED9A6F8A389B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="14125575" y="13039725"/>
+          <a:ext cx="0" cy="1066800"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>66646</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>323821</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="257" name="图片 256">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{695C299F-054B-4FFE-ACB8-1DD573719AA8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13582650" y="13839825"/>
+          <a:ext cx="228571" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>304776</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>247621</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="258" name="图片 257">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB0166E3-CE1D-4649-A2B1-9694748F9724}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16873,8 +18214,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3600450" y="13096875"/>
-          <a:ext cx="171429" cy="228571"/>
+          <a:off x="14230350" y="14116050"/>
+          <a:ext cx="190476" cy="228571"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16883,1141 +18224,25 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>118972</xdr:colOff>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>332527</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>224455</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>218227</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="弧形 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D02E7D9-C7D4-4918-AC2A-2B4F64C827D9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="21349100">
-          <a:off x="2719297" y="13724677"/>
-          <a:ext cx="476958" cy="238125"/>
-        </a:xfrm>
-        <a:prstGeom prst="arc">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 11957827"/>
-            <a:gd name="adj2" fmla="val 20605912"/>
-          </a:avLst>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>304779</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>123796</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>314296</xdr:rowOff>
+      <xdr:rowOff>228571</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="图片 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73C316D9-BBE8-4D07-AF2C-C34A1BA2B9AD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2867025" y="13477875"/>
-          <a:ext cx="228571" cy="228571"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="161" name="直接箭头连接符 160">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9C1AD3A-ADEC-4355-8F6D-9D8F32A00CDB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="5210175" y="12696825"/>
-          <a:ext cx="2228850" cy="1409700"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="162" name="直接箭头连接符 161">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FB93D36-3107-4AFB-9891-9192AC3FB2E4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5219700" y="14106524"/>
-          <a:ext cx="2219325" cy="1"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>352424</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="164" name="直接箭头连接符 163">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80469EE0-F720-445B-A9FB-27220F7BBA0A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="7429500" y="12696825"/>
-          <a:ext cx="0" cy="1400174"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="166" name="直接箭头连接符 165">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D52396C-600D-4AD0-9836-5A32CB522384}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5210175" y="14106525"/>
-          <a:ext cx="1114425" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>361921</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>304771</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="173" name="图片 172">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{009F3B76-4EEA-4BA8-9B95-AF0990D9BF45}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5705475" y="13820775"/>
-          <a:ext cx="228571" cy="228571"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>276194</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>304769</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="240" name="图片 239">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAC37058-4952-46EC-BEF1-8F0EDA3527D6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7086600" y="14154150"/>
-          <a:ext cx="247619" cy="247619"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>285719</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>276194</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="241" name="图片 240">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F43A9DE-20E6-4C38-A9CC-7F9757805AD0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7467600" y="13068300"/>
-          <a:ext cx="247619" cy="247619"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>314301</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>266671</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="242" name="图片 241">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{662A392A-4AAD-499D-A078-D098B19119E3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6810375" y="12725400"/>
-          <a:ext cx="190476" cy="228571"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>285730</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>276196</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="243" name="图片 242">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D22A354-2985-4CA5-81E2-F1A0F2261D15}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6067425" y="14144625"/>
-          <a:ext cx="161905" cy="228571"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>9528</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="178" name="直接箭头连接符 177">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16D26EE3-D148-4657-B1F7-37DC53676743}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="10401300" y="13744575"/>
-          <a:ext cx="742950" cy="714378"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="179" name="直接箭头连接符 178">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A18EAF3-B615-4DF9-AD5C-4C5BAF66065B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="10401300" y="14106525"/>
-          <a:ext cx="1866900" cy="352424"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>52297</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>94403</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>157780</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>332528</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="185" name="弧形 184">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2955EB9-8B9F-4B82-9EE6-C0F4F3BD8C07}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="1744720">
-          <a:off x="10453597" y="14191403"/>
-          <a:ext cx="476958" cy="238125"/>
-        </a:xfrm>
-        <a:prstGeom prst="arc">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 14727179"/>
-            <a:gd name="adj2" fmla="val 20605912"/>
-          </a:avLst>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>9526</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="193" name="直接箭头连接符 192">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F2F59D9-C07C-416F-888C-659BF1065435}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="10410825" y="12696826"/>
-          <a:ext cx="1" cy="1762124"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>342843</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>285721</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="255" name="图片 254">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA53D9F2-C3E1-48F1-9311-154DA045C7AC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9915525" y="13096875"/>
-          <a:ext cx="457143" cy="228571"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>9528</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="197" name="直接箭头连接符 196">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0BFC200-EE25-4ED2-9F66-CBF1E5EE7FAF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="13373100" y="13049250"/>
-          <a:ext cx="752475" cy="1057278"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>41</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="198" name="直接箭头连接符 197">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F81720DA-30A6-48FB-975D-447AD6888551}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="13373100" y="14097000"/>
-          <a:ext cx="1876425" cy="9524"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>43</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="55" name="直接连接符 54">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{455AC8A4-C098-42A6-914E-B8CE7E5BD606}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="14116050" y="13039725"/>
-          <a:ext cx="1866900" cy="9526"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>41</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>43</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>2</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="206" name="直接连接符 205">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D947A25-761F-4033-9BE1-D0EF0949179D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="15240000" y="13039725"/>
-          <a:ext cx="733425" cy="1057277"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="256" name="直接连接符 255">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{315CE25E-ACFC-44FE-ABDB-ED9A6F8A389B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="14125575" y="13039725"/>
-          <a:ext cx="0" cy="1066800"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>66646</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>323821</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="257" name="图片 256">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{695C299F-054B-4FFE-ACB8-1DD573719AA8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13582650" y="13839825"/>
-          <a:ext cx="228571" cy="228571"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>304776</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>247621</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="258" name="图片 257">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB0166E3-CE1D-4649-A2B1-9694748F9724}"/>
+        <xdr:cNvPr id="259" name="图片 258">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{413ECD15-491B-4B3A-966D-A7AEE05D3A3D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18033,8 +18258,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14230350" y="14116050"/>
-          <a:ext cx="190476" cy="228571"/>
+          <a:off x="13506450" y="13392150"/>
+          <a:ext cx="171429" cy="228571"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -18045,23 +18270,173 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>304779</xdr:colOff>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>209526</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>228571</xdr:rowOff>
+      <xdr:rowOff>295246</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="259" name="图片 258">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{413ECD15-491B-4B3A-966D-A7AEE05D3A3D}"/>
+        <xdr:cNvPr id="82" name="图片 81">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C49EF8AF-953E-4800-AB45-1078931EF566}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14135100" y="13458825"/>
+          <a:ext cx="190476" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="187" name="直接箭头连接符 186">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08584F2C-F729-4BE8-84B0-D699ACE852C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1479550" y="15646400"/>
+          <a:ext cx="1466850" cy="1060450"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="194" name="直接箭头连接符 193">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81044155-2C0D-4985-A6B3-44852DF5911F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2946400" y="15646400"/>
+          <a:ext cx="1104900" cy="1066800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>241300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>63476</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>117446</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="199" name="图片 198">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C7351C5-0D70-46B4-BB58-A18A7793AAAA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18077,8 +18452,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13506450" y="13392150"/>
-          <a:ext cx="171429" cy="228571"/>
+          <a:off x="2082800" y="15887700"/>
+          <a:ext cx="190476" cy="231746"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -18087,50 +18462,411 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>209526</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>295246</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="82" name="图片 81">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C49EF8AF-953E-4800-AB45-1078931EF566}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14135100" y="13458825"/>
-          <a:ext cx="190476" cy="228571"/>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>222250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="237" name="右弧形箭头 236"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3200400" y="15474950"/>
+          <a:ext cx="95250" cy="393700"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedLeftArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 1774"/>
+            <a:gd name="adj2" fmla="val 64400"/>
+            <a:gd name="adj3" fmla="val 25000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>158750</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="250" name="直接连接符 249"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="5683250" y="15081250"/>
+          <a:ext cx="1682750" cy="1631950"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="251" name="直接箭头连接符 250">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08584F2C-F729-4BE8-84B0-D699ACE852C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4794250" y="15640050"/>
+          <a:ext cx="1466850" cy="1066800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="252" name="直接箭头连接符 251">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81044155-2C0D-4985-A6B3-44852DF5911F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="6261100" y="15640050"/>
+          <a:ext cx="1098550" cy="1073150"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="262" name="右弧形箭头 261"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5918200" y="15411450"/>
+          <a:ext cx="88900" cy="393700"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedLeftArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 1774"/>
+            <a:gd name="adj2" fmla="val 64400"/>
+            <a:gd name="adj3" fmla="val 25000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="954107" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="264" name="文本框 263"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2266950" y="16713200"/>
+          <a:ext cx="954107" cy="356316"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>顺时针方向</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>158750</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="954107" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="265" name="文本框 264"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5683250" y="16706850"/>
+          <a:ext cx="954107" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>逆时针方向</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -35922,7 +36658,7 @@
       <selection activeCell="AS13" sqref="AS13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35939,7 +36675,7 @@
       <selection activeCell="AJ22" sqref="AJ22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35956,7 +36692,7 @@
       <selection activeCell="AR18" sqref="AR18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35972,13 +36708,13 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AU45" sqref="AU45"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA49" sqref="AA49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="4.875" style="1"/>
+    <col min="1" max="16384" width="4.83203125" style="1"/>
   </cols>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -35999,9 +36735,9 @@
       <selection activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="45" spans="15:15" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="15:15" ht="28.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O45" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified   doc/images/painter.xlsx Modified   doc/一起动手实现3D渲染引擎.md Modified   doc/一起动手实现3D渲染引擎.pdf Add        doc/images/vector-cross-dir.png
</commit_message>
<xml_diff>
--- a/doc/images/painter.xlsx
+++ b/doc/images/painter.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaronwang\workspace\projects\private\Tiny3D\steps\doc\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\MyGame\Tiny3D\steps\doc\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12170" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="左右手坐标系" sheetId="1" r:id="rId1"/>
@@ -8212,7 +8212,7 @@
         <xdr:cNvPr id="232" name="图片 231">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6442E85-0161-4B8E-91FB-7615A4D3B56D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000E8000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8256,7 +8256,7 @@
         <xdr:cNvPr id="261" name="图片 260">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6442E85-0161-4B8E-91FB-7615A4D3B56D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8300,7 +8300,7 @@
         <xdr:cNvPr id="260" name="图片 259">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C7351C5-0D70-46B4-BB58-A18A7793AAAA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8341,7 +8341,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="76" name="直接连接符 75"/>
+        <xdr:cNvPr id="76" name="直接连接符 75">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00004C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -8393,7 +8399,7 @@
         <xdr:cNvPr id="254" name="平行四边形 253">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8C0D485-A1C4-42C5-92D7-580CAC6E9D49}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000FE000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8461,7 +8467,7 @@
         <xdr:cNvPr id="253" name="平行四边形 252">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{468C32B4-6400-4EF0-8F37-0B017660BB88}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000FD000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8529,7 +8535,7 @@
         <xdr:cNvPr id="180" name="图片 179">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B65EA82D-7560-4BCA-8732-BE85497D7F63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000B4000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8573,7 +8579,7 @@
         <xdr:cNvPr id="181" name="图片 180">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B95E5B22-79C3-4A0D-8DC6-0D18344E6995}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000B5000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8617,7 +8623,7 @@
         <xdr:cNvPr id="186" name="图片 185">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CA7323D-2E8D-47BA-89A9-6EC7DF0DB972}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000BA000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8661,7 +8667,7 @@
         <xdr:cNvPr id="171" name="直接箭头连接符 170">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2D09F56-B425-472B-834B-B2875C44EC91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000AB000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16888,7 +16894,7 @@
         <xdr:cNvPr id="149" name="直接箭头连接符 148">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08584F2C-F729-4BE8-84B0-D699ACE852C8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000095000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16941,7 +16947,7 @@
         <xdr:cNvPr id="152" name="直接箭头连接符 151">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81044155-2C0D-4985-A6B3-44852DF5911F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000098000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16994,7 +17000,7 @@
         <xdr:cNvPr id="154" name="图片 153">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C7351C5-0D70-46B4-BB58-A18A7793AAAA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00009A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17038,7 +17044,7 @@
         <xdr:cNvPr id="155" name="图片 154">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6442E85-0161-4B8E-91FB-7615A4D3B56D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00009B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17082,7 +17088,7 @@
         <xdr:cNvPr id="7" name="弧形 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D02E7D9-C7D4-4918-AC2A-2B4F64C827D9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17143,7 +17149,7 @@
         <xdr:cNvPr id="11" name="图片 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73C316D9-BBE8-4D07-AF2C-C34A1BA2B9AD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17187,7 +17193,7 @@
         <xdr:cNvPr id="161" name="直接箭头连接符 160">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9C1AD3A-ADEC-4355-8F6D-9D8F32A00CDB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000A1000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17240,7 +17246,7 @@
         <xdr:cNvPr id="162" name="直接箭头连接符 161">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FB93D36-3107-4AFB-9891-9192AC3FB2E4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000A2000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17293,7 +17299,7 @@
         <xdr:cNvPr id="164" name="直接箭头连接符 163">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80469EE0-F720-445B-A9FB-27220F7BBA0A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000A4000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17346,7 +17352,7 @@
         <xdr:cNvPr id="166" name="直接箭头连接符 165">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D52396C-600D-4AD0-9836-5A32CB522384}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000A6000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17399,7 +17405,7 @@
         <xdr:cNvPr id="173" name="图片 172">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{009F3B76-4EEA-4BA8-9B95-AF0990D9BF45}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000AD000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17443,7 +17449,7 @@
         <xdr:cNvPr id="240" name="图片 239">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAC37058-4952-46EC-BEF1-8F0EDA3527D6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000F0000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17487,7 +17493,7 @@
         <xdr:cNvPr id="241" name="图片 240">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F43A9DE-20E6-4C38-A9CC-7F9757805AD0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000F1000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17531,7 +17537,7 @@
         <xdr:cNvPr id="242" name="图片 241">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{662A392A-4AAD-499D-A078-D098B19119E3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000F2000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17575,7 +17581,7 @@
         <xdr:cNvPr id="243" name="图片 242">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D22A354-2985-4CA5-81E2-F1A0F2261D15}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000F3000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17619,7 +17625,7 @@
         <xdr:cNvPr id="178" name="直接箭头连接符 177">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16D26EE3-D148-4657-B1F7-37DC53676743}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000B2000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17672,7 +17678,7 @@
         <xdr:cNvPr id="179" name="直接箭头连接符 178">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A18EAF3-B615-4DF9-AD5C-4C5BAF66065B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000B3000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17725,7 +17731,7 @@
         <xdr:cNvPr id="185" name="弧形 184">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2955EB9-8B9F-4B82-9EE6-C0F4F3BD8C07}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000B9000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17786,7 +17792,7 @@
         <xdr:cNvPr id="193" name="直接箭头连接符 192">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F2F59D9-C07C-416F-888C-659BF1065435}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000C1000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17839,7 +17845,7 @@
         <xdr:cNvPr id="255" name="图片 254">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA53D9F2-C3E1-48F1-9311-154DA045C7AC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000FF000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17883,7 +17889,7 @@
         <xdr:cNvPr id="197" name="直接箭头连接符 196">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0BFC200-EE25-4ED2-9F66-CBF1E5EE7FAF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000C5000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17936,7 +17942,7 @@
         <xdr:cNvPr id="198" name="直接箭头连接符 197">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F81720DA-30A6-48FB-975D-447AD6888551}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000C6000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17989,7 +17995,7 @@
         <xdr:cNvPr id="55" name="直接连接符 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{455AC8A4-C098-42A6-914E-B8CE7E5BD606}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000037000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18044,7 +18050,7 @@
         <xdr:cNvPr id="206" name="直接连接符 205">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D947A25-761F-4033-9BE1-D0EF0949179D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000CE000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18099,7 +18105,7 @@
         <xdr:cNvPr id="256" name="直接连接符 255">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{315CE25E-ACFC-44FE-ABDB-ED9A6F8A389B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000000010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18154,7 +18160,7 @@
         <xdr:cNvPr id="257" name="图片 256">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{695C299F-054B-4FFE-ACB8-1DD573719AA8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000001010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18198,7 +18204,7 @@
         <xdr:cNvPr id="258" name="图片 257">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB0166E3-CE1D-4649-A2B1-9694748F9724}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18242,7 +18248,7 @@
         <xdr:cNvPr id="259" name="图片 258">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{413ECD15-491B-4B3A-966D-A7AEE05D3A3D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18286,7 +18292,7 @@
         <xdr:cNvPr id="82" name="图片 81">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C49EF8AF-953E-4800-AB45-1078931EF566}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000052000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18330,7 +18336,7 @@
         <xdr:cNvPr id="187" name="直接箭头连接符 186">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08584F2C-F729-4BE8-84B0-D699ACE852C8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000BB000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18383,7 +18389,7 @@
         <xdr:cNvPr id="194" name="直接箭头连接符 193">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81044155-2C0D-4985-A6B3-44852DF5911F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000C2000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18436,7 +18442,7 @@
         <xdr:cNvPr id="199" name="图片 198">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C7351C5-0D70-46B4-BB58-A18A7793AAAA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000C7000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18477,7 +18483,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="237" name="右弧形箭头 236"/>
+        <xdr:cNvPr id="237" name="右弧形箭头 236">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000ED000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -18547,7 +18559,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="250" name="直接连接符 249"/>
+        <xdr:cNvPr id="250" name="直接连接符 249">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000FA000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -18599,7 +18617,7 @@
         <xdr:cNvPr id="251" name="直接箭头连接符 250">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08584F2C-F729-4BE8-84B0-D699ACE852C8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000FB000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18652,7 +18670,7 @@
         <xdr:cNvPr id="252" name="直接箭头连接符 251">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81044155-2C0D-4985-A6B3-44852DF5911F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000FC000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18702,7 +18720,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="262" name="右弧形箭头 261"/>
+        <xdr:cNvPr id="262" name="右弧形箭头 261">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006010000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -18767,7 +18791,13 @@
     <xdr:ext cx="954107" cy="356316"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="264" name="文本框 263"/>
+        <xdr:cNvPr id="264" name="文本框 263">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008010000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -18822,7 +18852,13 @@
     <xdr:ext cx="954107" cy="356316"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="265" name="文本框 264"/>
+        <xdr:cNvPr id="265" name="文本框 264">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009010000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -36658,7 +36694,7 @@
       <selection activeCell="AS13" sqref="AS13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -36675,7 +36711,7 @@
       <selection activeCell="AJ22" sqref="AJ22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -36692,7 +36728,7 @@
       <selection activeCell="AR18" sqref="AR18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -36708,13 +36744,13 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA49" sqref="AA49"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AT53" sqref="AT53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="4.83203125" style="1"/>
+    <col min="1" max="16384" width="4.875" style="1"/>
   </cols>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -36735,9 +36771,9 @@
       <selection activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="45" spans="15:15" ht="28.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="15:15" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O45" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified   doc/images/painter.xlsx Modified   doc/一起动手实现3D渲染引擎.md Modified   source/step04/Samples/TransformationApp/TransformationApp.cpp Add        doc/images/matrix-after-3D-transformation.png Add        doc/images/matrix-before-3D-transformation.png Add        doc/images/matrix-transformation-interpretation.png Add        doc/images/matrix-transformation.png
</commit_message>
<xml_diff>
--- a/doc/images/painter.xlsx
+++ b/doc/images/painter.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaronwang\workspace\projects\private\Tiny3D\steps\doc\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\MyGame\Tiny3D\steps\doc\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12170" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="左右手坐标系" sheetId="1" r:id="rId1"/>
@@ -18927,7 +18927,7 @@
         <xdr:cNvPr id="49" name="直接箭头连接符 48">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000AC000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000031000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18980,7 +18980,7 @@
         <xdr:cNvPr id="52" name="直接箭头连接符 51">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000AC000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000034000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19033,7 +19033,7 @@
         <xdr:cNvPr id="55" name="直接箭头连接符 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000AC000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000037000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19086,7 +19086,7 @@
         <xdr:cNvPr id="36" name="直接箭头连接符 35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000AC000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000024000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19139,7 +19139,7 @@
         <xdr:cNvPr id="32" name="直接箭头连接符 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000AC000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19192,7 +19192,7 @@
         <xdr:cNvPr id="2" name="直接箭头连接符 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000089000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19246,7 +19246,7 @@
         <xdr:cNvPr id="3" name="直接箭头连接符 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00008A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19295,7 +19295,7 @@
         <xdr:cNvPr id="4" name="文本框 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00008C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19366,7 +19366,7 @@
         <xdr:cNvPr id="5" name="文本框 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00008D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19437,7 +19437,7 @@
         <xdr:cNvPr id="6" name="文本框 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00008E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19508,7 +19508,7 @@
         <xdr:cNvPr id="7" name="文本框 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000090000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19584,7 +19584,7 @@
         <xdr:cNvPr id="8" name="直接箭头连接符 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000AC000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19637,7 +19637,7 @@
         <xdr:cNvPr id="9" name="直接箭头连接符 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000B0000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19690,7 +19690,7 @@
         <xdr:cNvPr id="15" name="直接箭头连接符 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000AC000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19743,7 +19743,7 @@
         <xdr:cNvPr id="19" name="直接箭头连接符 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000AC000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19796,7 +19796,7 @@
         <xdr:cNvPr id="22" name="直接箭头连接符 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000089000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19850,7 +19850,7 @@
         <xdr:cNvPr id="23" name="直接箭头连接符 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00008A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19899,7 +19899,7 @@
         <xdr:cNvPr id="24" name="文本框 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00008C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19970,7 +19970,7 @@
         <xdr:cNvPr id="25" name="文本框 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00008D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20041,7 +20041,7 @@
         <xdr:cNvPr id="26" name="文本框 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00008E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20112,7 +20112,7 @@
         <xdr:cNvPr id="27" name="文本框 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000090000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20188,7 +20188,7 @@
         <xdr:cNvPr id="28" name="直接箭头连接符 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000AC000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20241,7 +20241,7 @@
         <xdr:cNvPr id="29" name="直接箭头连接符 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000B0000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20294,7 +20294,7 @@
         <xdr:cNvPr id="30" name="直接箭头连接符 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000AC000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20334,11 +20334,11 @@
       <xdr:col>20</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>336550</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>342900</xdr:rowOff>
     </xdr:to>
@@ -20347,16 +20347,16 @@
         <xdr:cNvPr id="31" name="直接箭头连接符 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000AC000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="7727950" y="3536950"/>
-          <a:ext cx="730250" cy="6350"/>
+        <a:xfrm>
+          <a:off x="7791450" y="3514725"/>
+          <a:ext cx="762000" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -20400,7 +20400,7 @@
         <xdr:cNvPr id="44" name="直接箭头连接符 43">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000AC000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20450,7 +20450,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="59" name="直接连接符 58"/>
+        <xdr:cNvPr id="59" name="直接连接符 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -20494,7 +20500,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="60" name="直接连接符 59"/>
+        <xdr:cNvPr id="60" name="直接连接符 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -20538,7 +20550,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="63" name="直接连接符 62"/>
+        <xdr:cNvPr id="63" name="直接连接符 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -20582,7 +20600,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="65" name="直接连接符 64"/>
+        <xdr:cNvPr id="65" name="直接连接符 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000041000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -20626,7 +20650,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="73" name="直接连接符 72"/>
+        <xdr:cNvPr id="73" name="直接连接符 72">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000049000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -20670,7 +20700,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="74" name="直接连接符 73"/>
+        <xdr:cNvPr id="74" name="直接连接符 73">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00004A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -20714,7 +20750,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="78" name="直接连接符 77"/>
+        <xdr:cNvPr id="78" name="直接连接符 77">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00004E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -20758,7 +20800,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="84" name="直接连接符 83"/>
+        <xdr:cNvPr id="84" name="直接连接符 83">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000054000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -20787,30 +20835,25 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>101</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>114271</xdr:colOff>
-      <xdr:row>101</xdr:row>
-      <xdr:rowOff>342870</xdr:rowOff>
+      <xdr:colOff>87631</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="121" name="图片 120">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000079000000}"/>
+        <xdr:cNvPr id="10" name="图片 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22837E9D-408B-471B-ACB6-ABB135A00E82}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20826,8 +20869,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4343400" y="35699700"/>
-          <a:ext cx="228571" cy="238095"/>
+          <a:off x="3752850" y="2514600"/>
+          <a:ext cx="792481" cy="247650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -20838,23 +20881,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>98</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>257145</xdr:colOff>
-      <xdr:row>99</xdr:row>
-      <xdr:rowOff>19020</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>361951</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>70486</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="319" name="图片 318">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003F010000}"/>
+        <xdr:cNvPr id="11" name="图片 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59A76FAC-AE69-4860-AB8E-93E8D72F06F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20870,8 +20913,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5219700" y="34671000"/>
-          <a:ext cx="238095" cy="238095"/>
+          <a:off x="1476376" y="1800225"/>
+          <a:ext cx="822960" cy="228600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -20882,23 +20925,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>361905</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>180952</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>88195</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="264" name="图片 263">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000008010000}"/>
+        <xdr:cNvPr id="12" name="图片 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65F9B342-E6C7-4B84-92BB-0BEADA4AA33E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20914,6 +20957,479 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
+          <a:off x="3105150" y="933450"/>
+          <a:ext cx="697795" cy="438150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>110773</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="直接连接符 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20CF1881-9031-4E29-8057-EA172A6D1845}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="12" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2428875" y="1371600"/>
+          <a:ext cx="1025173" cy="485776"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>171451</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>285751</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="直接连接符 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0F77268-674F-4434-982F-A639A7048A34}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3295650" y="1371600"/>
+          <a:ext cx="590551" cy="1028701"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>78105</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="图片 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25A5D555-4D17-4209-9D77-4BEF75B7DC8C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9315449" y="2543175"/>
+          <a:ext cx="792481" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>156210</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="图片 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E779C33-D8B8-45AD-94D1-10D73B7335CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6391275" y="1781175"/>
+          <a:ext cx="822960" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>107244</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="50" name="图片 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CD98B11-6DDF-468C-BF34-3EDBAB5DB883}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8324849" y="676275"/>
+          <a:ext cx="697795" cy="438150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>129822</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="直接连接符 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F2E63D0-8220-4EC4-ABC5-A67A9C0F5656}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="50" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7315200" y="1114425"/>
+          <a:ext cx="1358547" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="53" name="直接连接符 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2148B089-FF19-4EAC-8138-120F85DF14FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8515350" y="1114426"/>
+          <a:ext cx="1152525" cy="1400174"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>114271</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>342870</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="121" name="图片 120">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000079000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4343400" y="35699700"/>
+          <a:ext cx="228571" cy="238095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>257145</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>19020</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="319" name="图片 318">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00003F010000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5219700" y="34671000"/>
+          <a:ext cx="238095" cy="238095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>361905</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>180952</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="264" name="图片 263">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008010000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
           <a:off x="10772775" y="27136725"/>
           <a:ext cx="361905" cy="180952"/>
         </a:xfrm>
@@ -20942,7 +21458,7 @@
         <xdr:cNvPr id="263" name="图片 262">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000007010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20986,7 +21502,7 @@
         <xdr:cNvPr id="261" name="图片 260">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21030,7 +21546,7 @@
         <xdr:cNvPr id="63" name="图片 62">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00003F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21074,7 +21590,7 @@
         <xdr:cNvPr id="50" name="图片 49">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000032000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000032000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21118,7 +21634,7 @@
         <xdr:cNvPr id="255" name="图片 254">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000FF000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000FF000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21162,7 +21678,7 @@
         <xdr:cNvPr id="246" name="图片 245">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000F6000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000F6000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21206,7 +21722,7 @@
         <xdr:cNvPr id="245" name="图片 244">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000F5000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000F5000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21250,7 +21766,7 @@
         <xdr:cNvPr id="35" name="椭圆 34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000023000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21311,7 +21827,7 @@
         <xdr:cNvPr id="153" name="图片 152">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000099000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000099000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21355,7 +21871,7 @@
         <xdr:cNvPr id="128" name="直接连接符 127">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000080000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000080000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21410,7 +21926,7 @@
         <xdr:cNvPr id="3" name="直接箭头连接符 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21467,7 +21983,7 @@
         <xdr:cNvPr id="5" name="直接箭头连接符 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21524,7 +22040,7 @@
         <xdr:cNvPr id="6" name="椭圆 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21585,7 +22101,7 @@
         <xdr:cNvPr id="7" name="文本框 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21646,7 +22162,7 @@
         <xdr:cNvPr id="8" name="文本框 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21711,7 +22227,7 @@
         <xdr:cNvPr id="9" name="文本框 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21776,7 +22292,7 @@
         <xdr:cNvPr id="10" name="文本框 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21841,7 +22357,7 @@
         <xdr:cNvPr id="11" name="文本框 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21911,7 +22427,7 @@
         <xdr:cNvPr id="13" name="直接连接符 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21964,7 +22480,7 @@
         <xdr:cNvPr id="15" name="直接连接符 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22017,7 +22533,7 @@
         <xdr:cNvPr id="17" name="直接连接符 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22069,7 +22585,7 @@
         <xdr:cNvPr id="19" name="直接连接符 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22121,7 +22637,7 @@
         <xdr:cNvPr id="22" name="直接箭头连接符 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22174,7 +22690,7 @@
         <xdr:cNvPr id="26" name="图片 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22218,7 +22734,7 @@
         <xdr:cNvPr id="27" name="图片 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00001B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22262,7 +22778,7 @@
         <xdr:cNvPr id="28" name="直接箭头连接符 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22315,7 +22831,7 @@
         <xdr:cNvPr id="29" name="图片 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00001D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22359,7 +22875,7 @@
         <xdr:cNvPr id="30" name="图片 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00001E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22398,7 +22914,7 @@
         <xdr:cNvPr id="31" name="文本框 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00001F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22463,7 +22979,7 @@
         <xdr:cNvPr id="32" name="文本框 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000020000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22527,7 +23043,7 @@
         <xdr:cNvPr id="34" name="直接箭头连接符 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000022000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000022000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22584,7 +23100,7 @@
         <xdr:cNvPr id="36" name="直接箭头连接符 35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000024000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000024000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22644,7 +23160,7 @@
         <xdr:cNvPr id="38" name="直接连接符 37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000026000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000026000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22689,7 +23205,7 @@
         <xdr:cNvPr id="39" name="文本框 38">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000027000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000027000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22760,7 +23276,7 @@
         <xdr:cNvPr id="40" name="文本框 39">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000028000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000028000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22831,7 +23347,7 @@
         <xdr:cNvPr id="45" name="文本框 44">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00002D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22902,7 +23418,7 @@
         <xdr:cNvPr id="46" name="文本框 45">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00002E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22973,7 +23489,7 @@
         <xdr:cNvPr id="47" name="文本框 46">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00002F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23049,7 +23565,7 @@
         <xdr:cNvPr id="49" name="直接连接符 48">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000031000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000031000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23106,7 +23622,7 @@
         <xdr:cNvPr id="52" name="直接连接符 51">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000034000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000034000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23158,7 +23674,7 @@
         <xdr:cNvPr id="53" name="文本框 52">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000035000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000035000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23233,7 +23749,7 @@
         <xdr:cNvPr id="54" name="文本框 53">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000036000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000036000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23313,7 +23829,7 @@
         <xdr:cNvPr id="56" name="直接箭头连接符 55">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000038000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000038000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23370,7 +23886,7 @@
         <xdr:cNvPr id="57" name="直接箭头连接符 56">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000039000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000039000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23430,7 +23946,7 @@
         <xdr:cNvPr id="58" name="直接连接符 57">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00003A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23475,7 +23991,7 @@
         <xdr:cNvPr id="59" name="文本框 58">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00003B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23546,7 +24062,7 @@
         <xdr:cNvPr id="60" name="文本框 59">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00003C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23617,7 +24133,7 @@
         <xdr:cNvPr id="61" name="文本框 60">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00003D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23688,7 +24204,7 @@
         <xdr:cNvPr id="62" name="文本框 61">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00003E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23764,7 +24280,7 @@
         <xdr:cNvPr id="67" name="直接连接符 66">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000043000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000043000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23814,7 +24330,7 @@
         <xdr:cNvPr id="69" name="直接箭头连接符 68">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000045000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000045000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23867,7 +24383,7 @@
         <xdr:cNvPr id="71" name="图片 70">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000047000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000047000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23906,7 +24422,7 @@
         <xdr:cNvPr id="72" name="文本框 71">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000048000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000048000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23976,7 +24492,7 @@
         <xdr:cNvPr id="73" name="图片 72">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000049000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000049000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24020,7 +24536,7 @@
         <xdr:cNvPr id="74" name="直接箭头连接符 73">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00004A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00004A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24077,7 +24593,7 @@
         <xdr:cNvPr id="75" name="直接箭头连接符 74">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00004B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00004B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24137,7 +24653,7 @@
         <xdr:cNvPr id="76" name="直接连接符 75">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00004C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00004C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24182,7 +24698,7 @@
         <xdr:cNvPr id="77" name="文本框 76">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00004D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00004D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24253,7 +24769,7 @@
         <xdr:cNvPr id="78" name="文本框 77">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00004E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00004E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24324,7 +24840,7 @@
         <xdr:cNvPr id="79" name="文本框 78">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00004F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00004F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24395,7 +24911,7 @@
         <xdr:cNvPr id="80" name="文本框 79">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000050000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000050000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24471,7 +24987,7 @@
         <xdr:cNvPr id="81" name="直接箭头连接符 80">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000051000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000051000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24524,7 +25040,7 @@
         <xdr:cNvPr id="82" name="图片 81">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000052000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000052000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24568,7 +25084,7 @@
         <xdr:cNvPr id="83" name="图片 82">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000053000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000053000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24612,7 +25128,7 @@
         <xdr:cNvPr id="84" name="椭圆 83">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000054000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000054000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24672,7 +25188,7 @@
         <xdr:cNvPr id="85" name="图片 84">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000055000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000055000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24716,7 +25232,7 @@
         <xdr:cNvPr id="87" name="直接连接符 86">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000057000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000057000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24771,7 +25287,7 @@
         <xdr:cNvPr id="91" name="直接箭头连接符 90">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00005B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00005B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24825,7 +25341,7 @@
         <xdr:cNvPr id="93" name="椭圆 92">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00005D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00005D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24885,7 +25401,7 @@
         <xdr:cNvPr id="94" name="椭圆 93">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00005E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00005E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24940,7 +25456,7 @@
         <xdr:cNvPr id="95" name="文本框 94">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00005F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00005F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25005,7 +25521,7 @@
         <xdr:cNvPr id="96" name="文本框 95">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000060000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000060000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25070,7 +25586,7 @@
         <xdr:cNvPr id="97" name="文本框 96">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000061000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000061000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25140,7 +25656,7 @@
         <xdr:cNvPr id="70" name="直接箭头连接符 69">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000046000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000046000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25197,7 +25713,7 @@
         <xdr:cNvPr id="86" name="直接箭头连接符 85">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000056000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000056000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25254,7 +25770,7 @@
         <xdr:cNvPr id="88" name="椭圆 87">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000058000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000058000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25320,7 +25836,7 @@
         <xdr:cNvPr id="2" name="椭圆 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25386,7 +25902,7 @@
         <xdr:cNvPr id="12" name="直接箭头连接符 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25438,7 +25954,7 @@
         <xdr:cNvPr id="98" name="文本框 97">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000062000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000062000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25509,7 +26025,7 @@
         <xdr:cNvPr id="99" name="文本框 98">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000063000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000063000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25580,7 +26096,7 @@
         <xdr:cNvPr id="100" name="文本框 99">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000064000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000064000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25651,7 +26167,7 @@
         <xdr:cNvPr id="101" name="文本框 100">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000065000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000065000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25722,7 +26238,7 @@
         <xdr:cNvPr id="102" name="文本框 101">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000066000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000066000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25793,7 +26309,7 @@
         <xdr:cNvPr id="103" name="文本框 102">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000067000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000067000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25864,7 +26380,7 @@
         <xdr:cNvPr id="18" name="文本框 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25934,7 +26450,7 @@
         <xdr:cNvPr id="21" name="直接连接符 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000015000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25981,7 +26497,7 @@
         <xdr:cNvPr id="23" name="文本框 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000017000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26051,7 +26567,7 @@
         <xdr:cNvPr id="14" name="平行四边形 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26121,7 +26637,7 @@
         <xdr:cNvPr id="20" name="直接箭头连接符 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26169,7 +26685,7 @@
         <xdr:cNvPr id="24" name="文本框 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26240,7 +26756,7 @@
         <xdr:cNvPr id="25" name="文本框 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000019000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26332,7 +26848,7 @@
         <xdr:cNvPr id="33" name="文本框 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000021000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000021000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26420,7 +26936,7 @@
         <xdr:cNvPr id="37" name="曲线连接符 36">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000025000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000025000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26476,7 +26992,7 @@
         <xdr:cNvPr id="90" name="平行四边形 89">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00005A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00005A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26546,7 +27062,7 @@
         <xdr:cNvPr id="92" name="直接箭头连接符 91">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00005C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00005C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26594,7 +27110,7 @@
         <xdr:cNvPr id="104" name="文本框 103">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000068000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000068000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26665,7 +27181,7 @@
         <xdr:cNvPr id="105" name="文本框 104">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000069000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000069000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26762,7 +27278,7 @@
         <xdr:cNvPr id="106" name="椭圆 105">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00006A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00006A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26822,7 +27338,7 @@
         <xdr:cNvPr id="107" name="椭圆 106">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00006B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00006B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26882,7 +27398,7 @@
         <xdr:cNvPr id="108" name="椭圆 107">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00006C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00006C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26942,7 +27458,7 @@
         <xdr:cNvPr id="44" name="直接连接符 43">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00002C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26995,7 +27511,7 @@
         <xdr:cNvPr id="51" name="直接连接符 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000033000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000033000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27048,7 +27564,7 @@
         <xdr:cNvPr id="64" name="图片 63">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000040000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000040000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27092,7 +27608,7 @@
         <xdr:cNvPr id="65" name="图片 64">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000041000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000041000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27136,7 +27652,7 @@
         <xdr:cNvPr id="66" name="图片 65">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000042000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000042000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27180,7 +27696,7 @@
         <xdr:cNvPr id="89" name="图片 88">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000059000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000059000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27224,7 +27740,7 @@
         <xdr:cNvPr id="109" name="图片 108">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00006D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00006D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27268,7 +27784,7 @@
         <xdr:cNvPr id="113" name="平行四边形 112">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000071000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000071000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27338,7 +27854,7 @@
         <xdr:cNvPr id="114" name="直接箭头连接符 113">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000072000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000072000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27386,7 +27902,7 @@
         <xdr:cNvPr id="115" name="文本框 114">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000073000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000073000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27483,7 +27999,7 @@
         <xdr:cNvPr id="117" name="椭圆 116">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000075000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000075000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27543,7 +28059,7 @@
         <xdr:cNvPr id="118" name="椭圆 117">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000076000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000076000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27603,7 +28119,7 @@
         <xdr:cNvPr id="120" name="直接连接符 119">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000078000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000078000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27653,7 +28169,7 @@
         <xdr:cNvPr id="122" name="图片 121">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00007A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00007A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27697,7 +28213,7 @@
         <xdr:cNvPr id="123" name="图片 122">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00007B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00007B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27741,7 +28257,7 @@
         <xdr:cNvPr id="124" name="图片 123">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00007C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00007C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27785,7 +28301,7 @@
         <xdr:cNvPr id="125" name="图片 124">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00007D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00007D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27829,7 +28345,7 @@
         <xdr:cNvPr id="4" name="等腰三角形 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27892,7 +28408,7 @@
         <xdr:cNvPr id="16" name="图片 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000010000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27936,7 +28452,7 @@
         <xdr:cNvPr id="41" name="图片 40">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000029000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000029000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27980,7 +28496,7 @@
         <xdr:cNvPr id="42" name="图片 41">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00002A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28024,7 +28540,7 @@
         <xdr:cNvPr id="43" name="弧形 42">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00002B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28085,7 +28601,7 @@
         <xdr:cNvPr id="116" name="弧形 115">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000074000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000074000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28146,7 +28662,7 @@
         <xdr:cNvPr id="119" name="弧形 118">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000077000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000077000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28207,7 +28723,7 @@
         <xdr:cNvPr id="129" name="图片 128">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000081000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000081000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28251,7 +28767,7 @@
         <xdr:cNvPr id="130" name="图片 129">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000082000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000082000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28295,7 +28811,7 @@
         <xdr:cNvPr id="131" name="图片 130">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000083000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000083000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28339,7 +28855,7 @@
         <xdr:cNvPr id="132" name="图片 131">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000084000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000084000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28383,7 +28899,7 @@
         <xdr:cNvPr id="133" name="图片 132">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000085000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000085000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28427,7 +28943,7 @@
         <xdr:cNvPr id="134" name="图片 133">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000086000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000086000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28471,7 +28987,7 @@
         <xdr:cNvPr id="136" name="直接箭头连接符 135">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000088000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000088000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28524,7 +29040,7 @@
         <xdr:cNvPr id="139" name="直接箭头连接符 138">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00008B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00008B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28577,7 +29093,7 @@
         <xdr:cNvPr id="143" name="直接箭头连接符 142">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00008F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00008F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28630,7 +29146,7 @@
         <xdr:cNvPr id="147" name="等腰三角形 146">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000093000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000093000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28690,7 +29206,7 @@
         <xdr:cNvPr id="148" name="等腰三角形 147">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000094000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000094000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28753,7 +29269,7 @@
         <xdr:cNvPr id="150" name="直接箭头连接符 149">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000096000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000096000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28807,7 +29323,7 @@
         <xdr:cNvPr id="152" name="直接箭头连接符 151">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000098000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000098000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28856,7 +29372,7 @@
         <xdr:cNvPr id="154" name="文本框 153">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00009A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00009A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28927,7 +29443,7 @@
         <xdr:cNvPr id="155" name="文本框 154">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00009B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00009B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29003,7 +29519,7 @@
         <xdr:cNvPr id="161" name="直接箭头连接符 160">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000A1000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000A1000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29060,7 +29576,7 @@
         <xdr:cNvPr id="167" name="直角三角形 166">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000A7000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000A7000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29134,7 +29650,7 @@
         <xdr:cNvPr id="163" name="直接箭头连接符 162">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000A3000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000A3000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29189,7 +29705,7 @@
         <xdr:cNvPr id="166" name="矩形 165">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000A6000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000A6000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29263,7 +29779,7 @@
         <xdr:cNvPr id="159" name="直接箭头连接符 158">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00009F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00009F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29320,7 +29836,7 @@
         <xdr:cNvPr id="168" name="等腰三角形 167">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000A8000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000A8000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29383,7 +29899,7 @@
         <xdr:cNvPr id="169" name="图片 168">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000A9000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000A9000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29427,7 +29943,7 @@
         <xdr:cNvPr id="170" name="图片 169">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000AA000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000AA000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29471,7 +29987,7 @@
         <xdr:cNvPr id="171" name="图片 170">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000AB000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000AB000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29515,7 +30031,7 @@
         <xdr:cNvPr id="172" name="椭圆 171">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000AC000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000AC000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29570,7 +30086,7 @@
         <xdr:cNvPr id="173" name="文本框 172">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000AD000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000AD000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29635,7 +30151,7 @@
         <xdr:cNvPr id="174" name="文本框 173">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000AE000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000AE000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29700,7 +30216,7 @@
         <xdr:cNvPr id="175" name="文本框 174">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000AF000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000AF000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29765,7 +30281,7 @@
         <xdr:cNvPr id="176" name="文本框 175">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000B0000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000B0000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29830,7 +30346,7 @@
         <xdr:cNvPr id="177" name="文本框 176">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000B1000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000B1000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29907,7 +30423,7 @@
         <xdr:cNvPr id="178" name="椭圆 177">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000B2000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000B2000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29967,7 +30483,7 @@
         <xdr:cNvPr id="179" name="椭圆 178">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000B3000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000B3000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30022,7 +30538,7 @@
         <xdr:cNvPr id="180" name="文本框 179">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000B4000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000B4000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30092,7 +30608,7 @@
         <xdr:cNvPr id="181" name="椭圆 180">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000B5000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000B5000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30147,7 +30663,7 @@
         <xdr:cNvPr id="182" name="文本框 181">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000B6000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000B6000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30224,7 +30740,7 @@
         <xdr:cNvPr id="184" name="图片 183">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000B8000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000B8000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30268,7 +30784,7 @@
         <xdr:cNvPr id="185" name="图片 184">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000B9000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000B9000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30312,7 +30828,7 @@
         <xdr:cNvPr id="186" name="图片 185">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000BA000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000BA000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30356,7 +30872,7 @@
         <xdr:cNvPr id="160" name="图片 159">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000A0000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000A0000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30400,7 +30916,7 @@
         <xdr:cNvPr id="162" name="图片 161">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000A2000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000A2000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30444,7 +30960,7 @@
         <xdr:cNvPr id="164" name="图片 163">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000A4000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000A4000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30488,7 +31004,7 @@
         <xdr:cNvPr id="68" name="直接连接符 67">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000044000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000044000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30543,7 +31059,7 @@
         <xdr:cNvPr id="126" name="直接连接符 125">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00007E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00007E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30598,7 +31114,7 @@
         <xdr:cNvPr id="183" name="直接连接符 182">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000B7000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000B7000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30653,7 +31169,7 @@
         <xdr:cNvPr id="187" name="直接连接符 186">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000BB000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000BB000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30708,7 +31224,7 @@
         <xdr:cNvPr id="158" name="等腰三角形 157">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00009E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00009E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30771,7 +31287,7 @@
         <xdr:cNvPr id="188" name="直接连接符 187">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000BC000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000BC000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30826,7 +31342,7 @@
         <xdr:cNvPr id="189" name="直接连接符 188">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000BD000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000BD000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30881,7 +31397,7 @@
         <xdr:cNvPr id="190" name="直接连接符 189">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000BE000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000BE000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30936,7 +31452,7 @@
         <xdr:cNvPr id="191" name="直接连接符 190">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000BF000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000BF000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30991,7 +31507,7 @@
         <xdr:cNvPr id="192" name="直接连接符 191">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000C0000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000C0000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31046,7 +31562,7 @@
         <xdr:cNvPr id="193" name="直接连接符 192">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000C1000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000C1000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31101,7 +31617,7 @@
         <xdr:cNvPr id="194" name="直接连接符 193">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000C2000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000C2000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31156,7 +31672,7 @@
         <xdr:cNvPr id="195" name="直接连接符 194">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000C3000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000C3000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31211,7 +31727,7 @@
         <xdr:cNvPr id="196" name="直接连接符 195">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000C4000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000C4000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31261,7 +31777,7 @@
         <xdr:cNvPr id="197" name="文本框 196">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000C5000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000C5000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31326,7 +31842,7 @@
         <xdr:cNvPr id="198" name="文本框 197">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000C6000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000C6000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31391,7 +31907,7 @@
         <xdr:cNvPr id="199" name="文本框 198">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000C7000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000C7000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31461,7 +31977,7 @@
         <xdr:cNvPr id="200" name="图片 199">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000C8000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000C8000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31505,7 +32021,7 @@
         <xdr:cNvPr id="201" name="图片 200">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000C9000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000C9000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31549,7 +32065,7 @@
         <xdr:cNvPr id="202" name="图片 201">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000CA000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000CA000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31588,7 +32104,7 @@
         <xdr:cNvPr id="203" name="文本框 202">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000CB000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000CB000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31653,7 +32169,7 @@
         <xdr:cNvPr id="204" name="文本框 203">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000CC000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000CC000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31718,7 +32234,7 @@
         <xdr:cNvPr id="205" name="文本框 204">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000CD000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000CD000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31783,7 +32299,7 @@
         <xdr:cNvPr id="206" name="文本框 205">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000CE000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000CE000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31848,7 +32364,7 @@
         <xdr:cNvPr id="207" name="文本框 206">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000CF000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000CF000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31913,7 +32429,7 @@
         <xdr:cNvPr id="208" name="文本框 207">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000D0000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000D0000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31983,7 +32499,7 @@
         <xdr:cNvPr id="209" name="等腰三角形 208">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000D1000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000D1000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32046,7 +32562,7 @@
         <xdr:cNvPr id="210" name="图片 209">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000D2000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000D2000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32090,7 +32606,7 @@
         <xdr:cNvPr id="211" name="图片 210">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000D3000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000D3000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32134,7 +32650,7 @@
         <xdr:cNvPr id="212" name="图片 211">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000D4000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000D4000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32178,7 +32694,7 @@
         <xdr:cNvPr id="48" name="直接连接符 47">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000030000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000030000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32230,7 +32746,7 @@
         <xdr:cNvPr id="55" name="直接连接符 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000037000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000037000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32282,7 +32798,7 @@
         <xdr:cNvPr id="110" name="直接连接符 109">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00006E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00006E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32334,7 +32850,7 @@
         <xdr:cNvPr id="216" name="椭圆 215">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000D8000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000D8000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32394,7 +32910,7 @@
         <xdr:cNvPr id="140" name="图片 139">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00008C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00008C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32438,7 +32954,7 @@
         <xdr:cNvPr id="141" name="图片 140">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00008D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00008D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32482,7 +32998,7 @@
         <xdr:cNvPr id="144" name="图片 143">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000090000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000090000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32526,7 +33042,7 @@
         <xdr:cNvPr id="145" name="图片 144">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000091000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000091000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32570,7 +33086,7 @@
         <xdr:cNvPr id="217" name="图片 216">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000D9000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000D9000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32614,7 +33130,7 @@
         <xdr:cNvPr id="218" name="图片 217">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000DA000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000DA000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32658,7 +33174,7 @@
         <xdr:cNvPr id="219" name="图片 218">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000DB000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000DB000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32702,7 +33218,7 @@
         <xdr:cNvPr id="220" name="等腰三角形 219">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000DC000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000DC000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32765,7 +33281,7 @@
         <xdr:cNvPr id="221" name="图片 220">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000DD000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000DD000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32809,7 +33325,7 @@
         <xdr:cNvPr id="222" name="图片 221">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000DE000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000DE000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32853,7 +33369,7 @@
         <xdr:cNvPr id="223" name="图片 222">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000DF000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000DF000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32897,7 +33413,7 @@
         <xdr:cNvPr id="224" name="图片 223">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000E0000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000E0000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32941,7 +33457,7 @@
         <xdr:cNvPr id="225" name="图片 224">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000E1000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000E1000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32985,7 +33501,7 @@
         <xdr:cNvPr id="226" name="图片 225">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000E2000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000E2000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33029,7 +33545,7 @@
         <xdr:cNvPr id="227" name="图片 226">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000E3000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000E3000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33073,7 +33589,7 @@
         <xdr:cNvPr id="228" name="图片 227">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000E4000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000E4000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33117,7 +33633,7 @@
         <xdr:cNvPr id="229" name="图片 228">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000E5000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000E5000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33161,7 +33677,7 @@
         <xdr:cNvPr id="230" name="图片 229">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000E6000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000E6000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33205,7 +33721,7 @@
         <xdr:cNvPr id="231" name="直接连接符 230">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000E7000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000E7000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33255,7 +33771,7 @@
         <xdr:cNvPr id="232" name="直接连接符 231">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000E8000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000E8000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33305,7 +33821,7 @@
         <xdr:cNvPr id="233" name="直接连接符 232">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000E9000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000E9000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33355,7 +33871,7 @@
         <xdr:cNvPr id="214" name="等腰三角形 213">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000D6000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000D6000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33418,7 +33934,7 @@
         <xdr:cNvPr id="215" name="图片 214">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000D7000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000D7000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33462,7 +33978,7 @@
         <xdr:cNvPr id="234" name="图片 233">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000EA000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000EA000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33506,7 +34022,7 @@
         <xdr:cNvPr id="235" name="图片 234">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000EB000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000EB000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33550,7 +34066,7 @@
         <xdr:cNvPr id="236" name="直接连接符 235">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000EC000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000EC000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33600,7 +34116,7 @@
         <xdr:cNvPr id="237" name="直接连接符 236">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000ED000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000ED000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33653,7 +34169,7 @@
         <xdr:cNvPr id="238" name="直接连接符 237">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000EE000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000EE000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33705,7 +34221,7 @@
         <xdr:cNvPr id="239" name="椭圆 238">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000EF000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000EF000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33765,7 +34281,7 @@
         <xdr:cNvPr id="240" name="等腰三角形 239">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000F0000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000F0000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33828,7 +34344,7 @@
         <xdr:cNvPr id="241" name="图片 240">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000F1000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000F1000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33872,7 +34388,7 @@
         <xdr:cNvPr id="242" name="图片 241">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000F2000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000F2000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33916,7 +34432,7 @@
         <xdr:cNvPr id="243" name="图片 242">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000F3000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000F3000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33960,7 +34476,7 @@
         <xdr:cNvPr id="244" name="椭圆 243">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000F4000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000F4000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -34020,7 +34536,7 @@
         <xdr:cNvPr id="247" name="直接连接符 246">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000F7000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000F7000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -34070,7 +34586,7 @@
         <xdr:cNvPr id="248" name="直接连接符 247">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000F8000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000F8000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -34122,7 +34638,7 @@
         <xdr:cNvPr id="249" name="直接连接符 248">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000F9000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000F9000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -34174,7 +34690,7 @@
         <xdr:cNvPr id="250" name="等腰三角形 249">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000FA000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000FA000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -34237,7 +34753,7 @@
         <xdr:cNvPr id="251" name="图片 250">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000FB000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000FB000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -34281,7 +34797,7 @@
         <xdr:cNvPr id="252" name="图片 251">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000FC000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000FC000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -34325,7 +34841,7 @@
         <xdr:cNvPr id="253" name="图片 252">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000FD000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000FD000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -34369,7 +34885,7 @@
         <xdr:cNvPr id="254" name="椭圆 253">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000FE000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-0000FE000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -34430,7 +34946,7 @@
         <xdr:cNvPr id="256" name="椭圆 255">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000000010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000000010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -34490,7 +35006,7 @@
         <xdr:cNvPr id="259" name="直接连接符 258">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -34548,7 +35064,7 @@
         <xdr:cNvPr id="262" name="直接连接符 261">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000006010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -34606,7 +35122,7 @@
         <xdr:cNvPr id="266" name="直接连接符 265">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000A010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000A010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -34663,7 +35179,7 @@
         <xdr:cNvPr id="276" name="立方体 275">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000014010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000014010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -34726,7 +35242,7 @@
         <xdr:cNvPr id="277" name="椭圆 276">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000015010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000015010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -34792,7 +35308,7 @@
         <xdr:cNvPr id="278" name="椭圆 277">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000016010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000016010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -34852,7 +35368,7 @@
         <xdr:cNvPr id="287" name="立方体 286">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001F010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00001F010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -34913,7 +35429,7 @@
         <xdr:cNvPr id="289" name="椭圆 288">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000021010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000021010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -34979,7 +35495,7 @@
         <xdr:cNvPr id="290" name="椭圆 289">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000022010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000022010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -35039,7 +35555,7 @@
         <xdr:cNvPr id="280" name="直接连接符 279">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000018010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000018010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -35092,7 +35608,7 @@
         <xdr:cNvPr id="257" name="等腰三角形 256">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000001010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000001010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -35150,7 +35666,7 @@
         <xdr:cNvPr id="258" name="文本框 257">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -35225,7 +35741,7 @@
         <xdr:cNvPr id="260" name="文本框 259">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -35300,7 +35816,7 @@
         <xdr:cNvPr id="265" name="文本框 264">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000009010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -35380,7 +35896,7 @@
         <xdr:cNvPr id="267" name="椭圆 266">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000B010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000B010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -35440,7 +35956,7 @@
         <xdr:cNvPr id="269" name="直接连接符 268">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000D010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000D010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -35493,7 +36009,7 @@
         <xdr:cNvPr id="270" name="直接连接符 269">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000E010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000E010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -35546,7 +36062,7 @@
         <xdr:cNvPr id="273" name="直接连接符 272">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000011010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000011010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -35594,7 +36110,7 @@
         <xdr:cNvPr id="279" name="文本框 278">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000017010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000017010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -35674,7 +36190,7 @@
         <xdr:cNvPr id="282" name="图片 281">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001A010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00001A010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -35718,7 +36234,7 @@
         <xdr:cNvPr id="283" name="图片 282">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001B010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00001B010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -35762,7 +36278,7 @@
         <xdr:cNvPr id="284" name="等腰三角形 283">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001C010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00001C010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -35825,7 +36341,7 @@
         <xdr:cNvPr id="285" name="图片 284">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001D010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00001D010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -35869,7 +36385,7 @@
         <xdr:cNvPr id="286" name="图片 285">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001E010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00001E010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -35913,7 +36429,7 @@
         <xdr:cNvPr id="288" name="图片 287">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000020010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000020010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -35957,7 +36473,7 @@
         <xdr:cNvPr id="291" name="椭圆 290">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000023010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000023010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -36018,7 +36534,7 @@
         <xdr:cNvPr id="293" name="直接连接符 292">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000025010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000025010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -36071,7 +36587,7 @@
         <xdr:cNvPr id="295" name="直接连接符 294">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000027010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000027010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -36124,7 +36640,7 @@
         <xdr:cNvPr id="297" name="直接连接符 296">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000029010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000029010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -36176,7 +36692,7 @@
         <xdr:cNvPr id="298" name="直接连接符 297">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002A010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00002A010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -36231,7 +36747,7 @@
         <xdr:cNvPr id="303" name="直接连接符 302">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002F010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00002F010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -36286,7 +36802,7 @@
         <xdr:cNvPr id="304" name="直接连接符 303">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000030010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000030010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -36341,7 +36857,7 @@
         <xdr:cNvPr id="292" name="椭圆 291">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000024010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000024010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -36401,7 +36917,7 @@
         <xdr:cNvPr id="305" name="图片 304">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000031010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000031010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -36445,7 +36961,7 @@
         <xdr:cNvPr id="306" name="图片 305">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000032010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000032010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -36489,7 +37005,7 @@
         <xdr:cNvPr id="307" name="图片 306">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000033010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000033010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -36533,7 +37049,7 @@
         <xdr:cNvPr id="308" name="椭圆 307">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000034010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000034010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -36594,7 +37110,7 @@
         <xdr:cNvPr id="309" name="椭圆 308">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000035010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000035010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -36654,7 +37170,7 @@
         <xdr:cNvPr id="311" name="直接连接符 310">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000037010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000037010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -36707,7 +37223,7 @@
         <xdr:cNvPr id="312" name="椭圆 311">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000038010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000038010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -36767,7 +37283,7 @@
         <xdr:cNvPr id="316" name="直接连接符 315">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003C010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00003C010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -36820,7 +37336,7 @@
         <xdr:cNvPr id="317" name="文本框 316">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003D010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00003D010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -36896,7 +37412,7 @@
         <xdr:cNvPr id="320" name="椭圆 319">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000040010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000040010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -36964,7 +37480,7 @@
         <xdr:cNvPr id="112" name="图片 111">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000070000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000070000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -37008,7 +37524,7 @@
         <xdr:cNvPr id="127" name="椭圆 126">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00007F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00007F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -37069,7 +37585,7 @@
         <xdr:cNvPr id="321" name="文本框 320">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000041010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000041010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -37139,7 +37655,7 @@
         <xdr:cNvPr id="274" name="直接连接符 273">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000012010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000012010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -37189,7 +37705,7 @@
         <xdr:cNvPr id="294" name="直接连接符 293">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000026010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000026010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -37239,7 +37755,7 @@
         <xdr:cNvPr id="299" name="直接连接符 298">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002B010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00002B010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -37289,7 +37805,7 @@
         <xdr:cNvPr id="301" name="直接连接符 300">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002D010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00002D010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -37339,7 +37855,7 @@
         <xdr:cNvPr id="310" name="直接连接符 309">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000036010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000036010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -37389,7 +37905,7 @@
         <xdr:cNvPr id="314" name="直接连接符 313">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003A010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00003A010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -37437,7 +37953,7 @@
         <xdr:cNvPr id="318" name="文本框 317">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003E010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00003E010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -37508,7 +38024,7 @@
         <xdr:cNvPr id="323" name="文本框 322">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000043010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000043010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -37579,7 +38095,7 @@
         <xdr:cNvPr id="324" name="文本框 323">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000044010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000044010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -37650,7 +38166,7 @@
         <xdr:cNvPr id="325" name="文本框 324">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000045010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000045010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -37726,7 +38242,7 @@
         <xdr:cNvPr id="326" name="椭圆 325">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000046010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000046010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -37786,7 +38302,7 @@
         <xdr:cNvPr id="328" name="直接连接符 327">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000048010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000048010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -37841,7 +38357,7 @@
         <xdr:cNvPr id="334" name="直接连接符 333">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00004E010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00004E010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -37896,7 +38412,7 @@
         <xdr:cNvPr id="348" name="直接连接符 347">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00005C010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00005C010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -37951,7 +38467,7 @@
         <xdr:cNvPr id="149" name="直接连接符 148">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000095000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000095000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38001,7 +38517,7 @@
         <xdr:cNvPr id="151" name="文本框 150">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000097000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000097000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38072,7 +38588,7 @@
         <xdr:cNvPr id="156" name="文本框 155">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00009C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00009C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38143,7 +38659,7 @@
         <xdr:cNvPr id="352" name="文本框 351">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000060010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000060010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38214,7 +38730,7 @@
         <xdr:cNvPr id="353" name="文本框 352">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000061010000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000061010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38578,7 +39094,7 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -38595,7 +39111,7 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -38612,7 +39128,7 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -38632,9 +39148,9 @@
       <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="4.83203125" style="1"/>
+    <col min="1" max="16384" width="4.875" style="1"/>
   </cols>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -38652,10 +39168,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH14" sqref="AH14"/>
+      <selection activeCell="Z13" sqref="Z13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.25" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -38675,9 +39191,9 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="45" spans="15:15" ht="28.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="15:15" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O45" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified   doc/images/painter.xlsx Modified   doc/一起动手实现3D渲染引擎.md Modified   doc/一起动手实现3D渲染引擎.pdf Add        doc/images/matrix-linear-transformation-01.png Add        doc/images/matrix-linear-transformation-02.png Add        doc/images/matrix-linear-transformation-03.png Add        doc/images/matrix-linear-transformation-04.png Add        doc/images/matrix-rotation-2D.png Add        doc/images/matrix-rotation-dir-left.png Add        doc/images/matrix-rotation-dir-right.png
</commit_message>
<xml_diff>
--- a/doc/images/painter.xlsx
+++ b/doc/images/painter.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaronwang\workspace\projects\private\Tiny3D\steps\doc\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\MyGame\Tiny3D\steps\doc\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12170" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="左右手坐标系" sheetId="1" r:id="rId1"/>
@@ -18911,20 +18911,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>367392</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>142279</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>37564</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="70" name="图片 69"/>
+        <xdr:cNvPr id="96" name="图片 95">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA498EC8-8E1E-497C-B6FB-632122E05DD1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18936,9 +18942,9 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm rot="924007">
-          <a:off x="7023100" y="6921500"/>
-          <a:ext cx="2920092" cy="1104900"/>
+        <a:xfrm rot="1011333">
+          <a:off x="6153149" y="10201275"/>
+          <a:ext cx="4761905" cy="4285714"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -18949,26 +18955,76 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>25401</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>146051</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>367393</xdr:colOff>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>367392</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>184151</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="图片 12"/>
+        <xdr:cNvPr id="70" name="图片 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000046000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="924007">
+          <a:off x="7023100" y="6921500"/>
+          <a:ext cx="2920092" cy="1104900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>25401</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>146051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>367393</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>184151</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="图片 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -20929,51 +20985,7 @@
         <xdr:cNvPr id="10" name="图片 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22837E9D-408B-471B-ACB6-ABB135A00E82}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3752850" y="2514600"/>
-          <a:ext cx="792481" cy="247650"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>361951</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>70486</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>266700</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="图片 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59A76FAC-AE69-4860-AB8E-93E8D72F06F9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20989,8 +21001,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1476376" y="1800225"/>
-          <a:ext cx="822960" cy="228600"/>
+          <a:off x="3752850" y="2514600"/>
+          <a:ext cx="792481" cy="247650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -21001,23 +21013,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>88195</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>314325</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>361951</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>70486</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="图片 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65F9B342-E6C7-4B84-92BB-0BEADA4AA33E}"/>
+        <xdr:cNvPr id="11" name="图片 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21033,8 +21045,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3105150" y="933450"/>
-          <a:ext cx="697795" cy="438150"/>
+          <a:off x="1476376" y="1800225"/>
+          <a:ext cx="822960" cy="228600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -21043,127 +21055,25 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>88195</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>314325</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>110773</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>95251</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="14" name="直接连接符 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20CF1881-9031-4E29-8057-EA172A6D1845}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:endCxn id="12" idx="2"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="2428875" y="1371600"/>
-          <a:ext cx="1025173" cy="485776"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>314325</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>171451</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>285751</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="17" name="直接连接符 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0F77268-674F-4434-982F-A639A7048A34}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="3295650" y="1371600"/>
-          <a:ext cx="590551" cy="1028701"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>78105</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>323850</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="47" name="图片 46">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25A5D555-4D17-4209-9D77-4BEF75B7DC8C}"/>
+        <xdr:cNvPr id="12" name="图片 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21172,15 +21082,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9315449" y="2543175"/>
-          <a:ext cx="792481" cy="247650"/>
+          <a:off x="3105150" y="933450"/>
+          <a:ext cx="697795" cy="438150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -21189,25 +21099,127 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>110773</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="直接连接符 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="12" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2428875" y="1371600"/>
+          <a:ext cx="1025173" cy="485776"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>171451</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>285751</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="直接连接符 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3295650" y="1371600"/>
+          <a:ext cx="590551" cy="1028701"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>156210</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>247650</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>78105</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="48" name="图片 47">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E779C33-D8B8-45AD-94D1-10D73B7335CD}"/>
+        <xdr:cNvPr id="47" name="图片 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21223,8 +21235,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6391275" y="1781175"/>
-          <a:ext cx="822960" cy="228600"/>
+          <a:off x="9315449" y="2543175"/>
+          <a:ext cx="792481" cy="247650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -21235,23 +21247,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>152399</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>323850</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>107244</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>156210</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="50" name="图片 49">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CD98B11-6DDF-468C-BF34-3EDBAB5DB883}"/>
+        <xdr:cNvPr id="48" name="图片 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000030000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21267,6 +21279,50 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
+          <a:off x="6391275" y="1781175"/>
+          <a:ext cx="822960" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>107244</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="50" name="图片 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000032000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
           <a:off x="8324849" y="676275"/>
           <a:ext cx="697795" cy="438150"/>
         </a:xfrm>
@@ -21295,7 +21351,7 @@
         <xdr:cNvPr id="51" name="直接连接符 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F2E63D0-8220-4EC4-ABC5-A67A9C0F5656}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000033000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21347,7 +21403,7 @@
         <xdr:cNvPr id="53" name="直接连接符 52">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2148B089-FF19-4EAC-8138-120F85DF14FF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000035000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21397,7 +21453,7 @@
         <xdr:cNvPr id="46" name="直接箭头连接符 45">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21451,7 +21507,7 @@
         <xdr:cNvPr id="54" name="直接箭头连接符 53">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000036000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21500,7 +21556,7 @@
         <xdr:cNvPr id="56" name="文本框 55">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000038000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21571,7 +21627,7 @@
         <xdr:cNvPr id="57" name="文本框 56">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000039000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21642,7 +21698,7 @@
         <xdr:cNvPr id="58" name="文本框 57">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21713,7 +21769,7 @@
         <xdr:cNvPr id="61" name="文本框 60">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21789,7 +21845,7 @@
         <xdr:cNvPr id="62" name="直接箭头连接符 61">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21843,7 +21899,7 @@
         <xdr:cNvPr id="64" name="直接箭头连接符 63">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000040000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21892,7 +21948,7 @@
         <xdr:cNvPr id="66" name="文本框 65">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000042000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21963,7 +22019,7 @@
         <xdr:cNvPr id="67" name="文本框 66">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000043000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22034,7 +22090,7 @@
         <xdr:cNvPr id="68" name="文本框 67">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000044000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22105,7 +22161,7 @@
         <xdr:cNvPr id="69" name="文本框 68">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000045000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22171,20 +22227,26 @@
       <xdr:rowOff>254000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>158750</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="右箭头 15"/>
+        <xdr:cNvPr id="16" name="右箭头 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5073650" y="7366000"/>
-          <a:ext cx="977900" cy="203200"/>
+          <a:off x="5114925" y="7302500"/>
+          <a:ext cx="676275" cy="203200"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst/>
@@ -22226,32 +22288,38 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:colOff>25401</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>40</xdr:col>
-      <xdr:colOff>348342</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
+      <xdr:colOff>367393</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>196850</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="71" name="图片 70"/>
+        <xdr:cNvPr id="81" name="图片 80">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000051000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12160250" y="6946900"/>
+        <a:xfrm rot="20670679">
+          <a:off x="12179301" y="1936750"/>
           <a:ext cx="2920092" cy="1104900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -22263,23 +22331,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>215901</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>4763</xdr:colOff>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>349250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="72" name="直接箭头连接符 71">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+        <xdr:cNvPr id="89" name="直接箭头连接符 88">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000059000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22287,8 +22355,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="13106401" y="5695950"/>
-          <a:ext cx="1022349" cy="3543300"/>
+          <a:off x="13627100" y="742950"/>
+          <a:ext cx="4763" cy="3517900"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -22319,30 +22387,30 @@
     <xdr:from>
       <xdr:col>32</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="75" name="直接箭头连接符 74">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+        <xdr:cNvPr id="90" name="直接箭头连接符 89">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00005A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11785600" y="6985000"/>
-          <a:ext cx="3689350" cy="1022350"/>
+        <a:xfrm flipV="1">
+          <a:off x="11785600" y="2489200"/>
+          <a:ext cx="3683000" cy="6350"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -22371,26 +22439,26 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>330200</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="437749" cy="400366"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="76" name="文本框 75">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+        <xdr:cNvPr id="91" name="文本框 90">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00005B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm rot="967537">
-          <a:off x="13960475" y="5340350"/>
+        <a:xfrm>
+          <a:off x="13420725" y="330200"/>
           <a:ext cx="437749" cy="400366"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -22442,26 +22510,26 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>15875</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>273051</xdr:rowOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>206375</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="379463" cy="400366"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="77" name="文本框 76">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
+        <xdr:cNvPr id="92" name="文本框 91">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00005C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm rot="814402">
-          <a:off x="12906375" y="9163051"/>
+        <a:xfrm>
+          <a:off x="13465175" y="4260850"/>
           <a:ext cx="379463" cy="400366"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -22514,25 +22582,25 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>368299</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>323849</xdr:rowOff>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="388761" cy="400366"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="79" name="文本框 78">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000006000000}"/>
+        <xdr:cNvPr id="93" name="文本框 92">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00005D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm rot="829235">
-          <a:off x="11417299" y="6724649"/>
+        <a:xfrm>
+          <a:off x="11379200" y="2286000"/>
           <a:ext cx="388761" cy="400366"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -22585,25 +22653,25 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>41</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>336550</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="447045" cy="400366"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="80" name="文本框 79">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000007000000}"/>
+        <xdr:cNvPr id="94" name="文本框 93">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00005E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm rot="789695">
-          <a:off x="15424150" y="7842250"/>
+        <a:xfrm>
+          <a:off x="15436850" y="2292350"/>
           <a:ext cx="447045" cy="400366"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -22655,33 +22723,39 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>25401</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>40</xdr:col>
-      <xdr:colOff>367393</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>5442</xdr:colOff>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>196850</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="81" name="图片 80"/>
+        <xdr:cNvPr id="101" name="图片 100">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000065000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm rot="20670679">
-          <a:off x="12179301" y="1936750"/>
+        <a:xfrm rot="924007">
+          <a:off x="1136650" y="11893550"/>
           <a:ext cx="2920092" cy="1104900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -22693,23 +22767,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>4763</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>349250</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>11113</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="89" name="直接箭头连接符 88">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+        <xdr:cNvPr id="102" name="直接箭头连接符 101">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000066000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22717,7 +22791,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="13627100" y="742950"/>
+          <a:off x="2584450" y="10693400"/>
           <a:ext cx="4763" cy="3517900"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -22747,23 +22821,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>42</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="90" name="直接箭头连接符 89">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+        <xdr:cNvPr id="103" name="直接箭头连接符 102">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000067000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22771,7 +22845,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="11785600" y="2489200"/>
+          <a:off x="742950" y="12439650"/>
           <a:ext cx="3683000" cy="6350"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -22801,18 +22875,18 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>330200</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>168275</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="437749" cy="400366"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="91" name="文本框 90">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+        <xdr:cNvPr id="104" name="文本框 103">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000068000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22820,7 +22894,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13420725" y="330200"/>
+          <a:off x="2378075" y="10280650"/>
           <a:ext cx="437749" cy="400366"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -22872,18 +22946,18 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>206375</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>349250</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>212725</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="379463" cy="400366"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="92" name="文本框 91">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
+        <xdr:cNvPr id="105" name="文本框 104">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000069000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22891,7 +22965,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13465175" y="4260850"/>
+          <a:off x="2422525" y="14211300"/>
           <a:ext cx="379463" cy="400366"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -22943,18 +23017,18 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>336550</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="388761" cy="400366"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="93" name="文本框 92">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000006000000}"/>
+        <xdr:cNvPr id="106" name="文本框 105">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00006A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22962,7 +23036,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11379200" y="2286000"/>
+          <a:off x="336550" y="12236450"/>
           <a:ext cx="388761" cy="400366"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -23014,18 +23088,18 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>41</xdr:col>
-      <xdr:colOff>336550</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="447045" cy="400366"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="94" name="文本框 93">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000007000000}"/>
+        <xdr:cNvPr id="107" name="文本框 106">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00006B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23033,7 +23107,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15436850" y="2292350"/>
+          <a:off x="4394200" y="12242800"/>
           <a:ext cx="447045" cy="400366"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -23085,20 +23159,234 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>31750</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>5442</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>196850</xdr:rowOff>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>237163</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="101" name="图片 100"/>
+        <xdr:cNvPr id="39" name="图片 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000027000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4089400" y="10699750"/>
+          <a:ext cx="567363" cy="361950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>165304</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>330200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>178586</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="直接连接符 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000029000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="101" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2743404" y="10998200"/>
+          <a:ext cx="1345996" cy="915186"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>18846</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>217909</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="115" name="图片 114">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000073000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9962946" y="10687050"/>
+          <a:ext cx="567363" cy="361950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>317500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>18846</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>165886</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="116" name="直接连接符 115">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000074000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8616950" y="10985500"/>
+          <a:ext cx="1345996" cy="915186"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>200027</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>132757</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>75663</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="图片 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45540FD1-CDE7-4055-A029-D24D0D9102FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -23110,9 +23398,9 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm rot="924007">
-          <a:off x="1136650" y="11893550"/>
-          <a:ext cx="2920092" cy="1104900"/>
+        <a:xfrm rot="1011333">
+          <a:off x="11344277" y="5305424"/>
+          <a:ext cx="4761905" cy="4285714"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -23123,23 +23411,95 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="等号 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{853C2421-C036-4057-AD9A-16736C0A07FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5238750" y="6819900"/>
+          <a:ext cx="609600" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="mathEqual">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>11113</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:colOff>17463</xdr:colOff>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>342900</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="102" name="直接箭头连接符 101">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+        <xdr:cNvPr id="117" name="直接箭头连接符 116">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D6D9EB6-F31E-4AEA-B405-77D69EB4B677}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23147,8 +23507,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="2584450" y="10693400"/>
-          <a:ext cx="4763" cy="3517900"/>
+          <a:off x="2613025" y="15532100"/>
+          <a:ext cx="4763" cy="3489325"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -23178,22 +23538,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>349250</xdr:rowOff>
+      <xdr:colOff>3175</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>3175</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="103" name="直接箭头连接符 102">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+        <xdr:cNvPr id="118" name="直接箭头连接符 117">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B69BCF43-FAC8-4521-91D5-15BA508CE0FC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23201,8 +23561,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="742950" y="12439650"/>
-          <a:ext cx="3683000" cy="6350"/>
+          <a:off x="746125" y="17980025"/>
+          <a:ext cx="3714750" cy="3175"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -23232,17 +23592,17 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>168275</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:colOff>174625</xdr:colOff>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>323850</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="437749" cy="400366"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="104" name="文本框 103">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+        <xdr:cNvPr id="119" name="文本框 118">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F56BEB80-8951-40FB-ACE1-F4AAD6670B5F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23250,7 +23610,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2378075" y="10280650"/>
+          <a:off x="2403475" y="15125700"/>
           <a:ext cx="437749" cy="400366"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -23303,17 +23663,17 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>212725</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>342900</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="379463" cy="400366"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="105" name="文本框 104">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
+        <xdr:cNvPr id="120" name="文本框 119">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76F18D1C-FE75-4505-804D-BD62CBFCC763}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23321,7 +23681,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2422525" y="14211300"/>
+          <a:off x="2447925" y="19021425"/>
           <a:ext cx="379463" cy="400366"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -23374,17 +23734,17 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>336550</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="388761" cy="400366"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="106" name="文本框 105">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000006000000}"/>
+        <xdr:cNvPr id="121" name="文本框 120">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00C376CA-82BE-4612-ADE8-36FC9ECC0A55}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23392,7 +23752,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="336550" y="12236450"/>
+          <a:off x="361950" y="17786350"/>
           <a:ext cx="388761" cy="400366"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -23445,17 +23805,17 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="447045" cy="400366"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="107" name="文本框 106">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000007000000}"/>
+        <xdr:cNvPr id="122" name="文本框 121">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DB3C9B1-9D09-4196-A6C8-563B4316222D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23463,7 +23823,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4394200" y="12242800"/>
+          <a:off x="4435475" y="17783175"/>
           <a:ext cx="447045" cy="400366"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -23513,36 +23873,406 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="123" name="直接箭头连接符 122">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4846BCB1-E1E1-4CCE-B7A7-A868D1C2582E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2619375" y="16573500"/>
+          <a:ext cx="0" cy="1409700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="124" name="直接箭头连接符 123">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45AA38CF-FB01-4F00-B589-6F490CAAFE3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2619375" y="17992725"/>
+          <a:ext cx="1466850" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>69993</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>301006</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>19052</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="125" name="直接箭头连接符 124">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AA8C44C-48E7-4A4D-913C-145657ECCEBF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2619375" y="16986393"/>
+          <a:ext cx="1024906" cy="1006334"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>70471</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>69993</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="126" name="直接箭头连接符 125">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7B504C1-DA70-45DD-A42D-477C3651A8C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1556371" y="16986393"/>
+          <a:ext cx="1053480" cy="1006332"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>287292</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>142812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>24839</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>31380</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="128" name="箭头: 下弧形 127">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0C5439F-D19A-4725-A766-AF155E87A24D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="14501763">
+          <a:off x="3016894" y="17653835"/>
+          <a:ext cx="593418" cy="109022"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedUpArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 5500"/>
+            <a:gd name="adj2" fmla="val 71990"/>
+            <a:gd name="adj3" fmla="val 63752"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>169780</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>49048</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>20248</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>133108</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="129" name="箭头: 下弧形 128">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCBC5B1D-1EE4-43C7-95AA-75910B79A6E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="9491210">
+          <a:off x="2027155" y="17317873"/>
+          <a:ext cx="593418" cy="84060"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedUpArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 5500"/>
+            <a:gd name="adj2" fmla="val 71990"/>
+            <a:gd name="adj3" fmla="val 63752"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>237163</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="39" name="图片 38"/>
+        <xdr:cNvPr id="131" name="图片 130">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{332EDB2D-C89A-48AA-9445-27831D5DC9F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4089400" y="10699750"/>
-          <a:ext cx="567363" cy="361950"/>
+          <a:off x="3152775" y="16706850"/>
+          <a:ext cx="1238250" cy="247650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -23551,91 +24281,42 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>165304</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>330200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>178586</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="41" name="直接连接符 40"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="101" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="2743404" y="10998200"/>
-          <a:ext cx="1345996" cy="915186"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="dk1"/>
-          </a:solidFill>
-          <a:prstDash val="dash"/>
-          <a:round/>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>12699</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>203202</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>354691</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>241302</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>149227</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="108" name="图片 107"/>
+        <xdr:cNvPr id="132" name="图片 131">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A1E1CEB-FBEF-497C-B0E2-16EC67848AE5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm rot="930789">
-          <a:off x="6642099" y="11938002"/>
-          <a:ext cx="2920092" cy="1104900"/>
+        <a:xfrm>
+          <a:off x="657225" y="16706850"/>
+          <a:ext cx="1349377" cy="238125"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -23644,428 +24325,42 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>254003</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>342901</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="109" name="直接箭头连接符 108">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="7620003" y="10674350"/>
-          <a:ext cx="1003297" cy="3536951"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd type="triangle"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>6351</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>241300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>12701</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>196850</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="110" name="直接箭头连接符 109">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6267451" y="11976100"/>
-          <a:ext cx="3689350" cy="1022350"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd type="triangle"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>365126</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="437749" cy="400366"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="111" name="文本框 110">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="967537">
-          <a:off x="8467726" y="10312401"/>
-          <a:ext cx="437749" cy="400366"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
-              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
-            </a:rPr>
-            <a:t>+Y</a:t>
-          </a:r>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
-            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>22226</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>285751</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="379463" cy="400366"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="112" name="文本框 111">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="814402">
-          <a:off x="7388226" y="14154151"/>
-          <a:ext cx="379463" cy="400366"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
-              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
-            </a:rPr>
-            <a:t>-Y</a:t>
-          </a:r>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
-            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>336549</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="388761" cy="400366"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="113" name="文本框 112">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000006000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="829235">
-          <a:off x="5899150" y="11715749"/>
-          <a:ext cx="388761" cy="400366"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
-              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
-            </a:rPr>
-            <a:t>-X</a:t>
-          </a:r>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
-            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>330201</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="447045" cy="400366"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="114" name="文本框 113">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000007000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="789695">
-          <a:off x="9906001" y="12833350"/>
-          <a:ext cx="447045" cy="400366"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
-              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
-            </a:rPr>
-            <a:t>+X</a:t>
-          </a:r>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
-            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>18846</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>217909</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>323851</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>348615</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="115" name="图片 114"/>
+        <xdr:cNvPr id="133" name="图片 132">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54C2EF84-7C48-494A-AAD6-09CBE93E8E74}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9962946" y="10687050"/>
-          <a:ext cx="567363" cy="361950"/>
+          <a:off x="3667126" y="18059400"/>
+          <a:ext cx="876300" cy="262890"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -24074,57 +24369,136 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>146050</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>317500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>18846</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>165886</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="116" name="直接连接符 115"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="8616950" y="10985500"/>
-          <a:ext cx="1345996" cy="915186"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="dk1"/>
-          </a:solidFill>
-          <a:prstDash val="dash"/>
-          <a:round/>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>336351</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="134" name="图片 133">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C4A30FC-7F7B-4A47-A6F3-4D2E1279952E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1838325" y="16306800"/>
+          <a:ext cx="771525" cy="241101"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>257146</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>314296</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="135" name="图片 134">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA0DD8D5-FE60-4407-9948-813EEB6FEFD9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3000375" y="17706975"/>
+          <a:ext cx="228571" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>323821</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>28546</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="136" name="图片 135">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7489A69-2655-4D7F-98C4-B0A9E5CADC2D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2324100" y="17421225"/>
+          <a:ext cx="228571" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -41918,7 +42292,7 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -41935,7 +42309,7 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -41952,7 +42326,7 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -41968,13 +42342,13 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="4.83203125" style="1"/>
+    <col min="1" max="16384" width="4.875" style="1"/>
   </cols>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -41991,11 +42365,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AN34" sqref="AN34"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD51" sqref="AD51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -42015,9 +42389,9 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="45" spans="15:15" ht="28.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="15:15" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O45" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified   doc/images/painter.xlsx Modified   doc/一起动手实现3D渲染引擎.md Add        doc/images/3D-rotation-by-axis-01.fbx Add        doc/images/3D-rotation-by-axis.fbx Add        doc/images/blue-01.png Add        doc/images/green-01.png Add        doc/images/matrix-3D-rotation-x.png Add        doc/images/matrix-3D-rotation-y.png Add        doc/images/matrix-3D-rotation-z.png Add        doc/images/red-01.png Add        doc/images/red.png Add        doc/images/yellow.png
</commit_message>
<xml_diff>
--- a/doc/images/painter.xlsx
+++ b/doc/images/painter.xlsx
@@ -24493,6 +24493,138 @@
         <a:xfrm>
           <a:off x="2324100" y="17421225"/>
           <a:ext cx="228571" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>151638</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>218432</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="图片 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAB65E8A-8CB7-4A35-AFDD-962B8AAE2579}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5943600" y="15163800"/>
+          <a:ext cx="6095238" cy="5142857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>161163</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>323195</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="图片 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6AB086E-B8B3-4E8D-9F48-08E3197B7302}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="381000" y="20812125"/>
+          <a:ext cx="6095238" cy="5238095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>151638</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>304145</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="图片 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCE01498-681B-40A4-AAF3-0D62C38A604C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7058025" y="20793075"/>
+          <a:ext cx="6095238" cy="5238095"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -42365,8 +42497,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD51" sqref="AD51"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AJ50" sqref="AJ50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Missing    doc/images/3D-rotation-by-axis-01.fbx Missing    doc/images/3D-rotation-by-axis.fbx Modified   doc/images/painter.xlsx Modified   doc/一起动手实现3D渲染引擎.md Add        doc/images/7404_9060247.JPG Add        doc/images/matrix-3D-rotation-by-axis-01.fbx Add        doc/images/matrix-3D-rotation-by-axis.fbx Add        doc/images/matrix-projection.fbx
</commit_message>
<xml_diff>
--- a/doc/images/painter.xlsx
+++ b/doc/images/painter.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\MyGame\Tiny3D\steps\doc\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaronwang\workspace\projects\private\Tiny3D\steps\doc\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12170" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="左右手坐标系" sheetId="1" r:id="rId1"/>
@@ -18911,26 +18911,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>209549</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>333375</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>142279</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>37564</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>279400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="96" name="图片 95">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA498EC8-8E1E-497C-B6FB-632122E05DD1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="207" name="图片 206"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18942,9 +18936,9 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm rot="1011333">
-          <a:off x="6153149" y="10201275"/>
-          <a:ext cx="4761905" cy="4285714"/>
+        <a:xfrm>
+          <a:off x="11747500" y="27076400"/>
+          <a:ext cx="228600" cy="228600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -18955,26 +18949,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>367392</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>196851</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>93981</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="70" name="图片 69">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000046000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="205" name="图片 204"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18986,9 +18974,9 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm rot="924007">
-          <a:off x="7023100" y="6921500"/>
-          <a:ext cx="2920092" cy="1104900"/>
+        <a:xfrm>
+          <a:off x="12719051" y="27514550"/>
+          <a:ext cx="265430" cy="209550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -18999,32 +18987,435 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>25401</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>146051</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>367393</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>184151</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>196850</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="图片 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000D000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="204" name="图片 203"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12109450" y="28060650"/>
+          <a:ext cx="285750" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="190" name="直接箭头连接符 189">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45AA38CF-FB01-4F00-B589-6F490CAAFE3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10318750" y="27019250"/>
+          <a:ext cx="1835150" cy="2844800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="176" name="直接箭头连接符 175">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45AA38CF-FB01-4F00-B589-6F490CAAFE3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10318750" y="28448000"/>
+          <a:ext cx="2946400" cy="1416050"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>12701</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>190224</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>355599</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="146" name="图片 145"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1117601" y="31838624"/>
+          <a:ext cx="1104899" cy="520975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>12701</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>6922</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>330</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="145" name="图片 144"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5537201" y="27743150"/>
+          <a:ext cx="1467421" cy="1416380"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>12701</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>368072</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="144" name="图片 143"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1117601" y="28448000"/>
+          <a:ext cx="723671" cy="698500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>142279</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>37564</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="96" name="图片 95">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA498EC8-8E1E-497C-B6FB-632122E05DD1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="1011333">
+          <a:off x="6153149" y="10201275"/>
+          <a:ext cx="4761905" cy="4285714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>367392</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>203200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="70" name="图片 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000046000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="924007">
+          <a:off x="7023100" y="6921500"/>
+          <a:ext cx="2920092" cy="1104900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>25401</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>146051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>367393</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>184151</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="图片 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -20994,7 +21385,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21038,7 +21429,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21082,7 +21473,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21228,7 +21619,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21272,7 +21663,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21316,7 +21707,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -22312,7 +22703,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -22748,7 +23139,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -23184,7 +23575,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -23289,7 +23680,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -23392,7 +23783,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -23931,13 +24322,13 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>51</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -23951,9 +24342,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2619375" y="17992725"/>
-          <a:ext cx="1466850" cy="1"/>
+        <a:xfrm flipV="1">
+          <a:off x="2597150" y="18141950"/>
+          <a:ext cx="1447800" cy="12700"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -24264,314 +24655,6 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3152775" y="16706850"/>
-          <a:ext cx="1238250" cy="247650"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>149227</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="132" name="图片 131">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A1E1CEB-FBEF-497C-B0E2-16EC67848AE5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="657225" y="16706850"/>
-          <a:ext cx="1349377" cy="238125"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>323851</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>85726</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>348615</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="133" name="图片 132">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54C2EF84-7C48-494A-AAD6-09CBE93E8E74}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3667126" y="18059400"/>
-          <a:ext cx="876300" cy="262890"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>336351</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="134" name="图片 133">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C4A30FC-7F7B-4A47-A6F3-4D2E1279952E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1838325" y="16306800"/>
-          <a:ext cx="771525" cy="241101"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>257146</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>314296</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="135" name="图片 134">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA0DD8D5-FE60-4407-9948-813EEB6FEFD9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3000375" y="17706975"/>
-          <a:ext cx="228571" cy="228571"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>323821</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>28546</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="136" name="图片 135">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7489A69-2655-4D7F-98C4-B0A9E5CADC2D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2324100" y="17421225"/>
-          <a:ext cx="228571" cy="228571"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>151638</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>218432</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="图片 19">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAB65E8A-8CB7-4A35-AFDD-962B8AAE2579}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5943600" y="15163800"/>
-          <a:ext cx="6095238" cy="5142857"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>161163</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>323195</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="图片 20">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6AB086E-B8B3-4E8D-9F48-08E3197B7302}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
         <a:stretch>
           <a:fillRect/>
@@ -24579,8 +24662,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="381000" y="20812125"/>
-          <a:ext cx="6095238" cy="5238095"/>
+          <a:off x="3152775" y="16706850"/>
+          <a:ext cx="1238250" cy="247650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -24591,23 +24674,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>151638</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>304145</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>149227</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="33" name="图片 32">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCE01498-681B-40A4-AAF3-0D62C38A604C}"/>
+        <xdr:cNvPr id="132" name="图片 131">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A1E1CEB-FBEF-497C-B0E2-16EC67848AE5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24623,8 +24706,3203 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
+          <a:off x="657225" y="16706850"/>
+          <a:ext cx="1349377" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>323851</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>348615</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="133" name="图片 132">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54C2EF84-7C48-494A-AAD6-09CBE93E8E74}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3667126" y="18059400"/>
+          <a:ext cx="876300" cy="262890"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>336351</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="134" name="图片 133">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C4A30FC-7F7B-4A47-A6F3-4D2E1279952E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1838325" y="16306800"/>
+          <a:ext cx="771525" cy="241101"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>257146</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>314296</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="135" name="图片 134">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA0DD8D5-FE60-4407-9948-813EEB6FEFD9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3000375" y="17706975"/>
+          <a:ext cx="228571" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>323821</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>28546</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="136" name="图片 135">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7489A69-2655-4D7F-98C4-B0A9E5CADC2D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2324100" y="17421225"/>
+          <a:ext cx="228571" cy="228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>151638</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>218432</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="图片 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAB65E8A-8CB7-4A35-AFDD-962B8AAE2579}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5943600" y="15163800"/>
+          <a:ext cx="6095238" cy="5142857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>161163</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>323195</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="图片 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6AB086E-B8B3-4E8D-9F48-08E3197B7302}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="381000" y="20812125"/>
+          <a:ext cx="6095238" cy="5238095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>151638</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>304145</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="图片 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCE01498-681B-40A4-AAF3-0D62C38A604C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
           <a:off x="7058025" y="20793075"/>
           <a:ext cx="6095238" cy="5238095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="109" name="直接箭头连接符 108">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1104900" y="27368500"/>
+          <a:ext cx="6350" cy="2152650"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="110" name="直接箭头连接符 109">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000036000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="736600" y="29152850"/>
+          <a:ext cx="2952750" cy="6350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>155575</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="437749" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="111" name="文本框 110">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000038000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="892175" y="26993850"/>
+          <a:ext cx="437749" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+Y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>330200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="379463" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="112" name="文本框 111">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000039000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="936625" y="29489400"/>
+          <a:ext cx="379463" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-Y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="388761" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="113" name="文本框 112">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="349250" y="28949650"/>
+          <a:ext cx="388761" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-X</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="447045" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="114" name="文本框 113">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3644900" y="28949650"/>
+          <a:ext cx="447045" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+X</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="矩形 33"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1111250" y="28448000"/>
+          <a:ext cx="736600" cy="704850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="130" name="直接箭头连接符 129">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5524500" y="27381200"/>
+          <a:ext cx="0" cy="2133600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="137" name="直接箭头连接符 136">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000036000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5156200" y="29159200"/>
+          <a:ext cx="2952750" cy="6350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>155575</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>336550</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="437749" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="138" name="文本框 137">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000038000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5311775" y="27006550"/>
+          <a:ext cx="437749" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+Y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>212725</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="379463" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="139" name="文本框 138">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000039000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5368925" y="29483050"/>
+          <a:ext cx="379463" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-Y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="388761" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="140" name="文本框 139">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4737100" y="28949650"/>
+          <a:ext cx="388761" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-X</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="447045" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="141" name="文本框 140">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8064500" y="28962350"/>
+          <a:ext cx="447045" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+X</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="142" name="矩形 141"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5530850" y="27736800"/>
+          <a:ext cx="1466850" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="147" name="直接箭头连接符 146">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1104900" y="30581600"/>
+          <a:ext cx="6350" cy="2139950"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="148" name="直接箭头连接符 147">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000036000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="742950" y="32359600"/>
+          <a:ext cx="2952750" cy="6350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>168275</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="437749" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="149" name="文本框 148">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000038000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="904875" y="30219650"/>
+          <a:ext cx="437749" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+Y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>206375</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>336550</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="379463" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="150" name="文本框 149">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000039000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="942975" y="32696150"/>
+          <a:ext cx="379463" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-Y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>336550</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="388761" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="151" name="文本框 150">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="336550" y="32156400"/>
+          <a:ext cx="388761" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-X</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="447045" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="152" name="文本框 151">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3670300" y="32156400"/>
+          <a:ext cx="447045" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+X</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="153" name="矩形 152"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1111250" y="31832550"/>
+          <a:ext cx="1111250" cy="533400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>330</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="154" name="图片 153"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5543551" y="30765750"/>
+          <a:ext cx="1092199" cy="1594180"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="155" name="直接箭头连接符 154">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5530850" y="30581600"/>
+          <a:ext cx="0" cy="2146300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="156" name="直接箭头连接符 155">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000036000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5162550" y="32359600"/>
+          <a:ext cx="2952750" cy="6350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>336550</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="437749" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="157" name="文本框 156">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000038000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5318125" y="30206950"/>
+          <a:ext cx="437749" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+Y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>206375</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="379463" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="158" name="文本框 157">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000039000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5362575" y="32702500"/>
+          <a:ext cx="379463" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-Y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="388761" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="159" name="文本框 158">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4743450" y="32150050"/>
+          <a:ext cx="388761" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-X</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>336550</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="447045" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="160" name="文本框 159">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8070850" y="32162750"/>
+          <a:ext cx="447045" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+X</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="161" name="矩形 160"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5537200" y="30765750"/>
+          <a:ext cx="1104900" cy="1600200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="87" name="直接连接符 86"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="374650" y="30048200"/>
+          <a:ext cx="8102600" cy="6350"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>336550</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="97" name="直接连接符 96"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4419600" y="27031950"/>
+          <a:ext cx="0" cy="6019800"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>57151</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>266701</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>306435</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="98" name="图片 97"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1530351" y="29603700"/>
+          <a:ext cx="2051050" cy="217535"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>63501</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>40267</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>298450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="99" name="图片 98"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5943600" y="29578301"/>
+          <a:ext cx="1094367" cy="234949"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>44449</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>285285</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="100" name="图片 99"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1517649" y="32778700"/>
+          <a:ext cx="1390651" cy="221785"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>57148</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>292100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="162" name="图片 161"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5962650" y="32791400"/>
+          <a:ext cx="1460498" cy="215900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>4763</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="164" name="直接箭头连接符 163">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D6D9EB6-F31E-4AEA-B405-77D69EB4B677}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="10312400" y="27051000"/>
+          <a:ext cx="4763" cy="3517900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>365125</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>365125</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>3175</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="165" name="直接箭头连接符 164">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B69BCF43-FAC8-4521-91D5-15BA508CE0FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9572625" y="29870400"/>
+          <a:ext cx="3683000" cy="3175"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="437749" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="166" name="文本框 165">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F56BEB80-8951-40FB-ACE1-F4AAD6670B5F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10106025" y="26638250"/>
+          <a:ext cx="437749" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+Y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>206375</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="379463" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="167" name="文本框 166">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76F18D1C-FE75-4505-804D-BD62CBFCC763}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10150475" y="30568900"/>
+          <a:ext cx="379463" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-Y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="388761" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="168" name="文本框 167">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00C376CA-82BE-4612-ADE8-36FC9ECC0A55}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9194800" y="29673550"/>
+          <a:ext cx="388761" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-X</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>155575</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="447045" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="169" name="文本框 168">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DB3C9B1-9D09-4196-A6C8-563B4316222D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13233400" y="29670375"/>
+          <a:ext cx="447045" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+X</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="173" name="直接箭头连接符 172">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45AA38CF-FB01-4F00-B589-6F490CAAFE3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10318750" y="28809950"/>
+          <a:ext cx="2197100" cy="1054100"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="170" name="直接箭头连接符 169">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45AA38CF-FB01-4F00-B589-6F490CAAFE3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10312400" y="29159200"/>
+          <a:ext cx="1473200" cy="717550"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="181" name="直接箭头连接符 180">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45AA38CF-FB01-4F00-B589-6F490CAAFE3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10312400" y="27374850"/>
+          <a:ext cx="1111250" cy="2489200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="184" name="直接箭头连接符 183">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45AA38CF-FB01-4F00-B589-6F490CAAFE3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="11417300" y="27374850"/>
+          <a:ext cx="1092200" cy="1435100"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="194" name="直接箭头连接符 193">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45AA38CF-FB01-4F00-B589-6F490CAAFE3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="12153900" y="27019250"/>
+          <a:ext cx="1104900" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>158751</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>342901</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="201" name="图片 200"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11576051" y="29292551"/>
+          <a:ext cx="209550" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>107950</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="202" name="图片 201"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12261850" y="28943300"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>158750</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>139699</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>84136</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="203" name="图片 202"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13049250" y="28587699"/>
+          <a:ext cx="228600" cy="300037"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>222251</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>52071</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>273050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="206" name="图片 205"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10902951" y="27781250"/>
+          <a:ext cx="198120" cy="228600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -42424,7 +45702,7 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -42441,7 +45719,7 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -42458,7 +45736,7 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -42474,13 +45752,13 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="4.875" style="1"/>
+    <col min="1" max="16384" width="4.83203125" style="1"/>
   </cols>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -42497,11 +45775,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AJ50" sqref="AJ50"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AN77" sqref="AN77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -42517,13 +45795,13 @@
   </sheetPr>
   <dimension ref="O45"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="45" spans="15:15" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="15:15" ht="28.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O45" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified   doc/images/painter.xlsx Modified   doc/一起动手实现3D渲染引擎.md Modified   source/step04/Samples/TransformationApp/TransformationApp.cpp Add        doc/images/matrix-3D-aperture-imaging.fbx Add        doc/images/matrix-3D-orth-projection.fbx Add        doc/images/matrix-3D-perp-projection- 01.fbx Add        doc/images/matrix-3D-perp-projection.fbx Add        doc/images/matrix-projection-plane.fbx Add        doc/images/project-plane.png Add        doc/images/white.png
</commit_message>
<xml_diff>
--- a/doc/images/painter.xlsx
+++ b/doc/images/painter.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\MyGame\Tiny3D\steps\doc\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaronwang\workspace\projects\private\Tiny3D\steps\doc\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12170" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="左右手坐标系" sheetId="1" r:id="rId1"/>
@@ -32270,6 +32270,1540 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>367532</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>343216</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>6150</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="242" name="直接箭头连接符 241">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C79658BF-7FF6-43A3-BE5E-0F11F79D33C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="258" idx="2"/>
+          <a:endCxn id="259" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1840732" y="38748016"/>
+          <a:ext cx="6918" cy="3574734"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>357011</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>349408</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>346075</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>349408</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="243" name="直接箭头连接符 242">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{236C9239-D7E2-4597-931B-ACAD146D9C61}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="260" idx="3"/>
+          <a:endCxn id="261" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="725311" y="40532208"/>
+          <a:ext cx="4408664" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>155575</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>298450</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="437749" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="258" name="文本框 257">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3173603-AED2-4256-958E-2A6CDDDA45DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1628775" y="38347650"/>
+          <a:ext cx="437749" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+Y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="379463" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="259" name="文本框 258">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57A5AA30-F9F8-4D75-B03A-167CE560C1AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1651000" y="42322750"/>
+          <a:ext cx="379463" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-Y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>336550</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>149225</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="388761" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="260" name="文本框 259">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59A66C86-26C0-4266-AA43-12185910B31A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="336550" y="40332025"/>
+          <a:ext cx="388761" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-Z</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>346075</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>149225</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="438069" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="261" name="文本框 260">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E49602A9-57F9-45AD-893F-69124D1906A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5133975" y="40332025"/>
+          <a:ext cx="438069" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+Z</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="83" name="直接连接符 82"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1111250" y="39109650"/>
+          <a:ext cx="0" cy="2844800"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="262" name="直接箭头连接符 261">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FA0D247-62FC-43B5-BB16-6EA35FCE59E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1111250" y="39116000"/>
+          <a:ext cx="3676650" cy="1771650"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="200" name="直接连接符 199"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1847850" y="39109650"/>
+          <a:ext cx="2940050" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="209" name="直接连接符 208"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4787900" y="39103300"/>
+          <a:ext cx="0" cy="1422400"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="227" name="直接箭头连接符 226"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1155700" y="39458900"/>
+          <a:ext cx="647700" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="274883" cy="334451"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="230" name="文本框 229"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1346200" y="39154100"/>
+          <a:ext cx="274883" cy="334451"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>d</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="869725" cy="576568"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="231" name="文本框 230"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="146050" y="39185850"/>
+          <a:ext cx="869725" cy="576568"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>Projection</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="r"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>Plane</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>336550</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2336409" cy="334451"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="232" name="文本框 231"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2178050" y="40887650"/>
+          <a:ext cx="2336409" cy="334451"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>Center of projection (the origin)</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>44450</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="234" name="直接连接符 233"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1885950" y="40582850"/>
+          <a:ext cx="336550" cy="317500"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>367532</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>349566</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>6150</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="283" name="直接箭头连接符 282">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C79658BF-7FF6-43A3-BE5E-0F11F79D33C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="285" idx="2"/>
+          <a:endCxn id="286" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7365232" y="38754366"/>
+          <a:ext cx="6918" cy="3574734"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>357011</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>158</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>346075</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>158</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="284" name="直接箭头连接符 283">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{236C9239-D7E2-4597-931B-ACAD146D9C61}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="287" idx="3"/>
+          <a:endCxn id="291" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6249811" y="40538558"/>
+          <a:ext cx="4408664" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>155575</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="437749" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="285" name="文本框 284">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3173603-AED2-4256-958E-2A6CDDDA45DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7153275" y="38354000"/>
+          <a:ext cx="437749" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+Y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="379463" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="286" name="文本框 285">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57A5AA30-F9F8-4D75-B03A-167CE560C1AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7175500" y="42329100"/>
+          <a:ext cx="379463" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-Y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>336550</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>155575</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="388761" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="287" name="文本框 286">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59A66C86-26C0-4266-AA43-12185910B31A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5861050" y="40338375"/>
+          <a:ext cx="388761" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-Z</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>346075</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>155575</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="438069" cy="400366"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="291" name="文本框 290">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E49602A9-57F9-45AD-893F-69124D1906A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10658475" y="40338375"/>
+          <a:ext cx="438069" cy="400366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+Z</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="292" name="直接连接符 291"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8102600" y="39122350"/>
+          <a:ext cx="0" cy="2844800"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="295" name="直接箭头连接符 294">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FA0D247-62FC-43B5-BB16-6EA35FCE59E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7372350" y="39122350"/>
+          <a:ext cx="2940050" cy="1409700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="869725" cy="576568"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="297" name="文本框 296"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8083550" y="41243250"/>
+          <a:ext cx="869725" cy="576568"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>Projection</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>Plane</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="298" name="直接箭头连接符 297"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7404100" y="39465250"/>
+          <a:ext cx="647700" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="274883" cy="334451"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="299" name="文本框 298"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7594600" y="39160450"/>
+          <a:ext cx="274883" cy="334451"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>d</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -50061,7 +51595,7 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -50078,7 +51612,7 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -50095,7 +51629,7 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -50115,9 +51649,9 @@
       <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="4.875" style="1"/>
+    <col min="1" max="16384" width="4.83203125" style="1"/>
   </cols>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -50134,11 +51668,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AM104" sqref="AM104"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AG113" sqref="AG113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -50158,9 +51692,9 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="45" spans="15:15" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="15:15" ht="28.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O45" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Missing    doc/images/7404_9060247.JPG Modified   doc/images/painter.xlsx Modified   doc/一起动手实现3D渲染引擎.md Modified   doc/一起动手实现3D渲染引擎.pdf Add        doc/images/matrix-2D-homogeneous.png Add        doc/images/matrix-3D-aperture-imaging-side-01.png Add        doc/images/matrix-3D-aperture-imaging-side.png Add        doc/images/matrix-3D-aperture-imaging.png Add        doc/images/matrix-3D-orth-projection.png Add        doc/images/matrix-3D-perp-projection-01.png Add        doc/images/matrix-3D-perp-projection.png Add        doc/images/matrix-projection-plane.png
</commit_message>
<xml_diff>
--- a/doc/images/painter.xlsx
+++ b/doc/images/painter.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaronwang\workspace\projects\private\Tiny3D\steps\doc\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\MyGame\Tiny3D\steps\doc\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12170" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="左右手坐标系" sheetId="1" r:id="rId1"/>
@@ -18927,7 +18927,7 @@
         <xdr:cNvPr id="251" name="图片 250">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89BD1D20-183D-4CB8-8D90-AF4DA6888A17}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000FB000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18971,7 +18971,7 @@
         <xdr:cNvPr id="250" name="图片 249">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{283C83AC-BB41-478C-8AEA-E77149F9F915}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000FA000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19015,7 +19015,7 @@
         <xdr:cNvPr id="249" name="图片 248">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76BA191A-1186-421E-97B1-3E516608476B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000F9000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19059,7 +19059,7 @@
         <xdr:cNvPr id="248" name="图片 247">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{666249D5-C2BD-4744-B6BB-F8E958B87452}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000F8000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19103,7 +19103,7 @@
         <xdr:cNvPr id="247" name="图片 246">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F52B9E73-85D6-4017-9311-C99107F845C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000F7000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19147,7 +19147,7 @@
         <xdr:cNvPr id="246" name="图片 245">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F0A255A-9E38-4845-993E-AA750D90EC7C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000F6000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19191,7 +19191,7 @@
         <xdr:cNvPr id="245" name="图片 244">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DD74DFD-4C5B-478F-875A-0ADD7A892373}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000F5000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19235,7 +19235,7 @@
         <xdr:cNvPr id="244" name="图片 243">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF5BBA06-4D9C-4581-9843-AF56E5CD3F2F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000F4000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19279,7 +19279,7 @@
         <xdr:cNvPr id="241" name="图片 240">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FEB70AB-7000-4347-BD8D-B03B05665ECC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000F1000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19323,7 +19323,7 @@
         <xdr:cNvPr id="240" name="图片 239">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6FCA6B4-0F98-45CB-8522-14D000B5C0DF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000F0000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19367,7 +19367,7 @@
         <xdr:cNvPr id="76" name="直接箭头连接符 75">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{302E7379-709F-46ED-8549-CB87839F4EFC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00004C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19421,7 +19421,7 @@
         <xdr:cNvPr id="79" name="直接箭头连接符 78">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68336B48-582B-40DA-A72B-115342F242C1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00004F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28603,7 +28603,7 @@
         <xdr:cNvPr id="163" name="图片 162">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EC67BBD-D728-4716-AEF9-8DE411D636CD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000A3000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28664,7 +28664,7 @@
         <xdr:cNvPr id="171" name="直接箭头连接符 170">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95D5D269-851C-4A09-8D1C-EB004FFC19B7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000AB000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28718,7 +28718,7 @@
         <xdr:cNvPr id="172" name="直接箭头连接符 171">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC25648B-9ADE-41FF-A272-01B55FBF3C7E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000AC000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28767,7 +28767,7 @@
         <xdr:cNvPr id="174" name="文本框 173">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{539D3C64-A0F9-452C-B1AA-8A77946AB76F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000AE000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28838,7 +28838,7 @@
         <xdr:cNvPr id="175" name="文本框 174">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C68DF69E-4A22-416F-A96A-C1B5BF8330B4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000AF000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28909,7 +28909,7 @@
         <xdr:cNvPr id="177" name="文本框 176">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99079CB4-232B-4CF1-A49D-80C1493E3F95}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000B1000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28980,7 +28980,7 @@
         <xdr:cNvPr id="178" name="文本框 177">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FD4E154-CECC-487C-BA7D-5AB5928D5FCE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000B2000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29056,7 +29056,7 @@
         <xdr:cNvPr id="179" name="图片 178">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6A2984E-7430-4057-92F4-0969584769D6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000B3000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29117,7 +29117,7 @@
         <xdr:cNvPr id="180" name="图片 179">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A151E1C8-B6AC-4F9B-BFAB-8FA8E9194863}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000B4000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29178,7 +29178,7 @@
         <xdr:cNvPr id="182" name="图片 181">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DF5766A-35F3-490F-A543-826DAE79538E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000B6000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29234,7 +29234,7 @@
         <xdr:cNvPr id="40" name="文本框 39">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5651C78-5F7A-401E-BB7E-AD511389EA4C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000028000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29295,7 +29295,7 @@
         <xdr:cNvPr id="42" name="文本框 41">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE59EF53-CA45-4D84-A1D8-8183D3A7B4F9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29367,7 +29367,7 @@
         <xdr:cNvPr id="43" name="文本框 42">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8DD4A60-D81D-4B84-8991-DE0F6CDEB2C1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29432,7 +29432,7 @@
         <xdr:cNvPr id="45" name="文本框 44">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9AC3179-8E53-469B-B3AA-37490A0621B8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29518,7 +29518,7 @@
         <xdr:cNvPr id="185" name="直接箭头连接符 184">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F79101C-286E-4429-B0D0-417418FD8D98}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000B9000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29572,7 +29572,7 @@
         <xdr:cNvPr id="186" name="直接箭头连接符 185">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30F75074-FC11-4E2F-9BE5-595AFD28C007}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000BA000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29621,7 +29621,7 @@
         <xdr:cNvPr id="187" name="文本框 186">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98EE386D-7A64-49C5-95DB-8B3E647AB422}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000BB000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29692,7 +29692,7 @@
         <xdr:cNvPr id="188" name="文本框 187">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB65E0AC-C783-4851-956F-BD17F9264D54}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000BC000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29763,7 +29763,7 @@
         <xdr:cNvPr id="189" name="文本框 188">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{942F8EE0-81C6-4AC8-928B-71845B2A4907}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000BD000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29834,7 +29834,7 @@
         <xdr:cNvPr id="191" name="文本框 190">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8976DBD0-80CA-4B29-ABA3-32CF6AFD6B69}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000BF000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29910,7 +29910,7 @@
         <xdr:cNvPr id="192" name="图片 191">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CC98C0C-A461-410F-B088-80F00E746C18}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000C0000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29971,7 +29971,7 @@
         <xdr:cNvPr id="72" name="直接箭头连接符 71">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C12C4FA-06DA-408A-838A-1E09A2A995B2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000048000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30020,7 +30020,7 @@
         <xdr:cNvPr id="85" name="文本框 84">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D541AEBD-D654-4403-9310-D4A99AC3F007}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000055000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30090,7 +30090,7 @@
         <xdr:cNvPr id="86" name="图片 85">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E46E0DCD-56AE-4AB0-9D76-C543EEEFEE97}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000056000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30134,7 +30134,7 @@
         <xdr:cNvPr id="88" name="图片 87">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6C403D9-A690-4223-AF9A-FF4FE056B0F8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000058000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30178,7 +30178,7 @@
         <xdr:cNvPr id="95" name="图片 94">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1DDCD03-BAFD-4394-A792-9DAEE4AB7C01}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00005F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30222,7 +30222,7 @@
         <xdr:cNvPr id="108" name="图片 107">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F8E9FAC-2FE8-4A7D-B016-7592EF768AEF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00006C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30266,7 +30266,7 @@
         <xdr:cNvPr id="127" name="图片 126">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27EA3166-1F67-4707-A387-61BACF493F35}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00007F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30310,7 +30310,7 @@
         <xdr:cNvPr id="143" name="图片 142">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF7B84A3-2862-4B38-B839-BE33E674BCF3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00008F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30354,7 +30354,7 @@
         <xdr:cNvPr id="195" name="直接连接符 194">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9C18D47-56B0-4AE5-8D6C-8F14969EC47B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000C3000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30404,7 +30404,7 @@
         <xdr:cNvPr id="198" name="直接连接符 197">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{774C0CE5-642B-4DA8-8448-BBC589581C39}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000C6000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30459,7 +30459,7 @@
         <xdr:cNvPr id="213" name="图片 212">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D81F7E3-7211-47A5-A57C-9FDB7D607A01}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000D5000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30503,7 +30503,7 @@
         <xdr:cNvPr id="214" name="图片 213">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D94BED71-8510-451C-9E2D-F15CED7904AA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000D6000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30547,7 +30547,7 @@
         <xdr:cNvPr id="215" name="图片 214">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFA3013A-5284-4473-A574-75B98FD67A83}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000D7000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30591,7 +30591,7 @@
         <xdr:cNvPr id="216" name="图片 215">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B2EFBC9-C3FB-4531-A63D-A44635677B2B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000D8000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30635,7 +30635,7 @@
         <xdr:cNvPr id="217" name="图片 216">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B58130D4-891C-4BAD-8D83-BC130FC9DA69}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000D9000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30679,7 +30679,7 @@
         <xdr:cNvPr id="218" name="图片 217">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA6B87A7-51EF-449B-A853-76038EC50642}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000DA000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30723,7 +30723,7 @@
         <xdr:cNvPr id="219" name="图片 218">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC1996E7-501C-440D-B6AC-F7862B030688}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000DB000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30767,7 +30767,7 @@
         <xdr:cNvPr id="220" name="图片 219">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{126A3D20-C7A9-43F7-93D5-DD171572B625}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000DC000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30811,7 +30811,7 @@
         <xdr:cNvPr id="221" name="图片 220">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F1ECB61-4613-4C8A-8DF0-2BDE44335946}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000DD000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30855,7 +30855,7 @@
         <xdr:cNvPr id="222" name="图片 221">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66575AEC-5A96-43CF-8221-2F72AF144814}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000DE000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30899,7 +30899,7 @@
         <xdr:cNvPr id="226" name="直接连接符 225">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D4BAC01-6CE4-408B-8805-8C6BA4038AE6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000E2000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30954,7 +30954,7 @@
         <xdr:cNvPr id="229" name="直接连接符 228">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEF9C458-808A-437F-B725-EB37B68EC549}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000E5000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31009,7 +31009,7 @@
         <xdr:cNvPr id="252" name="图片 251">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DC45AA8-6153-48D2-AD55-4DFA6B29018A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000FC000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31053,7 +31053,7 @@
         <xdr:cNvPr id="253" name="图片 252">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17682C4F-5F08-472C-B125-95FA11FDF2FE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000FD000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31097,7 +31097,7 @@
         <xdr:cNvPr id="254" name="图片 253">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EFE23A3-4EE5-470E-8958-CC74A47B2274}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000FE000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31141,7 +31141,7 @@
         <xdr:cNvPr id="255" name="图片 254">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4888A22-8A80-4797-B8B8-358836C6C269}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000FF000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31185,7 +31185,7 @@
         <xdr:cNvPr id="256" name="图片 255">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFB3874A-04E5-4294-BEA7-3E8E224329BE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000000010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31229,7 +31229,7 @@
         <xdr:cNvPr id="257" name="图片 256">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B8A7325-BC2E-46DB-B409-54B90B33EC94}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000001010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31273,7 +31273,7 @@
         <xdr:cNvPr id="224" name="直接连接符 223">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E46F4EA-0691-403D-B12A-8BAD1A123DE9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000E0000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31328,7 +31328,7 @@
         <xdr:cNvPr id="268" name="直接连接符 267">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E42C8EED-8846-4A8A-BD4F-DBA2292738B9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000C010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31383,7 +31383,7 @@
         <xdr:cNvPr id="273" name="直接连接符 272">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A68637E3-5F75-4A92-8FA3-0C72CE58D963}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000011010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31438,7 +31438,7 @@
         <xdr:cNvPr id="274" name="直接连接符 273">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEBE0E04-1666-4CD6-AEC6-7EC704C66254}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000012010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31493,7 +31493,7 @@
         <xdr:cNvPr id="275" name="直接箭头连接符 274">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C79658BF-7FF6-43A3-BE5E-0F11F79D33C3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000013010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31547,7 +31547,7 @@
         <xdr:cNvPr id="276" name="直接箭头连接符 275">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{236C9239-D7E2-4597-931B-ACAD146D9C61}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000014010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31596,7 +31596,7 @@
         <xdr:cNvPr id="277" name="文本框 276">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3173603-AED2-4256-958E-2A6CDDDA45DB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000015010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31667,7 +31667,7 @@
         <xdr:cNvPr id="278" name="文本框 277">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57A5AA30-F9F8-4D75-B03A-167CE560C1AF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000016010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31738,7 +31738,7 @@
         <xdr:cNvPr id="279" name="文本框 278">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59A66C86-26C0-4266-AA43-12185910B31A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000017010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31809,7 +31809,7 @@
         <xdr:cNvPr id="280" name="文本框 279">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E49602A9-57F9-45AD-893F-69124D1906A9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000018010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31885,7 +31885,7 @@
         <xdr:cNvPr id="281" name="直接箭头连接符 280">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DFFF7AB-E98F-4685-A391-B6D4DFF4C91F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000019010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31938,7 +31938,7 @@
         <xdr:cNvPr id="282" name="直接箭头连接符 281">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FA0D247-62FC-43B5-BB16-6EA35FCE59E9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001A010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31991,7 +31991,7 @@
         <xdr:cNvPr id="288" name="直接箭头连接符 287">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C028FF6-C576-4FBB-AAB2-B001980BFEF8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000020010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32047,7 +32047,7 @@
         <xdr:cNvPr id="289" name="直接箭头连接符 288">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C232EF10-B645-4DAE-B95E-BFC92FE468ED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000021010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32103,7 +32103,7 @@
         <xdr:cNvPr id="290" name="图片 289">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BEE0725C-ECBD-4D46-B68A-7A0A3F0E03BE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000022010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32147,7 +32147,7 @@
         <xdr:cNvPr id="293" name="图片 292">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3754EAA-071F-4F9E-9814-155DE92874ED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000025010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32191,7 +32191,7 @@
         <xdr:cNvPr id="294" name="图片 293">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70ACA633-9929-4371-9BA6-155E3D6FB003}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000026010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32235,7 +32235,7 @@
         <xdr:cNvPr id="296" name="直接箭头连接符 295">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01119B15-2C74-492D-BFF9-6711A8B829E1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000028010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32288,7 +32288,7 @@
         <xdr:cNvPr id="242" name="直接箭头连接符 241">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C79658BF-7FF6-43A3-BE5E-0F11F79D33C3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000F2000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32345,7 +32345,7 @@
         <xdr:cNvPr id="243" name="直接箭头连接符 242">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{236C9239-D7E2-4597-931B-ACAD146D9C61}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000F3000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32397,7 +32397,7 @@
         <xdr:cNvPr id="258" name="文本框 257">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3173603-AED2-4256-958E-2A6CDDDA45DB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32468,7 +32468,7 @@
         <xdr:cNvPr id="259" name="文本框 258">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57A5AA30-F9F8-4D75-B03A-167CE560C1AF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32539,7 +32539,7 @@
         <xdr:cNvPr id="260" name="文本框 259">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59A66C86-26C0-4266-AA43-12185910B31A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32610,7 +32610,7 @@
         <xdr:cNvPr id="261" name="文本框 260">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E49602A9-57F9-45AD-893F-69124D1906A9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32683,7 +32683,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="83" name="直接连接符 82"/>
+        <xdr:cNvPr id="83" name="直接连接符 82">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000053000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -32730,7 +32736,7 @@
         <xdr:cNvPr id="262" name="直接箭头连接符 261">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FA0D247-62FC-43B5-BB16-6EA35FCE59E9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000006010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32780,7 +32786,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="200" name="直接连接符 199"/>
+        <xdr:cNvPr id="200" name="直接连接符 199">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000C8000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -32824,7 +32836,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="209" name="直接连接符 208"/>
+        <xdr:cNvPr id="209" name="直接连接符 208">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000D1000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -32868,7 +32886,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="227" name="直接箭头连接符 226"/>
+        <xdr:cNvPr id="227" name="直接箭头连接符 226">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000E3000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -32911,7 +32935,13 @@
     <xdr:ext cx="274883" cy="334451"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="230" name="文本框 229"/>
+        <xdr:cNvPr id="230" name="文本框 229">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000E6000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -32970,7 +33000,13 @@
     <xdr:ext cx="869725" cy="576568"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="231" name="文本框 230"/>
+        <xdr:cNvPr id="231" name="文本框 230">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000E7000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -33039,7 +33075,13 @@
     <xdr:ext cx="2336409" cy="334451"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="232" name="文本框 231"/>
+        <xdr:cNvPr id="232" name="文本框 231">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000E8000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -33103,7 +33145,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="234" name="直接连接符 233"/>
+        <xdr:cNvPr id="234" name="直接连接符 233">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000EA000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -33150,7 +33198,7 @@
         <xdr:cNvPr id="283" name="直接箭头连接符 282">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C79658BF-7FF6-43A3-BE5E-0F11F79D33C3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001B010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33207,7 +33255,7 @@
         <xdr:cNvPr id="284" name="直接箭头连接符 283">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{236C9239-D7E2-4597-931B-ACAD146D9C61}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001C010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33259,7 +33307,7 @@
         <xdr:cNvPr id="285" name="文本框 284">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3173603-AED2-4256-958E-2A6CDDDA45DB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001D010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33330,7 +33378,7 @@
         <xdr:cNvPr id="286" name="文本框 285">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57A5AA30-F9F8-4D75-B03A-167CE560C1AF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001E010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33401,7 +33449,7 @@
         <xdr:cNvPr id="287" name="文本框 286">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59A66C86-26C0-4266-AA43-12185910B31A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001F010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33472,7 +33520,7 @@
         <xdr:cNvPr id="291" name="文本框 290">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E49602A9-57F9-45AD-893F-69124D1906A9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000023010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33545,7 +33593,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="292" name="直接连接符 291"/>
+        <xdr:cNvPr id="292" name="直接连接符 291">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000024010000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -33592,7 +33646,7 @@
         <xdr:cNvPr id="295" name="直接箭头连接符 294">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FA0D247-62FC-43B5-BB16-6EA35FCE59E9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000027010000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33637,7 +33691,13 @@
     <xdr:ext cx="869725" cy="576568"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="297" name="文本框 296"/>
+        <xdr:cNvPr id="297" name="文本框 296">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000029010000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -33712,7 +33772,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="298" name="直接箭头连接符 297"/>
+        <xdr:cNvPr id="298" name="直接箭头连接符 297">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002A010000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -33755,7 +33821,13 @@
     <xdr:ext cx="274883" cy="334451"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="299" name="文本框 298"/>
+        <xdr:cNvPr id="299" name="文本框 298">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002B010000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -51595,7 +51667,7 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -51612,7 +51684,7 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -51629,7 +51701,7 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -51649,9 +51721,9 @@
       <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="4.83203125" style="1"/>
+    <col min="1" max="16384" width="4.875" style="1"/>
   </cols>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -51668,11 +51740,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AG113" sqref="AG113"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AT123" sqref="AT123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -51692,9 +51764,9 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="45" spans="15:15" ht="28.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="15:15" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O45" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified   doc/images/painter.xlsx Modified   source/step04/Samples/TransformationApp/TransformationApp.cpp
</commit_message>
<xml_diff>
--- a/doc/images/painter.xlsx
+++ b/doc/images/painter.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="左右手坐标系" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,8 @@
     <sheet name="相机坐标系" sheetId="3" r:id="rId3"/>
     <sheet name="向量" sheetId="4" r:id="rId4"/>
     <sheet name="矩阵" sheetId="6" r:id="rId5"/>
-    <sheet name="几何图元" sheetId="5" r:id="rId6"/>
+    <sheet name="四元数" sheetId="7" r:id="rId6"/>
+    <sheet name="几何图元" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -33880,6 +33881,246 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F724907F-907E-418A-A76B-972CAD180966}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="742950" y="714375"/>
+          <a:ext cx="4953000" cy="4381500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76202</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>295275</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="连接符: 肘形 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA0A6C69-BDD6-40BA-8B09-A0F4885DBA95}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1190627" y="1571625"/>
+          <a:ext cx="3219448" cy="1190625"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 888"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="连接符: 肘形 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32D23177-4630-4ADF-B6C2-1347B42539F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1905000" y="1562100"/>
+          <a:ext cx="1466850" cy="533400"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 1948"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>85729</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>142877</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>133352</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>314323</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="连接符: 肘形 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19DEE77A-CD3C-43CA-AED9-C551D144431E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="1947867" y="2290764"/>
+          <a:ext cx="2638421" cy="1162048"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 10289"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -51740,7 +51981,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A108" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AT123" sqref="AT123"/>
     </sheetView>
   </sheetViews>
@@ -51754,6 +51995,26 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE7" sqref="AE7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>

</xml_diff>

<commit_message>
Modified   doc/images/painter.xlsx Modified   doc/一起动手实现3D渲染引擎.md Modified   source/step04/Samples/TransformationApp/TransformationApp.cpp Add        doc/images/orientation-matrix.png
</commit_message>
<xml_diff>
--- a/doc/images/painter.xlsx
+++ b/doc/images/painter.xlsx
@@ -33887,20 +33887,20 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="图片 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F724907F-907E-418A-A76B-972CAD180966}"/>
+        <xdr:cNvPr id="6" name="图片 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB81ACB2-3F27-46E4-997B-C327C78FC08B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33923,8 +33923,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="742950" y="714375"/>
-          <a:ext cx="4953000" cy="4381500"/>
+          <a:off x="742950" y="704850"/>
+          <a:ext cx="4572000" cy="4191000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -33945,16 +33945,76 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>76202</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>104778</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304802</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="连接符: 肘形 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19DEE77A-CD3C-43CA-AED9-C551D144431E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="776290" y="2900363"/>
+          <a:ext cx="2771772" cy="2"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>276227</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>295275</xdr:rowOff>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -33969,12 +34029,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1190627" y="1571625"/>
-          <a:ext cx="3219448" cy="1190625"/>
+          <a:off x="1019177" y="1543050"/>
+          <a:ext cx="3200398" cy="1647825"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 888"/>
+            <a:gd name="adj1" fmla="val 893"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="57150">
@@ -34003,14 +34063,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>333375</xdr:rowOff>
     </xdr:to>
@@ -34027,12 +34087,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1905000" y="1562100"/>
-          <a:ext cx="1466850" cy="533400"/>
+          <a:off x="1609725" y="1543050"/>
+          <a:ext cx="1333500" cy="552450"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 1948"/>
+            <a:gd name="adj1" fmla="val 2143"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="57150">
@@ -34059,62 +34119,48 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>85729</xdr:colOff>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>295054</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>142877</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>133352</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>314323</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="16" name="连接符: 肘形 15">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19DEE77A-CD3C-43CA-AED9-C551D144431E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000" flipH="1">
-          <a:off x="1947867" y="2290764"/>
-          <a:ext cx="2638421" cy="1162048"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 10289"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln w="57150">
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
+      <xdr:rowOff>38010</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="图片 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB119ABA-B2FA-4B25-A86A-81D90AAAF664}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="752475" y="723900"/>
+          <a:ext cx="1771429" cy="723810"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -52002,7 +52048,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE7" sqref="AE7"/>
+      <selection activeCell="AL7" sqref="AL7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Modified   doc/images/orientation-pitch.fbx Modified   doc/images/orientation-roll.fbx Modified   doc/images/orientation-yaw.fbx Modified   doc/images/painter.xlsx Modified   doc/一起动手实现3D渲染引擎.md Modified   doc/一起动手实现3D渲染引擎.pdf Add        doc/images/orientation-matrix-interpolation-01.png Add        doc/images/orientation-matrix-interpolation.png Add        doc/images/orientation-pitch.png Add        doc/images/orientation-quaternion-history.jpg Add        doc/images/orientation-roll.png Add        doc/images/orientation-yaw.png
</commit_message>
<xml_diff>
--- a/doc/images/painter.xlsx
+++ b/doc/images/painter.xlsx
@@ -34163,6 +34163,1542 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="直接箭头连接符 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{223D1BE3-091C-4186-9325-E5CA0BCAE595}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8543925" y="714375"/>
+          <a:ext cx="0" cy="4219575"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>3017</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>351014</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>3017</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="直接箭头连接符 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57ACF088-0CF0-4A82-9E14-ED4974D02E4E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6305550" y="2822417"/>
+          <a:ext cx="4446764" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>361949</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="椭圆 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01D44FB8-067F-43D7-909C-9E84D312A93E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7067550" y="1419225"/>
+          <a:ext cx="2952749" cy="2819400"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>219074</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="椭圆 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35F54E17-5ADF-440B-8931-AABC5F094C66}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7200900" y="1562100"/>
+          <a:ext cx="2676525" cy="2533649"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9528</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="直接箭头连接符 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55867EE6-4754-4FF4-95E4-3A6AE9B85EEC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8543925" y="1238250"/>
+          <a:ext cx="0" cy="1590678"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>342901</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="直接箭头连接符 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B6BF1F0-DF5C-4C71-AB24-09DEBC65FEF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8553450" y="1676400"/>
+          <a:ext cx="1219200" cy="1133476"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="342594" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="文本框 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{236DA692-546B-47F1-909C-6DF3774B7124}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8391525" y="361950"/>
+          <a:ext cx="342594" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>0°</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>276225</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="765274" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="文本框 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78709C4A-30D9-411F-A255-F942FF0DE060}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8572500" y="981075"/>
+          <a:ext cx="765274" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>A=270°</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="659861" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="文本框 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AFDCEE1-FA87-46A8-AF81-F9EA5712FEF9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9801225" y="1409700"/>
+          <a:ext cx="659861" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>B=45°</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="504690" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="文本框 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D329E4D-3C57-4D72-B223-9F10BB00B75D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6124575" y="2457450"/>
+          <a:ext cx="504690" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-90°</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="649537" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="文本框 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70537161-1689-417E-A375-D532AF209F5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6010275" y="2847975"/>
+          <a:ext cx="649537" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+270°</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="554639" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="文本框 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47972FDE-53A4-4CE6-8D94-483058244443}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10496550" y="2457450"/>
+          <a:ext cx="554639" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+90°</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="599588" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="文本框 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1147CDBE-EA0F-48D6-9131-CFC37B4F4553}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10467975" y="2828925"/>
+          <a:ext cx="599588" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-270°</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="直接箭头连接符 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40ACE90C-6358-4154-A6AF-B63C2389DDB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13744575" y="723900"/>
+          <a:ext cx="0" cy="4219575"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>12542</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>351014</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>12542</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="直接箭头连接符 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75CCA40E-7920-4D86-9715-172D58C1EB64}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11506200" y="2831942"/>
+          <a:ext cx="4446764" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="342594" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="文本框 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3B1BAEE-C480-4B27-AE0D-5B2B453FD2C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13554075" y="361950"/>
+          <a:ext cx="342594" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>0°</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="504690" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="文本框 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED319619-9DC4-43CE-9036-403D6AE74ECA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11287125" y="2457450"/>
+          <a:ext cx="504690" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-90°</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="649537" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="文本框 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8713E07B-FEF5-4C62-92CC-F3DB3F3C3C38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11172825" y="2847975"/>
+          <a:ext cx="649537" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+270°</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="554639" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="文本框 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1770D459-453E-4C34-9C3D-71E71EAE31C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15659100" y="2457450"/>
+          <a:ext cx="554639" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+90°</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="599588" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="文本框 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20049E5D-BE28-4BFA-8461-B6CDF3725283}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15630525" y="2828925"/>
+          <a:ext cx="599588" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-270°</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>361949</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>342899</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="椭圆 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CE4FEED-2801-4551-BBFB-E8D24B25FF9D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12268200" y="1419225"/>
+          <a:ext cx="2952749" cy="2800349"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>2</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="直接箭头连接符 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAA9A739-641E-4AEF-BE2A-7F1945ACB35E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="13382625" y="2828925"/>
+          <a:ext cx="361952" cy="1762125"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="直接箭头连接符 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20AF66D1-BC97-4AD9-8B4A-59AB7205AE2B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13754100" y="2828925"/>
+          <a:ext cx="361950" cy="1762125"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="832472" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="文本框 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65D54DEC-58D0-417C-9F7E-6A4D3697A62B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12792075" y="4572000"/>
+          <a:ext cx="832472" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>A=-170°</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="754758" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="45" name="文本框 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AD82C2C-CCE0-4B63-847D-1639EA0D1B46}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14001750" y="4572000"/>
+          <a:ext cx="754758" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>B=170°</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -52027,7 +53563,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A108" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A102" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AT123" sqref="AT123"/>
     </sheetView>
   </sheetViews>
@@ -52048,7 +53584,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AL7" sqref="AL7"/>
+      <selection activeCell="AB19" sqref="AB19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Modified   doc/images/painter.xlsx Modified   doc/一起动手实现3D渲染引擎.md Add        doc/images/orientation-ijk-unit-vector.png
</commit_message>
<xml_diff>
--- a/doc/images/painter.xlsx
+++ b/doc/images/painter.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\MyGame\Tiny3D\steps\doc\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaronwang\workspace\projects\private\Tiny3D\steps\doc\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12170" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="左右手坐标系" sheetId="1" r:id="rId1"/>
@@ -33882,6 +33882,94 @@
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="直接连接符 17"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12153900" y="7112000"/>
+          <a:ext cx="2946400" cy="1422400"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="直接连接符 14"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12890500" y="6394450"/>
+          <a:ext cx="1479550" cy="2851150"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
@@ -35689,6 +35777,2342 @@
               <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
             </a:rPr>
             <a:t>B=170°</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="直接箭头连接符 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{223D1BE3-091C-4186-9325-E5CA0BCAE595}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2952750" y="5695950"/>
+          <a:ext cx="0" cy="4257675"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>355442</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>357364</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>355442</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="直接箭头连接符 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57ACF088-0CF0-4A82-9E14-ED4974D02E4E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="736600" y="7823042"/>
+          <a:ext cx="4408664" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>3174</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="椭圆 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01D44FB8-067F-43D7-909C-9E84D312A93E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1485900" y="6407150"/>
+          <a:ext cx="2936874" cy="2838450"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="401585" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="文本框 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2749550" y="5334000"/>
+          <a:ext cx="401585" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+Y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="351635" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="文本框 41"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2787650" y="9969500"/>
+          <a:ext cx="351635" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-Y</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="409536" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="文本框 42"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5130800" y="7651750"/>
+          <a:ext cx="409536" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>+X</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="359586" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="文本框 45"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="368300" y="7645400"/>
+          <a:ext cx="359586" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-X</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="279564" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="文本框 46"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4419600" y="7467600"/>
+          <a:ext cx="279564" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="346762" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="文本框 47"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1104900" y="7467600"/>
+          <a:ext cx="346762" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-1</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="279564" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="49" name="文本框 48"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2946400" y="6045200"/>
+          <a:ext cx="279564" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="346762" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="文本框 49"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2946400" y="9245600"/>
+          <a:ext cx="346762" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-1</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="直接箭头连接符 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{223D1BE3-091C-4186-9325-E5CA0BCAE595}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8477250" y="5695950"/>
+          <a:ext cx="0" cy="4257675"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>355442</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>357364</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>355442</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="52" name="直接箭头连接符 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57ACF088-0CF0-4A82-9E14-ED4974D02E4E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6261100" y="7823042"/>
+          <a:ext cx="4408664" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>3174</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="53" name="椭圆 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01D44FB8-067F-43D7-909C-9E84D312A93E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7010400" y="6407150"/>
+          <a:ext cx="2936874" cy="2838450"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="387414" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="54" name="文本框 53"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8274050" y="5334000"/>
+          <a:ext cx="387414" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>Im</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="381708" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="56" name="文本框 55"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10655300" y="7651750"/>
+          <a:ext cx="381708" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>Re</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="279564" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="58" name="文本框 57"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9944100" y="7467600"/>
+          <a:ext cx="279564" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="346762" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="59" name="文本框 58"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6629400" y="7467600"/>
+          <a:ext cx="346762" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-1</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="230191" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="60" name="文本框 59"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8470900" y="6045200"/>
+          <a:ext cx="230191" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>i</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="297389" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61" name="文本框 60"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8470900" y="9245600"/>
+          <a:ext cx="297389" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-i</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="62" name="直接箭头连接符 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{223D1BE3-091C-4186-9325-E5CA0BCAE595}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13627100" y="5695950"/>
+          <a:ext cx="0" cy="4257675"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>355442</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>351014</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>355442</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="63" name="直接箭头连接符 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57ACF088-0CF0-4A82-9E14-ED4974D02E4E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11410950" y="7823042"/>
+          <a:ext cx="4408664" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>196850</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="64" name="椭圆 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01D44FB8-067F-43D7-909C-9E84D312A93E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11982450" y="6229350"/>
+          <a:ext cx="3289300" cy="3200400"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="387414" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="65" name="文本框 64"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13423900" y="5334000"/>
+          <a:ext cx="387414" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>Im</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>336550</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="381708" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="66" name="文本框 65"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15805150" y="7651750"/>
+          <a:ext cx="381708" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>Re</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="279564" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="67" name="文本框 66"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14211300" y="7467600"/>
+          <a:ext cx="279564" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="346762" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="68" name="文本框 67"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12725400" y="7467600"/>
+          <a:ext cx="346762" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-1</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="230191" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="69" name="文本框 68"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13646150" y="6940550"/>
+          <a:ext cx="230191" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>i</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="297389" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="70" name="文本框 69"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13627100" y="8343900"/>
+          <a:ext cx="297389" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-i</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>196850</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="346762" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="80" name="文本框 79"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11982450" y="7461250"/>
+          <a:ext cx="346762" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-2</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="279564" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="81" name="文本框 80"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14960600" y="7467600"/>
+          <a:ext cx="279564" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>2</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="325089" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="82" name="文本框 81"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13646150" y="6254750"/>
+          <a:ext cx="325089" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>2i</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="392287" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="83" name="文本框 82"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13633450" y="9067800"/>
+          <a:ext cx="392287" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>-2i</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>311150</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="753540" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="文本框 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15043150" y="6769100"/>
+          <a:ext cx="753540" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>p = 2+i</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="915443" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="84" name="文本框 83"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12026900" y="6051550"/>
+          <a:ext cx="915443" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>q = -1+2i</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="733534" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="85" name="文本框 84"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11417300" y="8528050"/>
+          <a:ext cx="733534" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>r = -2-i</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+            <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="772006" cy="356316"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="86" name="文本框 85"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14363700" y="9245600"/>
+          <a:ext cx="772006" cy="356316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:rPr>
+            <a:t>s = 1-2i</a:t>
           </a:r>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
             <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
@@ -53490,7 +55914,7 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -53507,7 +55931,7 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -53524,7 +55948,7 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -53544,9 +55968,9 @@
       <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="4.875" style="1"/>
+    <col min="1" max="16384" width="4.83203125" style="1"/>
   </cols>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -53567,7 +55991,7 @@
       <selection activeCell="AT123" sqref="AT123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -53583,11 +56007,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB19" sqref="AB19"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -53607,9 +56031,9 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="45" spans="15:15" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="15:15" ht="28.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O45" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified   doc/images/painter.xlsx Modified   source/step02/Math/Include/T3DFix32.h Modified   source/step02/Math/Include/T3DFix64.h Modified   source/step02/Math/Include/T3DQuaternion.h Modified   source/step02/Math/Include/T3DQuaternion.inl Modified   source/step02/Math/Source/T3DFix32.cpp Modified   source/step02/Math/Source/T3DFix64.cpp Modified   source/step02/Math/Source/T3DReal.cpp
</commit_message>
<xml_diff>
--- a/doc/images/painter.xlsx
+++ b/doc/images/painter.xlsx
@@ -33885,6 +33885,272 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>306200</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>318900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="72" name="图片 71"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3708400" y="13550900"/>
+          <a:ext cx="280800" cy="280800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>318900</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>318900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="105" name="图片 104"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9245600" y="13550900"/>
+          <a:ext cx="280800" cy="280800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>219832</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>39500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="119" name="图片 118"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10267950" y="13627100"/>
+          <a:ext cx="264282" cy="280800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>197900</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>120700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>74400</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>21500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="118" name="图片 117"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="10326700" y="11683500"/>
+          <a:ext cx="612000" cy="244800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>361366</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>184764</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>237866</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>261164</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="117" name="图片 116"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="11316766" y="12724364"/>
+          <a:ext cx="432000" cy="244800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>100334</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>217166</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>12834</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>304934</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="116" name="图片 115"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="17893113">
+          <a:off x="10699750" y="12744450"/>
+          <a:ext cx="443368" cy="280800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>227468</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>318900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="115" name="图片 114"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9359900" y="13906500"/>
+          <a:ext cx="443368" cy="280800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>196850</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>31750</xdr:rowOff>
@@ -33903,7 +34169,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -33979,7 +34245,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -34017,7 +34283,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -34149,7 +34415,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -34386,7 +34652,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -38508,20 +38774,58 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>306200</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>318900</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>196851</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>69851</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>107951</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>349251</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="72" name="图片 71"/>
+        <xdr:cNvPr id="55" name="图片 54"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6457951" y="13938251"/>
+          <a:ext cx="279400" cy="279400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>4939</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>215900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="97" name="图片 96"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -38534,8 +38838,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3708400" y="13550900"/>
-          <a:ext cx="280800" cy="280800"/>
+          <a:off x="9417050" y="12833350"/>
+          <a:ext cx="531989" cy="184150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -38546,20 +38850,58 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>196851</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>69851</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>107951</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>349251</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>296032</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>77600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="55" name="图片 54"/>
+        <xdr:cNvPr id="98" name="图片 97"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11817350" y="11887200"/>
+          <a:ext cx="264282" cy="280800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>306200</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>71250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="99" name="图片 98"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -38572,7 +38914,314 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6457951" y="13938251"/>
+          <a:off x="11074400" y="11525250"/>
+          <a:ext cx="280800" cy="280800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>196850</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>109350</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>20450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="100" name="图片 99"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10140950" y="10763250"/>
+          <a:ext cx="280800" cy="280800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>6351</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>3651</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="101" name="直接箭头连接符 100">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000C6000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8845551" y="13868400"/>
+          <a:ext cx="3312000" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>106600</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>109300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>106600</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>220900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="102" name="直接箭头连接符 101">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000C6000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="-3600000" flipV="1">
+          <a:off x="8026400" y="12433300"/>
+          <a:ext cx="3312000" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>7703</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>5000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>5003</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>5000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="103" name="直接箭头连接符 102">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000C6000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="-2400000" flipV="1">
+          <a:off x="8478603" y="12806600"/>
+          <a:ext cx="3312000" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="104" name="环形箭头 103"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5619750" y="10318750"/>
+          <a:ext cx="6737350" cy="7264400"/>
+        </a:xfrm>
+        <a:prstGeom prst="circularArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 1406"/>
+            <a:gd name="adj2" fmla="val 165944"/>
+            <a:gd name="adj3" fmla="val 14400168"/>
+            <a:gd name="adj4" fmla="val 10893893"/>
+            <a:gd name="adj5" fmla="val 2043"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>209551</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>69851</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>120651</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>349251</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="106" name="图片 105"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11995151" y="13938251"/>
           <a:ext cx="279400" cy="279400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -38580,6 +39229,200 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>260350</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="107" name="直接箭头连接符 106">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000C6000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8845550" y="13868400"/>
+          <a:ext cx="1358900" cy="6350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="108" name="直接箭头连接符 107">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000C6000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10198100" y="11734800"/>
+          <a:ext cx="1200150" cy="2127250"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="109" name="直接连接符 108"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10496550" y="11017250"/>
+          <a:ext cx="6350" cy="2851150"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="111" name="直接连接符 110"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11404600" y="11747500"/>
+          <a:ext cx="0" cy="2120900"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -56467,7 +57310,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y35" sqref="Y35"/>
+      <selection activeCell="AK37" sqref="AK37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="28.4" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>